<commit_message>
create excel project to test color cells
</commit_message>
<xml_diff>
--- a/FreeWork/ADECUA/AppFinalQt/database.xlsx
+++ b/FreeWork/ADECUA/AppFinalQt/database.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo\GitHub\PYTHON\FreeWork\ADECUA\AppFinalQt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique\Documents\Trabajo\Github\PYTHON\FreeWork\ADECUA\AppFinalQt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAC3A86-26C3-4A70-BC15-EE74EFCAB399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1589F80C-4C75-4018-8DA0-D2FFC47BB820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="V1" sheetId="8" r:id="rId2"/>
     <sheet name="V2" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1502,13 +1505,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1858,46 +1861,47 @@
   <dimension ref="B1:M190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B145" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="G148" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A160" sqref="A160:XFD160"/>
+      <selection pane="bottomRight" activeCell="L117" sqref="L117:L122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="2.1796875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="1.85546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="32.26953125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="1.81640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="30.81640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="4.453125" style="7" customWidth="1"/>
     <col min="11" max="11" width="52" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="9" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="12" max="12" width="22.6328125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="20.453125" style="7" customWidth="1"/>
+    <col min="14" max="16384" width="11.453125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-    </row>
-    <row r="3" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
@@ -1927,7 +1931,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="9" t="s">
         <v>74</v>
@@ -1954,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="10">
         <v>3</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10">
         <v>4</v>
       </c>
@@ -2014,13 +2018,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>28</v>
       </c>
@@ -2050,7 +2054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>39</v>
       </c>
@@ -2080,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>40</v>
       </c>
@@ -2110,7 +2114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>41</v>
       </c>
@@ -2140,7 +2144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>42</v>
       </c>
@@ -2170,7 +2174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>45</v>
       </c>
@@ -2200,7 +2204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <v>46</v>
       </c>
@@ -2230,13 +2234,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1">
         <v>28</v>
       </c>
@@ -2266,7 +2270,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
         <v>39</v>
       </c>
@@ -2296,7 +2300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
         <v>40</v>
       </c>
@@ -2326,7 +2330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
         <v>41</v>
       </c>
@@ -2356,7 +2360,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
         <v>42</v>
       </c>
@@ -2386,7 +2390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
         <v>45</v>
       </c>
@@ -2416,7 +2420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <v>46</v>
       </c>
@@ -2446,13 +2450,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10">
         <v>3</v>
       </c>
@@ -2482,7 +2486,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="10">
         <v>4</v>
       </c>
@@ -2512,7 +2516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="8">
         <v>61</v>
       </c>
@@ -2543,7 +2547,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="8">
         <v>62</v>
       </c>
@@ -2574,7 +2578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="8">
         <v>63</v>
       </c>
@@ -2605,7 +2609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="8">
         <v>64</v>
       </c>
@@ -2636,8 +2640,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
       <c r="C32" s="9" t="s">
         <v>74</v>
@@ -2665,7 +2669,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="10">
         <v>1</v>
       </c>
@@ -2695,7 +2699,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10">
         <v>2</v>
       </c>
@@ -2725,7 +2729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="1">
         <v>11</v>
       </c>
@@ -2755,7 +2759,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="1">
         <v>22</v>
       </c>
@@ -2785,7 +2789,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="1">
         <v>23</v>
       </c>
@@ -2815,7 +2819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="1">
         <v>24</v>
       </c>
@@ -2845,7 +2849,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="1">
         <v>25</v>
       </c>
@@ -2875,7 +2879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="1">
         <v>26</v>
       </c>
@@ -2905,7 +2909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="1">
         <v>27</v>
       </c>
@@ -2935,7 +2939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="19">
         <v>12</v>
       </c>
@@ -2965,7 +2969,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="19">
         <v>13</v>
       </c>
@@ -2995,7 +2999,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="19">
         <v>29</v>
       </c>
@@ -3025,7 +3029,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="19">
         <v>30</v>
       </c>
@@ -3055,7 +3059,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="19">
         <v>31</v>
       </c>
@@ -3085,14 +3089,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="20">
+    <row r="48" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="21">
         <v>5</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -3121,8 +3125,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="20"/>
+    <row r="49" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="21"/>
       <c r="C49" s="9" t="s">
         <v>74</v>
       </c>
@@ -3149,8 +3153,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="20">
+    <row r="50" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="21">
         <v>6</v>
       </c>
       <c r="C50" s="9" t="s">
@@ -3179,8 +3183,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="20"/>
+    <row r="51" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="21"/>
       <c r="C51" s="9" t="s">
         <v>74</v>
       </c>
@@ -3207,8 +3211,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="20">
+    <row r="52" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="21">
         <v>7</v>
       </c>
       <c r="C52" s="9" t="s">
@@ -3237,8 +3241,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="20"/>
+    <row r="53" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="21"/>
       <c r="C53" s="9" t="s">
         <v>74</v>
       </c>
@@ -3265,8 +3269,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="20">
+    <row r="54" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="21">
         <v>8</v>
       </c>
       <c r="C54" s="9" t="s">
@@ -3295,8 +3299,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="20"/>
+    <row r="55" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="21"/>
       <c r="C55" s="9" t="s">
         <v>74</v>
       </c>
@@ -3323,8 +3327,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="20">
+    <row r="56" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="21">
         <v>9</v>
       </c>
       <c r="C56" s="9" t="s">
@@ -3353,8 +3357,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="20"/>
+    <row r="57" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="21"/>
       <c r="C57" s="9" t="s">
         <v>74</v>
       </c>
@@ -3381,8 +3385,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="20">
+    <row r="58" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="21">
         <v>10</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -3411,8 +3415,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="20"/>
+    <row r="59" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="21"/>
       <c r="C59" s="9" t="s">
         <v>74</v>
       </c>
@@ -3439,8 +3443,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="20">
+    <row r="60" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="21">
         <v>14</v>
       </c>
       <c r="C60" s="9" t="s">
@@ -3469,8 +3473,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="20"/>
+    <row r="61" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="21"/>
       <c r="C61" s="9" t="s">
         <v>74</v>
       </c>
@@ -3497,8 +3501,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="20">
+    <row r="62" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="21">
         <v>15</v>
       </c>
       <c r="C62" s="9" t="s">
@@ -3527,8 +3531,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="20"/>
+    <row r="63" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="21"/>
       <c r="C63" s="9" t="s">
         <v>74</v>
       </c>
@@ -3555,8 +3559,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="20">
+    <row r="64" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="21">
         <v>16</v>
       </c>
       <c r="C64" s="9" t="s">
@@ -3585,8 +3589,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="20"/>
+    <row r="65" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="21"/>
       <c r="C65" s="9" t="s">
         <v>74</v>
       </c>
@@ -3613,8 +3617,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="20">
+    <row r="66" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="21">
         <v>17</v>
       </c>
       <c r="C66" s="9" t="s">
@@ -3643,8 +3647,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="20"/>
+    <row r="67" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="21"/>
       <c r="C67" s="9" t="s">
         <v>74</v>
       </c>
@@ -3671,7 +3675,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B68" s="1">
         <v>11</v>
       </c>
@@ -3701,7 +3705,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="1">
         <v>22</v>
       </c>
@@ -3731,7 +3735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="1">
         <v>23</v>
       </c>
@@ -3761,7 +3765,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="1">
         <v>24</v>
       </c>
@@ -3791,7 +3795,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" s="1">
         <v>25</v>
       </c>
@@ -3821,7 +3825,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="1">
         <v>26</v>
       </c>
@@ -3851,7 +3855,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="1">
         <v>27</v>
       </c>
@@ -3881,7 +3885,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="19">
         <v>12</v>
       </c>
@@ -3911,7 +3915,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="19">
         <v>13</v>
       </c>
@@ -3941,7 +3945,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="19">
         <v>29</v>
       </c>
@@ -3971,7 +3975,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="19">
         <v>30</v>
       </c>
@@ -4001,7 +4005,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="19">
         <v>31</v>
       </c>
@@ -4031,14 +4035,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
     </row>
-    <row r="81" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="20">
+    <row r="81" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="21">
         <v>5</v>
       </c>
       <c r="C81" s="9" t="s">
@@ -4067,8 +4071,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="20"/>
+    <row r="82" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B82" s="21"/>
       <c r="C82" s="9" t="s">
         <v>74</v>
       </c>
@@ -4095,8 +4099,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="20">
+    <row r="83" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="21">
         <v>6</v>
       </c>
       <c r="C83" s="9" t="s">
@@ -4125,8 +4129,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="20"/>
+    <row r="84" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B84" s="21"/>
       <c r="C84" s="9" t="s">
         <v>74</v>
       </c>
@@ -4153,8 +4157,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="20">
+    <row r="85" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B85" s="21">
         <v>7</v>
       </c>
       <c r="C85" s="9" t="s">
@@ -4183,8 +4187,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="20"/>
+    <row r="86" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="21"/>
       <c r="C86" s="9" t="s">
         <v>74</v>
       </c>
@@ -4211,8 +4215,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="20">
+    <row r="87" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="21">
         <v>8</v>
       </c>
       <c r="C87" s="9" t="s">
@@ -4241,8 +4245,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="20"/>
+    <row r="88" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="21"/>
       <c r="C88" s="9" t="s">
         <v>74</v>
       </c>
@@ -4269,8 +4273,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="89" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="20">
+    <row r="89" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="21">
         <v>9</v>
       </c>
       <c r="C89" s="9" t="s">
@@ -4299,8 +4303,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="90" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="20"/>
+    <row r="90" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="21"/>
       <c r="C90" s="9" t="s">
         <v>74</v>
       </c>
@@ -4327,8 +4331,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="20">
+    <row r="91" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="21">
         <v>10</v>
       </c>
       <c r="C91" s="9" t="s">
@@ -4357,8 +4361,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="92" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="20"/>
+    <row r="92" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="21"/>
       <c r="C92" s="9" t="s">
         <v>74</v>
       </c>
@@ -4385,8 +4389,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="93" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="20">
+    <row r="93" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="21">
         <v>14</v>
       </c>
       <c r="C93" s="9" t="s">
@@ -4415,8 +4419,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="94" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="20"/>
+    <row r="94" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="21"/>
       <c r="C94" s="9" t="s">
         <v>74</v>
       </c>
@@ -4443,8 +4447,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="95" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="20">
+    <row r="95" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B95" s="21">
         <v>15</v>
       </c>
       <c r="C95" s="9" t="s">
@@ -4473,8 +4477,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="20"/>
+    <row r="96" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="21"/>
       <c r="C96" s="9" t="s">
         <v>74</v>
       </c>
@@ -4501,8 +4505,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="20">
+    <row r="97" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="21">
         <v>16</v>
       </c>
       <c r="C97" s="9" t="s">
@@ -4531,8 +4535,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="98" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="20"/>
+    <row r="98" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="21"/>
       <c r="C98" s="9" t="s">
         <v>74</v>
       </c>
@@ -4559,8 +4563,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="20">
+    <row r="99" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B99" s="21">
         <v>17</v>
       </c>
       <c r="C99" s="9" t="s">
@@ -4589,8 +4593,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="20"/>
+    <row r="100" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="21"/>
       <c r="C100" s="9" t="s">
         <v>74</v>
       </c>
@@ -4617,7 +4621,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B101" s="1">
         <v>11</v>
       </c>
@@ -4647,7 +4651,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="102" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B102" s="1">
         <v>22</v>
       </c>
@@ -4677,7 +4681,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="1">
         <v>23</v>
       </c>
@@ -4707,7 +4711,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="104" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="1">
         <v>24</v>
       </c>
@@ -4737,7 +4741,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="105" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B105" s="1">
         <v>25</v>
       </c>
@@ -4767,7 +4771,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="1">
         <v>26</v>
       </c>
@@ -4797,7 +4801,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="107" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="1">
         <v>27</v>
       </c>
@@ -4827,7 +4831,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="108" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" s="19">
         <v>12</v>
       </c>
@@ -4857,7 +4861,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="109" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="19">
         <v>13</v>
       </c>
@@ -4887,7 +4891,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="110" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B110" s="19">
         <v>29</v>
       </c>
@@ -4917,7 +4921,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="19">
         <v>30</v>
       </c>
@@ -4947,7 +4951,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B112" s="19">
         <v>31</v>
       </c>
@@ -4977,14 +4981,14 @@
         <v>102</v>
       </c>
     </row>
-    <row r="113" spans="2:13" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:13" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C113" s="9"/>
       <c r="D113" s="9"/>
       <c r="E113" s="9"/>
       <c r="F113" s="9"/>
       <c r="L113" s="12"/>
     </row>
-    <row r="114" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B114" s="10">
         <v>43</v>
       </c>
@@ -5014,7 +5018,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="115" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B115" s="10">
         <v>44</v>
       </c>
@@ -5040,12 +5044,12 @@
         <v>168</v>
       </c>
       <c r="L115" s="12">
-        <f t="shared" ref="L115:L117" si="6">L114+1</f>
+        <f t="shared" ref="L115:L122" si="6">L114+1</f>
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="21">
+    <row r="116" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B116" s="22">
         <v>61</v>
       </c>
       <c r="C116" s="9" t="s">
@@ -5079,8 +5083,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="117" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="21"/>
+    <row r="117" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B117" s="22"/>
       <c r="C117" s="9" t="s">
         <v>74</v>
       </c>
@@ -5109,8 +5113,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="118" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="21">
+    <row r="118" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B118" s="22">
         <v>63</v>
       </c>
       <c r="C118" s="9" t="s">
@@ -5136,13 +5140,13 @@
       <c r="K118" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="L118" s="12" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="119" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="21"/>
+      <c r="L118" s="12">
+        <f t="shared" si="6"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="119" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B119" s="22"/>
       <c r="C119" s="9" t="s">
         <v>74</v>
       </c>
@@ -5166,13 +5170,13 @@
       <c r="K119" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="L119" s="12" t="e">
-        <f t="shared" ref="L119:L122" si="7">L118+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="120" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="21">
+      <c r="L119" s="12">
+        <f t="shared" si="6"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="120" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B120" s="22">
         <v>64</v>
       </c>
       <c r="C120" s="9" t="s">
@@ -5198,13 +5202,13 @@
       <c r="K120" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="L120" s="12" t="e">
-        <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="121" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="21"/>
+      <c r="L120" s="12">
+        <f t="shared" si="6"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="121" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B121" s="22"/>
       <c r="C121" s="9" t="s">
         <v>74</v>
       </c>
@@ -5228,12 +5232,12 @@
       <c r="K121" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="L121" s="12" t="e">
-        <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="122" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L121" s="12">
+        <f t="shared" si="6"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="122" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B122" s="11">
         <v>67</v>
       </c>
@@ -5260,13 +5264,13 @@
       <c r="K122" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="L122" s="12" t="e">
-        <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="123" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L122" s="12">
+        <f t="shared" si="6"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="123" spans="2:13" ht="50.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="124" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B124" s="5"/>
       <c r="C124" s="7" t="s">
         <v>74</v>
@@ -5289,12 +5293,12 @@
       <c r="K124" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="L124" s="12" t="e">
+      <c r="L124" s="12">
         <f>L122+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="125" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="125" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B125" s="10">
         <v>18</v>
       </c>
@@ -5319,12 +5323,12 @@
       <c r="K125" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="L125" s="12" t="e">
+      <c r="L125" s="12">
         <f>L124+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="126" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="126" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B126" s="10">
         <v>19</v>
       </c>
@@ -5349,12 +5353,12 @@
       <c r="K126" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="L126" s="12" t="e">
+      <c r="L126" s="12">
         <f>L125+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="127" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="127" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B127" s="10">
         <v>20</v>
       </c>
@@ -5379,19 +5383,19 @@
       <c r="K127" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="L127" s="12" t="e">
+      <c r="L127" s="12">
         <f>L126+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="128" spans="2:13" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="128" spans="2:13" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C128" s="9"/>
       <c r="D128" s="9"/>
       <c r="E128" s="9"/>
       <c r="F128" s="9"/>
     </row>
-    <row r="129" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="20">
+    <row r="129" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B129" s="21">
         <v>1</v>
       </c>
       <c r="C129" s="9" t="s">
@@ -5415,13 +5419,13 @@
       <c r="K129" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="L129" s="12" t="e">
+      <c r="L129" s="12">
         <f>L127+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="130" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="20"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="130" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B130" s="21"/>
       <c r="C130" s="9" t="s">
         <v>74</v>
       </c>
@@ -5443,13 +5447,13 @@
       <c r="K130" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="L130" s="12" t="e">
-        <f t="shared" ref="L130:L132" si="8">L129+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="131" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="20">
+      <c r="L130" s="12">
+        <f t="shared" ref="L130:L132" si="7">L129+1</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="131" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B131" s="21">
         <v>2</v>
       </c>
       <c r="C131" s="9" t="s">
@@ -5473,13 +5477,13 @@
       <c r="K131" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="L131" s="12" t="e">
-        <f t="shared" si="8"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="132" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="20"/>
+      <c r="L131" s="12">
+        <f t="shared" si="7"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="132" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B132" s="21"/>
       <c r="C132" s="9" t="s">
         <v>74</v>
       </c>
@@ -5501,12 +5505,12 @@
       <c r="K132" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="L132" s="12" t="e">
-        <f t="shared" si="8"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="133" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L132" s="12">
+        <f t="shared" si="7"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="133" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B133" s="1">
         <v>11</v>
       </c>
@@ -5531,12 +5535,12 @@
       <c r="K133" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="L133" s="12" t="e">
+      <c r="L133" s="12">
         <f>L132+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="134" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="134" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B134" s="1">
         <v>22</v>
       </c>
@@ -5561,12 +5565,12 @@
       <c r="K134" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="L134" s="12" t="e">
+      <c r="L134" s="12">
         <f>L133+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="135" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="135" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B135" s="1">
         <v>23</v>
       </c>
@@ -5591,12 +5595,12 @@
       <c r="K135" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="L135" s="12" t="e">
-        <f t="shared" ref="L135:L139" si="9">L134+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="136" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L135" s="12">
+        <f t="shared" ref="L135:L139" si="8">L134+1</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="136" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B136" s="1">
         <v>24</v>
       </c>
@@ -5621,12 +5625,12 @@
       <c r="K136" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="L136" s="12" t="e">
-        <f t="shared" si="9"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="137" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L136" s="12">
+        <f t="shared" si="8"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="137" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B137" s="1">
         <v>25</v>
       </c>
@@ -5651,12 +5655,12 @@
       <c r="K137" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="L137" s="12" t="e">
-        <f t="shared" si="9"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="138" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L137" s="12">
+        <f t="shared" si="8"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="138" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B138" s="1">
         <v>26</v>
       </c>
@@ -5681,12 +5685,12 @@
       <c r="K138" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="L138" s="12" t="e">
-        <f t="shared" si="9"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="139" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L138" s="12">
+        <f t="shared" si="8"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="139" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B139" s="1">
         <v>27</v>
       </c>
@@ -5711,19 +5715,19 @@
       <c r="K139" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="L139" s="12" t="e">
-        <f t="shared" si="9"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="140" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L139" s="12">
+        <f t="shared" si="8"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="140" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C140" s="9"/>
       <c r="D140" s="9"/>
       <c r="E140" s="9"/>
       <c r="F140" s="9"/>
     </row>
-    <row r="141" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="20">
+    <row r="141" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B141" s="21">
         <v>1</v>
       </c>
       <c r="C141" s="9" t="s">
@@ -5747,13 +5751,13 @@
       <c r="K141" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="L141" s="12" t="e">
+      <c r="L141" s="12">
         <f>L139+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="142" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="20"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="142" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B142" s="21"/>
       <c r="C142" s="9" t="s">
         <v>74</v>
       </c>
@@ -5775,13 +5779,13 @@
       <c r="K142" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="L142" s="12" t="e">
-        <f t="shared" ref="L142:L146" si="10">L141+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="143" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="20">
+      <c r="L142" s="12">
+        <f t="shared" ref="L142:L146" si="9">L141+1</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="143" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B143" s="21">
         <v>2</v>
       </c>
       <c r="C143" s="9" t="s">
@@ -5805,13 +5809,13 @@
       <c r="K143" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="L143" s="12" t="e">
-        <f t="shared" si="10"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="144" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="20"/>
+      <c r="L143" s="12">
+        <f t="shared" si="9"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="144" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B144" s="21"/>
       <c r="C144" s="9" t="s">
         <v>74</v>
       </c>
@@ -5833,12 +5837,12 @@
       <c r="K144" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="L144" s="12" t="e">
-        <f t="shared" si="10"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="145" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L144" s="12">
+        <f t="shared" si="9"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="145" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B145" s="1">
         <v>11</v>
       </c>
@@ -5863,12 +5867,12 @@
       <c r="K145" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="L145" s="12" t="e">
-        <f t="shared" si="10"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="146" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L145" s="12">
+        <f t="shared" si="9"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="146" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B146" s="1">
         <v>22</v>
       </c>
@@ -5893,12 +5897,12 @@
       <c r="K146" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="L146" s="12" t="e">
-        <f t="shared" si="10"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="147" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L146" s="12">
+        <f t="shared" si="9"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="147" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B147" s="1">
         <v>23</v>
       </c>
@@ -5923,12 +5927,12 @@
       <c r="K147" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="L147" s="12" t="e">
-        <f t="shared" ref="L147:L151" si="11">L146+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="148" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L147" s="12">
+        <f t="shared" ref="L147:L151" si="10">L146+1</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B148" s="1">
         <v>24</v>
       </c>
@@ -5953,12 +5957,12 @@
       <c r="K148" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="L148" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="149" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L148" s="12">
+        <f t="shared" si="10"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="149" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B149" s="1">
         <v>25</v>
       </c>
@@ -5983,12 +5987,12 @@
       <c r="K149" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="L149" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="150" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L149" s="12">
+        <f t="shared" si="10"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="150" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B150" s="1">
         <v>26</v>
       </c>
@@ -6013,12 +6017,12 @@
       <c r="K150" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="L150" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="151" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L150" s="12">
+        <f t="shared" si="10"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="151" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B151" s="1">
         <v>27</v>
       </c>
@@ -6043,18 +6047,18 @@
       <c r="K151" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="L151" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="152" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L151" s="12">
+        <f t="shared" si="10"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="152" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C152" s="9"/>
       <c r="D152" s="9"/>
       <c r="E152" s="9"/>
       <c r="F152" s="9"/>
     </row>
-    <row r="153" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B153" s="10">
         <v>1</v>
       </c>
@@ -6079,12 +6083,12 @@
       <c r="K153" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="L153" s="12" t="e">
+      <c r="L153" s="12">
         <f>L151+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="154" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="154" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B154" s="10">
         <v>2</v>
       </c>
@@ -6111,12 +6115,12 @@
       <c r="K154" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="L154" s="12" t="e">
+      <c r="L154" s="12">
         <f>L153+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="155" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="155" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B155" s="8">
         <v>61</v>
       </c>
@@ -6143,12 +6147,12 @@
       <c r="K155" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="L155" s="12" t="e">
-        <f t="shared" ref="L155:L159" si="12">L154+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="156" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L155" s="12">
+        <f t="shared" ref="L155:L159" si="11">L154+1</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="156" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B156" s="8">
         <v>62</v>
       </c>
@@ -6175,12 +6179,12 @@
       <c r="K156" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="L156" s="12" t="e">
-        <f t="shared" si="12"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="157" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L156" s="12">
+        <f t="shared" si="11"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="157" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B157" s="8">
         <v>63</v>
       </c>
@@ -6207,12 +6211,12 @@
       <c r="K157" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="L157" s="12" t="e">
-        <f t="shared" si="12"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="158" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L157" s="12">
+        <f t="shared" si="11"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="158" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B158" s="8">
         <v>64</v>
       </c>
@@ -6239,12 +6243,12 @@
       <c r="K158" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="L158" s="12" t="e">
-        <f t="shared" si="12"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="159" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L158" s="12">
+        <f t="shared" si="11"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="159" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B159" s="2">
         <v>65</v>
       </c>
@@ -6271,55 +6275,49 @@
       <c r="K159" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="L159" s="12" t="e">
-        <f t="shared" si="12"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="160" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="L159" s="12">
+        <f t="shared" si="11"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="160" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="187" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="188" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="189" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="190" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B141:B142"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="B120:B121"/>
     <mergeCell ref="B118:B119"/>
     <mergeCell ref="B85:B86"/>
     <mergeCell ref="B66:B67"/>
@@ -6332,11 +6330,17 @@
     <mergeCell ref="B97:B98"/>
     <mergeCell ref="B99:B100"/>
     <mergeCell ref="B116:B117"/>
-    <mergeCell ref="B141:B142"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6348,46 +6352,46 @@
   <dimension ref="B1:L99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11:L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="39.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="1.140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="1.5703125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="51.28515625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="9" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="2.1796875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="39.7265625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="1.1796875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="29.26953125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="1.54296875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="51.26953125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" style="9" customWidth="1"/>
+    <col min="13" max="16384" width="11.453125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-    </row>
-    <row r="3" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
@@ -6417,7 +6421,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>47</v>
       </c>
@@ -6446,7 +6450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="4">
         <v>48</v>
       </c>
@@ -6476,7 +6480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>49</v>
       </c>
@@ -6506,7 +6510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>50</v>
       </c>
@@ -6536,8 +6540,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>47</v>
       </c>
@@ -6567,7 +6571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>48</v>
       </c>
@@ -6597,7 +6601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>50</v>
       </c>
@@ -6622,13 +6626,13 @@
       <c r="K12" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="L12" s="12" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="12">
+        <f>L11+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>47</v>
       </c>
@@ -6653,12 +6657,12 @@
       <c r="K14" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="L14" s="12" t="e">
+      <c r="L14" s="12">
         <f>L12+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>48</v>
       </c>
@@ -6683,12 +6687,12 @@
       <c r="K15" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="L15" s="12" t="e">
+      <c r="L15" s="12">
         <f>L14+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>49</v>
       </c>
@@ -6713,12 +6717,12 @@
       <c r="K16" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="L16" s="12" t="e">
+      <c r="L16" s="12">
         <f t="shared" ref="L16:L17" si="1">L15+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
         <v>50</v>
       </c>
@@ -6743,15 +6747,15 @@
       <c r="K17" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="L17" s="12" t="e">
+      <c r="L17" s="12">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K18" s="16"/>
     </row>
-    <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <v>47</v>
       </c>
@@ -6776,12 +6780,12 @@
       <c r="K19" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="L19" s="12" t="e">
+      <c r="L19" s="12">
         <f>L17+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
         <v>48</v>
       </c>
@@ -6806,12 +6810,12 @@
       <c r="K20" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="L20" s="12" t="e">
+      <c r="L20" s="12">
         <f>L19+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="4">
         <v>49</v>
       </c>
@@ -6836,12 +6840,12 @@
       <c r="K21" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="L21" s="12" t="e">
+      <c r="L21" s="12">
         <f t="shared" ref="L21:L22" si="2">L20+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <v>50</v>
       </c>
@@ -6866,13 +6870,13 @@
       <c r="K22" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="L22" s="12" t="e">
+      <c r="L22" s="12">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="4">
         <v>47</v>
       </c>
@@ -6897,12 +6901,12 @@
       <c r="K24" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="L24" s="12" t="e">
+      <c r="L24" s="12">
         <f>L22+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <v>48</v>
       </c>
@@ -6927,12 +6931,12 @@
       <c r="K25" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="L25" s="12" t="e">
+      <c r="L25" s="12">
         <f>L24+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="4">
         <v>49</v>
       </c>
@@ -6957,12 +6961,12 @@
       <c r="K26" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="L26" s="12" t="e">
+      <c r="L26" s="12">
         <f t="shared" ref="L26:L27" si="3">L25+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
         <v>50</v>
       </c>
@@ -6987,15 +6991,15 @@
       <c r="K27" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="L27" s="12" t="e">
+      <c r="L27" s="12">
         <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K28" s="16"/>
     </row>
-    <row r="29" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="23" t="s">
         <v>233</v>
       </c>
@@ -7007,8 +7011,8 @@
       <c r="I29" s="9"/>
       <c r="K29" s="17"/>
     </row>
-    <row r="30" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
       <c r="C31" s="9" t="s">
         <v>199</v>
@@ -7031,12 +7035,12 @@
       <c r="K31" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="L31" s="12" t="e">
+      <c r="L31" s="12">
         <f>L27+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10">
         <v>1</v>
       </c>
@@ -7061,12 +7065,12 @@
       <c r="K32" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="L32" s="12" t="e">
+      <c r="L32" s="12">
         <f t="shared" ref="L32:L37" si="4">L31+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="10">
         <v>2</v>
       </c>
@@ -7091,12 +7095,12 @@
       <c r="K33" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="L33" s="12" t="e">
+      <c r="L33" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <v>56</v>
       </c>
@@ -7121,12 +7125,12 @@
       <c r="K34" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="L34" s="12" t="e">
+      <c r="L34" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
         <v>57</v>
       </c>
@@ -7151,12 +7155,12 @@
       <c r="K35" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="L35" s="12" t="e">
+      <c r="L35" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="6">
         <v>59</v>
       </c>
@@ -7181,12 +7185,12 @@
       <c r="K36" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="L36" s="12" t="e">
+      <c r="L36" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="6">
         <v>60</v>
       </c>
@@ -7211,14 +7215,14 @@
       <c r="K37" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="L37" s="12" t="e">
+      <c r="L37" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="21">
         <v>5</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -7242,13 +7246,13 @@
       <c r="K39" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="L39" s="12" t="e">
+      <c r="L39" s="12">
         <f>L37+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="20"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="21"/>
       <c r="C40" s="9" t="s">
         <v>199</v>
       </c>
@@ -7270,13 +7274,13 @@
       <c r="K40" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="L40" s="12" t="e">
+      <c r="L40" s="12">
         <f>L39+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="20">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="21">
         <v>6</v>
       </c>
       <c r="C41" s="9" t="s">
@@ -7300,13 +7304,13 @@
       <c r="K41" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="L41" s="12" t="e">
+      <c r="L41" s="12">
         <f t="shared" ref="L41:L58" si="5">L40+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="20"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="21"/>
       <c r="C42" s="9" t="s">
         <v>199</v>
       </c>
@@ -7328,13 +7332,13 @@
       <c r="K42" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="L42" s="12" t="e">
+      <c r="L42" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="21">
         <v>7</v>
       </c>
       <c r="C43" s="9" t="s">
@@ -7358,13 +7362,13 @@
       <c r="K43" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="L43" s="12" t="e">
+      <c r="L43" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="20"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="21"/>
       <c r="C44" s="9" t="s">
         <v>199</v>
       </c>
@@ -7386,13 +7390,13 @@
       <c r="K44" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="L44" s="12" t="e">
+      <c r="L44" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="21">
         <v>8</v>
       </c>
       <c r="C45" s="9" t="s">
@@ -7416,13 +7420,13 @@
       <c r="K45" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="L45" s="12" t="e">
+      <c r="L45" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="20"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="21"/>
       <c r="C46" s="9" t="s">
         <v>199</v>
       </c>
@@ -7444,13 +7448,13 @@
       <c r="K46" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="L46" s="12" t="e">
+      <c r="L46" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="20">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="21">
         <v>9</v>
       </c>
       <c r="C47" s="9" t="s">
@@ -7474,13 +7478,13 @@
       <c r="K47" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="L47" s="12" t="e">
+      <c r="L47" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="20"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="21"/>
       <c r="C48" s="9" t="s">
         <v>199</v>
       </c>
@@ -7502,13 +7506,13 @@
       <c r="K48" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="L48" s="12" t="e">
+      <c r="L48" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="20">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="21">
         <v>10</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -7532,13 +7536,13 @@
       <c r="K49" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="L49" s="12" t="e">
+      <c r="L49" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="20"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="21"/>
       <c r="C50" s="9" t="s">
         <v>199</v>
       </c>
@@ -7560,13 +7564,13 @@
       <c r="K50" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="L50" s="12" t="e">
+      <c r="L50" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="21">
         <v>14</v>
       </c>
       <c r="C51" s="9" t="s">
@@ -7590,13 +7594,13 @@
       <c r="K51" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="L51" s="12" t="e">
+      <c r="L51" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="20"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="21"/>
       <c r="C52" s="9" t="s">
         <v>199</v>
       </c>
@@ -7618,13 +7622,13 @@
       <c r="K52" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="L52" s="12" t="e">
+      <c r="L52" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="21">
         <v>15</v>
       </c>
       <c r="C53" s="9" t="s">
@@ -7648,13 +7652,13 @@
       <c r="K53" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="L53" s="12" t="e">
+      <c r="L53" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="20"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="21"/>
       <c r="C54" s="9" t="s">
         <v>199</v>
       </c>
@@ -7676,13 +7680,13 @@
       <c r="K54" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="L54" s="12" t="e">
+      <c r="L54" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="20">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="21">
         <v>16</v>
       </c>
       <c r="C55" s="9" t="s">
@@ -7706,13 +7710,13 @@
       <c r="K55" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="L55" s="12" t="e">
+      <c r="L55" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="20"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="21"/>
       <c r="C56" s="9" t="s">
         <v>199</v>
       </c>
@@ -7734,13 +7738,13 @@
       <c r="K56" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="L56" s="12" t="e">
+      <c r="L56" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="20">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="21">
         <v>17</v>
       </c>
       <c r="C57" s="9" t="s">
@@ -7764,13 +7768,13 @@
       <c r="K57" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="L57" s="12" t="e">
+      <c r="L57" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="20"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="21"/>
       <c r="C58" s="9" t="s">
         <v>199</v>
       </c>
@@ -7792,12 +7796,12 @@
       <c r="K58" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="L58" s="12" t="e">
+      <c r="L58" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="4">
         <v>56</v>
       </c>
@@ -7822,12 +7826,12 @@
       <c r="K59" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="L59" s="12" t="e">
+      <c r="L59" s="12">
         <f>L58+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="4">
         <v>57</v>
       </c>
@@ -7852,12 +7856,12 @@
       <c r="K60" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="L60" s="12" t="e">
+      <c r="L60" s="12">
         <f t="shared" ref="L60:L62" si="6">L59+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B61" s="6">
         <v>59</v>
       </c>
@@ -7882,12 +7886,12 @@
       <c r="K61" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="L61" s="12" t="e">
+      <c r="L61" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="6">
         <v>60</v>
       </c>
@@ -7912,13 +7916,13 @@
       <c r="K62" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="L62" s="12" t="e">
+      <c r="L62" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="23" t="s">
         <v>236</v>
       </c>
@@ -7931,13 +7935,13 @@
       <c r="I64" s="9"/>
       <c r="K64" s="17"/>
     </row>
-    <row r="65" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L65" s="9" t="e">
+    <row r="65" spans="2:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L65" s="9">
         <f>L77-L62</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="5"/>
       <c r="C66" s="9" t="s">
         <v>199</v>
@@ -7960,12 +7964,12 @@
       <c r="K66" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="L66" s="12" t="e">
+      <c r="L66" s="12">
         <f>L62+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="10">
         <v>1</v>
       </c>
@@ -7990,12 +7994,12 @@
       <c r="K67" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="L67" s="12" t="e">
+      <c r="L67" s="12">
         <f t="shared" ref="L67:L74" si="7">L66+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B68" s="10">
         <v>2</v>
       </c>
@@ -8020,12 +8024,12 @@
       <c r="K68" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="L68" s="12" t="e">
+      <c r="L68" s="12">
         <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="4">
         <v>56</v>
       </c>
@@ -8050,12 +8054,12 @@
       <c r="K69" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="L69" s="12" t="e">
+      <c r="L69" s="12">
         <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="4">
         <v>57</v>
       </c>
@@ -8080,13 +8084,13 @@
       <c r="K70" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="L70" s="12" t="e">
+      <c r="L70" s="12">
         <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="20">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="21">
         <v>1</v>
       </c>
       <c r="C71" s="9" t="s">
@@ -8110,13 +8114,13 @@
       <c r="K71" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="L71" s="12" t="e">
+      <c r="L71" s="12">
         <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="20"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="21"/>
       <c r="C72" s="9" t="s">
         <v>199</v>
       </c>
@@ -8138,13 +8142,13 @@
       <c r="K72" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="L72" s="12" t="e">
+      <c r="L72" s="12">
         <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="20">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="21">
         <v>2</v>
       </c>
       <c r="C73" s="9" t="s">
@@ -8168,13 +8172,13 @@
       <c r="K73" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="L73" s="12" t="e">
+      <c r="L73" s="12">
         <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="20"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="21"/>
       <c r="C74" s="9" t="s">
         <v>199</v>
       </c>
@@ -8196,12 +8200,12 @@
       <c r="K74" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="L74" s="12" t="e">
+      <c r="L74" s="12">
         <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="75" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="10">
         <v>18</v>
       </c>
@@ -8226,12 +8230,12 @@
       <c r="K75" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="L75" s="12" t="e">
+      <c r="L75" s="12">
         <f>L74+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="76" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="10">
         <v>19</v>
       </c>
@@ -8256,12 +8260,12 @@
       <c r="K76" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="L76" s="12" t="e">
+      <c r="L76" s="12">
         <f>L75+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="77" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="10">
         <v>20</v>
       </c>
@@ -8286,15 +8290,15 @@
       <c r="K77" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="L77" s="12" t="e">
+      <c r="L77" s="12">
         <f>L76+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="78" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K78" s="16"/>
     </row>
-    <row r="79" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="23" t="s">
         <v>233</v>
       </c>
@@ -8306,26 +8310,26 @@
       <c r="I79" s="9"/>
       <c r="K79" s="17"/>
     </row>
-    <row r="80" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="B39:B40"/>
@@ -8355,46 +8359,46 @@
   <dimension ref="B1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="D77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11:L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="39.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="1.140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="1.5703125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="51.7109375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="9" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="2.1796875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="39.7265625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="1.1796875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="29.26953125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="1.54296875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="51.7265625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" style="9" customWidth="1"/>
+    <col min="13" max="16384" width="11.453125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-    </row>
-    <row r="3" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
@@ -8424,7 +8428,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>47</v>
       </c>
@@ -8453,7 +8457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="4">
         <v>48</v>
       </c>
@@ -8483,7 +8487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>49</v>
       </c>
@@ -8513,7 +8517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>50</v>
       </c>
@@ -8543,8 +8547,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>47</v>
       </c>
@@ -8574,7 +8578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>48</v>
       </c>
@@ -8604,7 +8608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>50</v>
       </c>
@@ -8629,13 +8633,13 @@
       <c r="K12" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="L12" s="12" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="12">
+        <f>L11+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>47</v>
       </c>
@@ -8660,12 +8664,12 @@
       <c r="K14" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="L14" s="12" t="e">
+      <c r="L14" s="12">
         <f>L12+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>48</v>
       </c>
@@ -8690,12 +8694,12 @@
       <c r="K15" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="L15" s="12" t="e">
+      <c r="L15" s="12">
         <f>L14+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>49</v>
       </c>
@@ -8720,12 +8724,12 @@
       <c r="K16" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="L16" s="12" t="e">
+      <c r="L16" s="12">
         <f t="shared" ref="L16:L17" si="1">L15+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
         <v>50</v>
       </c>
@@ -8750,15 +8754,15 @@
       <c r="K17" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="L17" s="12" t="e">
+      <c r="L17" s="12">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K18" s="16"/>
     </row>
-    <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <v>47</v>
       </c>
@@ -8783,12 +8787,12 @@
       <c r="K19" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="L19" s="12" t="e">
+      <c r="L19" s="12">
         <f>L17+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
         <v>48</v>
       </c>
@@ -8813,12 +8817,12 @@
       <c r="K20" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="L20" s="12" t="e">
+      <c r="L20" s="12">
         <f>L19+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="4">
         <v>49</v>
       </c>
@@ -8843,12 +8847,12 @@
       <c r="K21" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="L21" s="12" t="e">
+      <c r="L21" s="12">
         <f t="shared" ref="L21:L22" si="2">L20+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <v>50</v>
       </c>
@@ -8873,13 +8877,13 @@
       <c r="K22" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="L22" s="12" t="e">
+      <c r="L22" s="12">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="4">
         <v>47</v>
       </c>
@@ -8904,12 +8908,12 @@
       <c r="K24" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="L24" s="12" t="e">
+      <c r="L24" s="12">
         <f>L22+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <v>48</v>
       </c>
@@ -8934,12 +8938,12 @@
       <c r="K25" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="L25" s="12" t="e">
+      <c r="L25" s="12">
         <f>L24+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="4">
         <v>49</v>
       </c>
@@ -8964,12 +8968,12 @@
       <c r="K26" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="L26" s="12" t="e">
+      <c r="L26" s="12">
         <f t="shared" ref="L26:L27" si="3">L25+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
         <v>50</v>
       </c>
@@ -8994,15 +8998,15 @@
       <c r="K27" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="L27" s="12" t="e">
+      <c r="L27" s="12">
         <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K28" s="16"/>
     </row>
-    <row r="29" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="23" t="s">
         <v>233</v>
       </c>
@@ -9016,8 +9020,8 @@
       <c r="I29" s="24"/>
       <c r="K29" s="17"/>
     </row>
-    <row r="30" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
       <c r="C31" s="9" t="s">
         <v>251</v>
@@ -9040,12 +9044,12 @@
       <c r="K31" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="L31" s="12" t="e">
+      <c r="L31" s="12">
         <f>L27+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10">
         <v>1</v>
       </c>
@@ -9070,12 +9074,12 @@
       <c r="K32" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="L32" s="12" t="e">
+      <c r="L32" s="12">
         <f>L31+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="10">
         <v>2</v>
       </c>
@@ -9100,12 +9104,12 @@
       <c r="K33" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="L33" s="12" t="e">
+      <c r="L33" s="12">
         <f t="shared" ref="L33:L37" si="4">L32+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <v>56</v>
       </c>
@@ -9130,12 +9134,12 @@
       <c r="K34" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="L34" s="12" t="e">
+      <c r="L34" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
         <v>57</v>
       </c>
@@ -9160,12 +9164,12 @@
       <c r="K35" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="L35" s="12" t="e">
+      <c r="L35" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="6">
         <v>59</v>
       </c>
@@ -9190,12 +9194,12 @@
       <c r="K36" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="L36" s="12" t="e">
+      <c r="L36" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="6">
         <v>60</v>
       </c>
@@ -9220,13 +9224,13 @@
       <c r="K37" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="L37" s="12" t="e">
+      <c r="L37" s="12">
         <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="18">
         <v>53</v>
       </c>
@@ -9251,12 +9255,12 @@
       <c r="K39" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="L39" s="12" t="e">
+      <c r="L39" s="12">
         <f>L37+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="18">
         <v>53</v>
       </c>
@@ -9281,12 +9285,12 @@
       <c r="K40" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="L40" s="12" t="e">
+      <c r="L40" s="12">
         <f t="shared" ref="L40:L42" si="5">L39+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="18">
         <v>54</v>
       </c>
@@ -9311,12 +9315,12 @@
       <c r="K41" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="L41" s="12" t="e">
+      <c r="L41" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="18">
         <v>54</v>
       </c>
@@ -9341,14 +9345,14 @@
       <c r="K42" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="L42" s="12" t="e">
+      <c r="L42" s="12">
         <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="21">
         <v>5</v>
       </c>
       <c r="C44" s="9" t="s">
@@ -9372,13 +9376,13 @@
       <c r="K44" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="L44" s="12" t="e">
+      <c r="L44" s="12">
         <f>L42+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="20"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="21"/>
       <c r="C45" s="9" t="s">
         <v>251</v>
       </c>
@@ -9400,13 +9404,13 @@
       <c r="K45" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="L45" s="12" t="e">
+      <c r="L45" s="12">
         <f t="shared" ref="L45:L63" si="6">L44+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="21">
         <v>6</v>
       </c>
       <c r="C46" s="9" t="s">
@@ -9430,13 +9434,13 @@
       <c r="K46" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="L46" s="12" t="e">
+      <c r="L46" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="20"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="21"/>
       <c r="C47" s="9" t="s">
         <v>251</v>
       </c>
@@ -9458,13 +9462,13 @@
       <c r="K47" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="L47" s="12" t="e">
+      <c r="L47" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="20">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="21">
         <v>7</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -9488,13 +9492,13 @@
       <c r="K48" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="L48" s="12" t="e">
+      <c r="L48" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="20"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="21"/>
       <c r="C49" s="9" t="s">
         <v>251</v>
       </c>
@@ -9516,13 +9520,13 @@
       <c r="K49" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="L49" s="12" t="e">
+      <c r="L49" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="20">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="21">
         <v>8</v>
       </c>
       <c r="C50" s="9" t="s">
@@ -9546,13 +9550,13 @@
       <c r="K50" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="L50" s="12" t="e">
+      <c r="L50" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="20"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="21"/>
       <c r="C51" s="9" t="s">
         <v>251</v>
       </c>
@@ -9574,13 +9578,13 @@
       <c r="K51" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="L51" s="12" t="e">
+      <c r="L51" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="21">
         <v>9</v>
       </c>
       <c r="C52" s="9" t="s">
@@ -9604,13 +9608,13 @@
       <c r="K52" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="L52" s="12" t="e">
+      <c r="L52" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="20"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="21"/>
       <c r="C53" s="9" t="s">
         <v>251</v>
       </c>
@@ -9632,13 +9636,13 @@
       <c r="K53" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="L53" s="12" t="e">
+      <c r="L53" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="21">
         <v>10</v>
       </c>
       <c r="C54" s="9" t="s">
@@ -9662,13 +9666,13 @@
       <c r="K54" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="L54" s="12" t="e">
+      <c r="L54" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="20"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="21"/>
       <c r="C55" s="9" t="s">
         <v>251</v>
       </c>
@@ -9690,13 +9694,13 @@
       <c r="K55" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="L55" s="12" t="e">
+      <c r="L55" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="20">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="21">
         <v>14</v>
       </c>
       <c r="C56" s="9" t="s">
@@ -9720,13 +9724,13 @@
       <c r="K56" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="L56" s="12" t="e">
+      <c r="L56" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="20"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="21"/>
       <c r="C57" s="9" t="s">
         <v>251</v>
       </c>
@@ -9748,13 +9752,13 @@
       <c r="K57" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="L57" s="12" t="e">
+      <c r="L57" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="20">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="21">
         <v>15</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -9778,13 +9782,13 @@
       <c r="K58" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="L58" s="12" t="e">
+      <c r="L58" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="20"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="21"/>
       <c r="C59" s="9" t="s">
         <v>251</v>
       </c>
@@ -9806,13 +9810,13 @@
       <c r="K59" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="L59" s="12" t="e">
+      <c r="L59" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="21">
         <v>16</v>
       </c>
       <c r="C60" s="9" t="s">
@@ -9836,13 +9840,13 @@
       <c r="K60" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L60" s="12" t="e">
+      <c r="L60" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="21"/>
       <c r="C61" s="9" t="s">
         <v>251</v>
       </c>
@@ -9864,13 +9868,13 @@
       <c r="K61" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="L61" s="12" t="e">
+      <c r="L61" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="20">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="21">
         <v>17</v>
       </c>
       <c r="C62" s="9" t="s">
@@ -9894,13 +9898,13 @@
       <c r="K62" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="L62" s="12" t="e">
+      <c r="L62" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="20"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="21"/>
       <c r="C63" s="9" t="s">
         <v>251</v>
       </c>
@@ -9922,12 +9926,12 @@
       <c r="K63" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="L63" s="12" t="e">
+      <c r="L63" s="12">
         <f t="shared" si="6"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="6">
         <v>59</v>
       </c>
@@ -9952,12 +9956,12 @@
       <c r="K64" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="L64" s="12" t="e">
+      <c r="L64" s="12">
         <f>L63+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" s="6">
         <v>60</v>
       </c>
@@ -9982,13 +9986,13 @@
       <c r="K65" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="L65" s="12" t="e">
+      <c r="L65" s="12">
         <f t="shared" ref="L65" si="7">L64+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="67" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="23" t="s">
         <v>236</v>
       </c>
@@ -10001,8 +10005,8 @@
       <c r="I67" s="9"/>
       <c r="K67" s="17"/>
     </row>
-    <row r="68" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="5"/>
       <c r="C69" s="9" t="s">
         <v>251</v>
@@ -10025,12 +10029,12 @@
       <c r="K69" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="L69" s="12" t="e">
+      <c r="L69" s="12">
         <f>L65+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="10">
         <v>1</v>
       </c>
@@ -10055,12 +10059,12 @@
       <c r="K70" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="L70" s="12" t="e">
+      <c r="L70" s="12">
         <f>L69+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="10">
         <v>2</v>
       </c>
@@ -10085,12 +10089,12 @@
       <c r="K71" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="L71" s="12" t="e">
+      <c r="L71" s="12">
         <f t="shared" ref="L71:L73" si="8">L70+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" s="4">
         <v>56</v>
       </c>
@@ -10115,12 +10119,12 @@
       <c r="K72" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="L72" s="12" t="e">
+      <c r="L72" s="12">
         <f t="shared" si="8"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="4">
         <v>57</v>
       </c>
@@ -10145,13 +10149,13 @@
       <c r="K73" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="L73" s="12" t="e">
+      <c r="L73" s="12">
         <f t="shared" si="8"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="20">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="21">
         <v>1</v>
       </c>
       <c r="C74" s="9" t="s">
@@ -10175,13 +10179,13 @@
       <c r="K74" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="L74" s="12" t="e">
+      <c r="L74" s="12">
         <f>L73+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="75" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="20"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="21"/>
       <c r="C75" s="9" t="s">
         <v>251</v>
       </c>
@@ -10203,13 +10207,13 @@
       <c r="K75" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="L75" s="12" t="e">
+      <c r="L75" s="12">
         <f t="shared" ref="L75:L77" si="9">L74+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="76" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="20">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="21">
         <v>2</v>
       </c>
       <c r="C76" s="9" t="s">
@@ -10233,13 +10237,13 @@
       <c r="K76" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="L76" s="12" t="e">
+      <c r="L76" s="12">
         <f t="shared" si="9"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="77" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="20"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B77" s="21"/>
       <c r="C77" s="9" t="s">
         <v>251</v>
       </c>
@@ -10261,12 +10265,12 @@
       <c r="K77" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="L77" s="12" t="e">
+      <c r="L77" s="12">
         <f t="shared" si="9"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="78" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="10">
         <v>18</v>
       </c>
@@ -10291,12 +10295,12 @@
       <c r="K78" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="L78" s="12" t="e">
+      <c r="L78" s="12">
         <f>L77+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="79" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="10">
         <v>19</v>
       </c>
@@ -10321,12 +10325,12 @@
       <c r="K79" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="L79" s="12" t="e">
+      <c r="L79" s="12">
         <f>L78+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="80" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="10">
         <v>20</v>
       </c>
@@ -10351,15 +10355,15 @@
       <c r="K80" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="L80" s="12" t="e">
+      <c r="L80" s="12">
         <f>L79+1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K81" s="16"/>
     </row>
-    <row r="82" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B82" s="23" t="s">
         <v>233</v>
       </c>
@@ -10373,39 +10377,28 @@
       <c r="I82" s="24"/>
       <c r="K82" s="17"/>
     </row>
-    <row r="83" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="100" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="101" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B67:H67"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B50:B51"/>
@@ -10413,6 +10406,17 @@
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B74:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
treeviewitemUnlock does not work properly
</commit_message>
<xml_diff>
--- a/FreeWork/ADECUA/AppFinalQt/database.xlsx
+++ b/FreeWork/ADECUA/AppFinalQt/database.xlsx
@@ -285,6 +285,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -727,7 +795,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K5" s="25" t="inlineStr">
+      <c r="K5" s="26" t="inlineStr">
         <is>
           <t>DB-P1-00-LC1A</t>
         </is>

</xml_diff>

<commit_message>
treeview item locked/unlocked done!
</commit_message>
<xml_diff>
--- a/FreeWork/ADECUA/AppFinalQt/database.xlsx
+++ b/FreeWork/ADECUA/AppFinalQt/database.xlsx
@@ -285,74 +285,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -834,7 +766,7 @@
       <c r="I6" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="9" t="inlineStr">
+      <c r="K6" s="26" t="inlineStr">
         <is>
           <t>DB-P1-00-3MF_1D.A_E</t>
         </is>
@@ -1762,7 +1694,7 @@
       <c r="I33" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="K33" s="9" t="inlineStr">
+      <c r="K33" s="26" t="inlineStr">
         <is>
           <t>DB-P2-00-3MF_1D.A</t>
         </is>

</xml_diff>

<commit_message>
load locked items form the excel y solved some bugs
</commit_message>
<xml_diff>
--- a/FreeWork/ADECUA/AppFinalQt/database.xlsx
+++ b/FreeWork/ADECUA/AppFinalQt/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -220,9 +220,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -247,25 +244,28 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -615,11 +615,11 @@
   </sheetPr>
   <dimension ref="B2:M159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="D173" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="D143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="K152" sqref="K152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -637,13 +637,13 @@
     <col width="52" customWidth="1" style="25" min="11" max="11"/>
     <col width="22.5703125" customWidth="1" style="25" min="12" max="12"/>
     <col width="20.42578125" customWidth="1" style="25" min="13" max="13"/>
-    <col width="11.42578125" customWidth="1" style="25" min="14" max="14"/>
-    <col width="11.42578125" customWidth="1" style="25" min="15" max="16384"/>
+    <col width="11.42578125" customWidth="1" style="25" min="14" max="17"/>
+    <col width="11.42578125" customWidth="1" style="25" min="18" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="6" customHeight="1"/>
     <row r="2" ht="49.5" customHeight="1">
-      <c r="B2" s="22" t="inlineStr">
+      <c r="B2" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">D     I     S     E     Ñ     O           B     A     S     E </t>
         </is>
@@ -651,48 +651,48 @@
     </row>
     <row r="3" ht="4.5" customHeight="1"/>
     <row r="4" ht="50.1" customHeight="1">
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nº                                   Plano </t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="9" t="inlineStr">
         <is>
           <t>Estructura</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>Perfil</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="9" t="inlineStr">
         <is>
           <t>Planta</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>Tipología</t>
         </is>
       </c>
-      <c r="G4" s="11" t="n"/>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="G4" s="10" t="n"/>
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Situación </t>
         </is>
       </c>
-      <c r="I4" s="10" t="inlineStr">
+      <c r="I4" s="9" t="inlineStr">
         <is>
           <t>Nº         Dormit.</t>
         </is>
       </c>
-      <c r="K4" s="10" t="inlineStr">
+      <c r="K4" s="9" t="inlineStr">
         <is>
           <t>Nombre del Archivo (.jpg)</t>
         </is>
       </c>
-      <c r="L4" s="12" t="inlineStr">
+      <c r="L4" s="11" t="inlineStr">
         <is>
           <t>orden de Imágenes</t>
         </is>
@@ -728,17 +728,17 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K5" s="18" t="inlineStr">
+      <c r="K5" s="15" t="inlineStr">
         <is>
           <t>DB-P1-00-LC1A</t>
         </is>
       </c>
-      <c r="L5" s="9" t="n">
+      <c r="L5" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="18" customHeight="1">
-      <c r="B6" s="19" t="n">
+      <c r="B6" s="21" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="25" t="inlineStr">
@@ -767,17 +767,17 @@
       <c r="I6" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="18" t="inlineStr">
+      <c r="K6" s="15" t="inlineStr">
         <is>
           <t>DB-P1-00-3MF_1D.A_E</t>
         </is>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1">
-      <c r="B7" s="19" t="n">
+      <c r="B7" s="21" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="25" t="inlineStr">
@@ -806,12 +806,12 @@
       <c r="I7" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="25" t="inlineStr">
+      <c r="K7" s="15" t="inlineStr">
         <is>
           <t>DB-P1-00-3MF_1D.B_E</t>
         </is>
       </c>
-      <c r="L7" s="9" t="n">
+      <c r="L7" s="8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -851,7 +851,7 @@
           <t>DB-P1-01-3MP_2D.A</t>
         </is>
       </c>
-      <c r="L9" s="9" t="n">
+      <c r="L9" s="8" t="n">
         <v>4</v>
       </c>
     </row>
@@ -890,7 +890,7 @@
           <t>DB-P1-01-3MP_3D.A</t>
         </is>
       </c>
-      <c r="L10" s="9" t="n">
+      <c r="L10" s="8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -929,7 +929,7 @@
           <t>DB-P1-01-3MP_3D.B</t>
         </is>
       </c>
-      <c r="L11" s="9" t="n">
+      <c r="L11" s="8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -968,7 +968,7 @@
           <t>DB-P1-01-3MP_3D.C</t>
         </is>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="8" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
           <t>DB-P1-01-3MP_3D.D</t>
         </is>
       </c>
-      <c r="L13" s="9" t="n">
+      <c r="L13" s="8" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
           <t>DB-P1-01-3MP_4D.A</t>
         </is>
       </c>
-      <c r="L14" s="9" t="n">
+      <c r="L14" s="8" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1085,7 +1085,7 @@
           <t>DB-P1-01-3MP_4D.B</t>
         </is>
       </c>
-      <c r="L15" s="9" t="n">
+      <c r="L15" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1120,12 +1120,12 @@
       <c r="I17" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="K17" s="25" t="inlineStr">
+      <c r="K17" s="15" t="inlineStr">
         <is>
           <t>DB-P1-02-3MP_2D.A</t>
         </is>
       </c>
-      <c r="L17" s="9" t="n">
+      <c r="L17" s="8" t="n">
         <v>11</v>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
           <t>DB-P1-02-3MP_3D.A</t>
         </is>
       </c>
-      <c r="L18" s="9" t="n">
+      <c r="L18" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1203,7 +1203,7 @@
           <t>DB-P1-02-3MP_3D.B</t>
         </is>
       </c>
-      <c r="L19" s="9" t="n">
+      <c r="L19" s="8" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1242,7 +1242,7 @@
           <t>DB-P1-02-3MP_3D.C</t>
         </is>
       </c>
-      <c r="L20" s="9" t="n">
+      <c r="L20" s="8" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
           <t>DB-P1-02-3MP_3D.D</t>
         </is>
       </c>
-      <c r="L21" s="9" t="n">
+      <c r="L21" s="8" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
           <t>DB-P1-02-3MP_4D.A</t>
         </is>
       </c>
-      <c r="L22" s="9" t="n">
+      <c r="L22" s="8" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1359,13 +1359,13 @@
           <t>DB-P1-02-3MP_4D.B</t>
         </is>
       </c>
-      <c r="L23" s="9" t="n">
+      <c r="L23" s="8" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="24" ht="3" customHeight="1"/>
     <row r="25" ht="18" customHeight="1">
-      <c r="B25" s="19" t="n">
+      <c r="B25" s="21" t="n">
         <v>3</v>
       </c>
       <c r="C25" s="25" t="inlineStr">
@@ -1399,12 +1399,12 @@
           <t>DB-P1-03-3MF_1D.A_E</t>
         </is>
       </c>
-      <c r="L25" s="9" t="n">
+      <c r="L25" s="8" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="1">
-      <c r="B26" s="19" t="n">
+      <c r="B26" s="21" t="n">
         <v>4</v>
       </c>
       <c r="C26" s="25" t="inlineStr">
@@ -1438,12 +1438,12 @@
           <t>DB-P1-03-3MF_1D.B_E</t>
         </is>
       </c>
-      <c r="L26" s="9" t="n">
+      <c r="L26" s="8" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="27" ht="18" customHeight="1">
-      <c r="B27" s="21" t="n">
+      <c r="B27" s="22" t="n">
         <v>61</v>
       </c>
       <c r="C27" s="25" t="inlineStr">
@@ -1479,12 +1479,12 @@
           <t>DB-P1-03_Atico-3MF_0D.A_DA&amp;3MF_2D.A1_DA</t>
         </is>
       </c>
-      <c r="L27" s="9" t="n">
+      <c r="L27" s="8" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="B28" s="21" t="n">
+      <c r="B28" s="22" t="n">
         <v>62</v>
       </c>
       <c r="C28" s="25" t="inlineStr">
@@ -1520,12 +1520,12 @@
           <t>DB-P1-03_Atico-3MF_0D.B&amp;3MF_2D.A2</t>
         </is>
       </c>
-      <c r="L28" s="9" t="n">
+      <c r="L28" s="8" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1">
-      <c r="B29" s="21" t="n">
+      <c r="B29" s="22" t="n">
         <v>63</v>
       </c>
       <c r="C29" s="25" t="inlineStr">
@@ -1561,12 +1561,12 @@
           <t>DB-P1-03_Atico-3MF_1D.A&amp;3MF_3D.A1</t>
         </is>
       </c>
-      <c r="L29" s="9" t="n">
+      <c r="L29" s="8" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="30" ht="18" customHeight="1">
-      <c r="B30" s="21" t="n">
+      <c r="B30" s="22" t="n">
         <v>64</v>
       </c>
       <c r="C30" s="25" t="inlineStr">
@@ -1602,7 +1602,7 @@
           <t>DB-P1-03_Atico-3MF_0D.C&amp;3MF_3D.A2</t>
         </is>
       </c>
-      <c r="L30" s="9" t="n">
+      <c r="L30" s="8" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1642,12 +1642,12 @@
           <t>DB-P2-00-LC1B</t>
         </is>
       </c>
-      <c r="L32" s="9" t="n">
+      <c r="L32" s="8" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="1">
-      <c r="B33" s="19" t="n">
+      <c r="B33" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="25" t="inlineStr">
@@ -1676,17 +1676,17 @@
       <c r="I33" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K33" s="18" t="inlineStr">
+      <c r="K33" s="15" t="inlineStr">
         <is>
           <t>DB-P2-00-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L33" s="9" t="n">
+      <c r="L33" s="8" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="1">
-      <c r="B34" s="19" t="n">
+      <c r="B34" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C34" s="25" t="inlineStr">
@@ -1720,7 +1720,7 @@
           <t>DB-P2-00-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L34" s="9" t="n">
+      <c r="L34" s="8" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
           <t>DB-P2-00-2MP_1D.A</t>
         </is>
       </c>
-      <c r="L35" s="9" t="n">
+      <c r="L35" s="8" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1798,7 +1798,7 @@
           <t>DB-P2-00-2MP_2D.A</t>
         </is>
       </c>
-      <c r="L36" s="9" t="n">
+      <c r="L36" s="8" t="n">
         <v>28</v>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
           <t>DB-P2-00-2MP_2D.B</t>
         </is>
       </c>
-      <c r="L37" s="9" t="n">
+      <c r="L37" s="8" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1876,7 +1876,7 @@
           <t>DB-P2-00-2MP_2D.C</t>
         </is>
       </c>
-      <c r="L38" s="9" t="n">
+      <c r="L38" s="8" t="n">
         <v>30</v>
       </c>
     </row>
@@ -1915,7 +1915,7 @@
           <t>DB-P2-00-2MP_2D.D</t>
         </is>
       </c>
-      <c r="L39" s="9" t="n">
+      <c r="L39" s="8" t="n">
         <v>31</v>
       </c>
     </row>
@@ -1954,7 +1954,7 @@
           <t>DB-P2-00-2MP_2D.A_MIN</t>
         </is>
       </c>
-      <c r="L40" s="9" t="n">
+      <c r="L40" s="8" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1993,12 +1993,12 @@
           <t>DB-P2-00-2MP_2D.B_MIN</t>
         </is>
       </c>
-      <c r="L41" s="9" t="n">
+      <c r="L41" s="8" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="1">
-      <c r="B42" s="15" t="n">
+      <c r="B42" s="14" t="n">
         <v>12</v>
       </c>
       <c r="C42" s="25" t="inlineStr">
@@ -2032,12 +2032,12 @@
           <t>DB-P2-00-2ME_1D.A</t>
         </is>
       </c>
-      <c r="L42" s="9" t="n">
+      <c r="L42" s="8" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="1">
-      <c r="B43" s="15" t="n">
+      <c r="B43" s="14" t="n">
         <v>13</v>
       </c>
       <c r="C43" s="25" t="inlineStr">
@@ -2071,12 +2071,12 @@
           <t>DB-P2-00-2ME_1D.B</t>
         </is>
       </c>
-      <c r="L43" s="9" t="n">
+      <c r="L43" s="8" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="44" ht="18" customHeight="1">
-      <c r="B44" s="15" t="n">
+      <c r="B44" s="14" t="n">
         <v>29</v>
       </c>
       <c r="C44" s="25" t="inlineStr">
@@ -2110,12 +2110,12 @@
           <t>DB-P2-00-2ME_2D.A</t>
         </is>
       </c>
-      <c r="L44" s="9" t="n">
+      <c r="L44" s="8" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="45" ht="18" customHeight="1">
-      <c r="B45" s="15" t="n">
+      <c r="B45" s="14" t="n">
         <v>30</v>
       </c>
       <c r="C45" s="25" t="inlineStr">
@@ -2149,12 +2149,12 @@
           <t>DB-P2-00-2ME_2D.B</t>
         </is>
       </c>
-      <c r="L45" s="9" t="n">
+      <c r="L45" s="8" t="n">
         <v>37</v>
       </c>
     </row>
     <row r="46" ht="18" customHeight="1">
-      <c r="B46" s="15" t="n">
+      <c r="B46" s="14" t="n">
         <v>31</v>
       </c>
       <c r="C46" s="25" t="inlineStr">
@@ -2188,13 +2188,13 @@
           <t>DB-P2-00-2ME_2D.C</t>
         </is>
       </c>
-      <c r="L46" s="9" t="n">
+      <c r="L46" s="8" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="47" ht="11.25" customHeight="1"/>
     <row r="48" ht="18" customHeight="1">
-      <c r="B48" s="19" t="n">
+      <c r="B48" s="21" t="n">
         <v>5</v>
       </c>
       <c r="C48" s="25" t="inlineStr">
@@ -2228,7 +2228,7 @@
           <t>DB-P2.1-01-4MF_1D.A</t>
         </is>
       </c>
-      <c r="L48" s="9" t="n">
+      <c r="L48" s="8" t="n">
         <v>39</v>
       </c>
     </row>
@@ -2264,12 +2264,12 @@
           <t>DB-P2.2-01-4MF_1D.A</t>
         </is>
       </c>
-      <c r="L49" s="9" t="n">
+      <c r="L49" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="50" ht="18" customHeight="1">
-      <c r="B50" s="19" t="n">
+      <c r="B50" s="21" t="n">
         <v>6</v>
       </c>
       <c r="C50" s="25" t="inlineStr">
@@ -2303,7 +2303,7 @@
           <t>DB-P2.1-01-4MF_1D.B</t>
         </is>
       </c>
-      <c r="L50" s="9" t="n">
+      <c r="L50" s="8" t="n">
         <v>41</v>
       </c>
     </row>
@@ -2339,12 +2339,12 @@
           <t>DB-P2.2-01-4MF_1D.B</t>
         </is>
       </c>
-      <c r="L51" s="9" t="n">
+      <c r="L51" s="8" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="52" ht="18" customHeight="1">
-      <c r="B52" s="19" t="n">
+      <c r="B52" s="21" t="n">
         <v>7</v>
       </c>
       <c r="C52" s="25" t="inlineStr">
@@ -2378,7 +2378,7 @@
           <t>DB-P2.1-01-4MF_1D.C</t>
         </is>
       </c>
-      <c r="L52" s="9" t="n">
+      <c r="L52" s="8" t="n">
         <v>43</v>
       </c>
     </row>
@@ -2414,12 +2414,12 @@
           <t>DB-P2.2-01-4MF_1D.C</t>
         </is>
       </c>
-      <c r="L53" s="9" t="n">
+      <c r="L53" s="8" t="n">
         <v>44</v>
       </c>
     </row>
     <row r="54" ht="18" customHeight="1">
-      <c r="B54" s="19" t="n">
+      <c r="B54" s="21" t="n">
         <v>8</v>
       </c>
       <c r="C54" s="25" t="inlineStr">
@@ -2453,7 +2453,7 @@
           <t>DB-P2.1-01-4MF_1D.D</t>
         </is>
       </c>
-      <c r="L54" s="9" t="n">
+      <c r="L54" s="8" t="n">
         <v>45</v>
       </c>
     </row>
@@ -2489,12 +2489,12 @@
           <t>DB-P2.2-01-4MF_1D.D</t>
         </is>
       </c>
-      <c r="L55" s="9" t="n">
+      <c r="L55" s="8" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="56" ht="18" customHeight="1">
-      <c r="B56" s="19" t="n">
+      <c r="B56" s="21" t="n">
         <v>9</v>
       </c>
       <c r="C56" s="25" t="inlineStr">
@@ -2528,7 +2528,7 @@
           <t>DB-P2.1-01-4MF_1D.E</t>
         </is>
       </c>
-      <c r="L56" s="9" t="n">
+      <c r="L56" s="8" t="n">
         <v>47</v>
       </c>
     </row>
@@ -2564,12 +2564,12 @@
           <t>DB-P2.2-01-4MF_1D.E</t>
         </is>
       </c>
-      <c r="L57" s="9" t="n">
+      <c r="L57" s="8" t="n">
         <v>48</v>
       </c>
     </row>
     <row r="58" ht="18" customHeight="1">
-      <c r="B58" s="19" t="n">
+      <c r="B58" s="21" t="n">
         <v>10</v>
       </c>
       <c r="C58" s="25" t="inlineStr">
@@ -2603,7 +2603,7 @@
           <t>DB-P2.1-01-4MF_1D.MINUS.</t>
         </is>
       </c>
-      <c r="L58" s="9" t="n">
+      <c r="L58" s="8" t="n">
         <v>49</v>
       </c>
     </row>
@@ -2639,12 +2639,12 @@
           <t>DB-P2.2-01-4MF_1D.MINUS.</t>
         </is>
       </c>
-      <c r="L59" s="9" t="n">
+      <c r="L59" s="8" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="60" ht="18" customHeight="1">
-      <c r="B60" s="19" t="n">
+      <c r="B60" s="21" t="n">
         <v>14</v>
       </c>
       <c r="C60" s="25" t="inlineStr">
@@ -2678,7 +2678,7 @@
           <t>DB-P2.1-01-4MF_2D.A</t>
         </is>
       </c>
-      <c r="L60" s="9" t="n">
+      <c r="L60" s="8" t="n">
         <v>51</v>
       </c>
     </row>
@@ -2714,12 +2714,12 @@
           <t>DB-P2.2-01-4MF_2D.A</t>
         </is>
       </c>
-      <c r="L61" s="9" t="n">
+      <c r="L61" s="8" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="62" ht="18" customHeight="1">
-      <c r="B62" s="19" t="n">
+      <c r="B62" s="21" t="n">
         <v>15</v>
       </c>
       <c r="C62" s="25" t="inlineStr">
@@ -2753,7 +2753,7 @@
           <t>DB-P2.1-01-4MF_2D.B</t>
         </is>
       </c>
-      <c r="L62" s="9" t="n">
+      <c r="L62" s="8" t="n">
         <v>53</v>
       </c>
     </row>
@@ -2789,12 +2789,12 @@
           <t>DB-P2.2-01-4MF_2D.B</t>
         </is>
       </c>
-      <c r="L63" s="9" t="n">
+      <c r="L63" s="8" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="64" ht="18" customHeight="1">
-      <c r="B64" s="19" t="n">
+      <c r="B64" s="21" t="n">
         <v>16</v>
       </c>
       <c r="C64" s="25" t="inlineStr">
@@ -2828,7 +2828,7 @@
           <t>DB-P2.1-01-4MF_2D.C</t>
         </is>
       </c>
-      <c r="L64" s="9" t="n">
+      <c r="L64" s="8" t="n">
         <v>55</v>
       </c>
     </row>
@@ -2864,12 +2864,12 @@
           <t>DB-P2.2-01-4MF_2D.C</t>
         </is>
       </c>
-      <c r="L65" s="9" t="n">
+      <c r="L65" s="8" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="66" ht="18" customHeight="1">
-      <c r="B66" s="19" t="n">
+      <c r="B66" s="21" t="n">
         <v>17</v>
       </c>
       <c r="C66" s="25" t="inlineStr">
@@ -2903,7 +2903,7 @@
           <t>DB-P2.1-01-4MF_2D.D</t>
         </is>
       </c>
-      <c r="L66" s="9" t="n">
+      <c r="L66" s="8" t="n">
         <v>57</v>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
           <t>DB-P2.2-01-4MF_2D.D</t>
         </is>
       </c>
-      <c r="L67" s="9" t="n">
+      <c r="L67" s="8" t="n">
         <v>58</v>
       </c>
     </row>
@@ -2978,7 +2978,7 @@
           <t>DB-P2-01-2MP_1D.A</t>
         </is>
       </c>
-      <c r="L68" s="9" t="n">
+      <c r="L68" s="8" t="n">
         <v>59</v>
       </c>
     </row>
@@ -3017,7 +3017,7 @@
           <t>DB-P2-01-2MP_2D.A</t>
         </is>
       </c>
-      <c r="L69" s="9" t="n">
+      <c r="L69" s="8" t="n">
         <v>60</v>
       </c>
     </row>
@@ -3056,7 +3056,7 @@
           <t>DB-P2-01-2MP_2D.B</t>
         </is>
       </c>
-      <c r="L70" s="9" t="n">
+      <c r="L70" s="8" t="n">
         <v>61</v>
       </c>
     </row>
@@ -3095,7 +3095,7 @@
           <t>DB-P2-01-2MP_2D.C</t>
         </is>
       </c>
-      <c r="L71" s="9" t="n">
+      <c r="L71" s="8" t="n">
         <v>62</v>
       </c>
     </row>
@@ -3134,7 +3134,7 @@
           <t>DB-P2-01-2MP_2D.D</t>
         </is>
       </c>
-      <c r="L72" s="9" t="n">
+      <c r="L72" s="8" t="n">
         <v>63</v>
       </c>
     </row>
@@ -3173,7 +3173,7 @@
           <t>DB-P2-01-2MP_2D.A_MIN</t>
         </is>
       </c>
-      <c r="L73" s="9" t="n">
+      <c r="L73" s="8" t="n">
         <v>64</v>
       </c>
     </row>
@@ -3212,12 +3212,12 @@
           <t>DB-P2-01-2MP_2D.B_MIN</t>
         </is>
       </c>
-      <c r="L74" s="9" t="n">
+      <c r="L74" s="8" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="75" ht="18" customHeight="1">
-      <c r="B75" s="15" t="n">
+      <c r="B75" s="14" t="n">
         <v>12</v>
       </c>
       <c r="C75" s="25" t="inlineStr">
@@ -3251,12 +3251,12 @@
           <t>DB-P2-01-2ME_1D.A</t>
         </is>
       </c>
-      <c r="L75" s="9" t="n">
+      <c r="L75" s="8" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="76" ht="18" customHeight="1">
-      <c r="B76" s="15" t="n">
+      <c r="B76" s="14" t="n">
         <v>13</v>
       </c>
       <c r="C76" s="25" t="inlineStr">
@@ -3290,12 +3290,12 @@
           <t>DB-P2-01-2ME_1D.B</t>
         </is>
       </c>
-      <c r="L76" s="9" t="n">
+      <c r="L76" s="8" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="77" ht="18" customHeight="1">
-      <c r="B77" s="15" t="n">
+      <c r="B77" s="14" t="n">
         <v>29</v>
       </c>
       <c r="C77" s="25" t="inlineStr">
@@ -3329,12 +3329,12 @@
           <t>DB-P2-01-2ME_2D.A</t>
         </is>
       </c>
-      <c r="L77" s="9" t="n">
+      <c r="L77" s="8" t="n">
         <v>68</v>
       </c>
     </row>
     <row r="78" ht="18" customHeight="1">
-      <c r="B78" s="15" t="n">
+      <c r="B78" s="14" t="n">
         <v>30</v>
       </c>
       <c r="C78" s="25" t="inlineStr">
@@ -3368,12 +3368,12 @@
           <t>DB-P2-01-2ME_2D.B</t>
         </is>
       </c>
-      <c r="L78" s="9" t="n">
+      <c r="L78" s="8" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="79" ht="18" customHeight="1">
-      <c r="B79" s="15" t="n">
+      <c r="B79" s="14" t="n">
         <v>31</v>
       </c>
       <c r="C79" s="25" t="inlineStr">
@@ -3407,13 +3407,13 @@
           <t>DB-P2-01-2ME_2D.C</t>
         </is>
       </c>
-      <c r="L79" s="9" t="n">
+      <c r="L79" s="8" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="80" ht="3" customHeight="1"/>
     <row r="81" ht="18" customHeight="1">
-      <c r="B81" s="19" t="n">
+      <c r="B81" s="21" t="n">
         <v>5</v>
       </c>
       <c r="C81" s="25" t="inlineStr">
@@ -3447,7 +3447,7 @@
           <t>DB-P2.1-02-4MF_1D.A</t>
         </is>
       </c>
-      <c r="L81" s="9" t="n">
+      <c r="L81" s="8" t="n">
         <v>71</v>
       </c>
     </row>
@@ -3483,12 +3483,12 @@
           <t>DB-P2.2-02-4MF_1D.A</t>
         </is>
       </c>
-      <c r="L82" s="9" t="n">
+      <c r="L82" s="8" t="n">
         <v>72</v>
       </c>
     </row>
     <row r="83" ht="18" customHeight="1">
-      <c r="B83" s="19" t="n">
+      <c r="B83" s="21" t="n">
         <v>6</v>
       </c>
       <c r="C83" s="25" t="inlineStr">
@@ -3522,7 +3522,7 @@
           <t>DB-P2.1-02-4MF_1D.B</t>
         </is>
       </c>
-      <c r="L83" s="9" t="n">
+      <c r="L83" s="8" t="n">
         <v>73</v>
       </c>
     </row>
@@ -3558,12 +3558,12 @@
           <t>DB-P2.2-02-4MF_1D.B</t>
         </is>
       </c>
-      <c r="L84" s="9" t="n">
+      <c r="L84" s="8" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="85" ht="18" customHeight="1">
-      <c r="B85" s="19" t="n">
+      <c r="B85" s="21" t="n">
         <v>7</v>
       </c>
       <c r="C85" s="25" t="inlineStr">
@@ -3597,7 +3597,7 @@
           <t>DB-P2.1-02-4MF_1D.C</t>
         </is>
       </c>
-      <c r="L85" s="9" t="n">
+      <c r="L85" s="8" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3633,12 +3633,12 @@
           <t>DB-P2.2-02-4MF_1D.C</t>
         </is>
       </c>
-      <c r="L86" s="9" t="n">
+      <c r="L86" s="8" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="87" ht="18" customHeight="1">
-      <c r="B87" s="19" t="n">
+      <c r="B87" s="21" t="n">
         <v>8</v>
       </c>
       <c r="C87" s="25" t="inlineStr">
@@ -3672,7 +3672,7 @@
           <t>DB-P2.1-02-4MF_1D.D</t>
         </is>
       </c>
-      <c r="L87" s="9" t="n">
+      <c r="L87" s="8" t="n">
         <v>77</v>
       </c>
     </row>
@@ -3708,12 +3708,12 @@
           <t>DB-P2.2-02-4MF_1D.D</t>
         </is>
       </c>
-      <c r="L88" s="9" t="n">
+      <c r="L88" s="8" t="n">
         <v>78</v>
       </c>
     </row>
     <row r="89" ht="18" customHeight="1">
-      <c r="B89" s="19" t="n">
+      <c r="B89" s="21" t="n">
         <v>9</v>
       </c>
       <c r="C89" s="25" t="inlineStr">
@@ -3747,7 +3747,7 @@
           <t>DB-P2.1-02-4MF_1D.E</t>
         </is>
       </c>
-      <c r="L89" s="9" t="n">
+      <c r="L89" s="8" t="n">
         <v>79</v>
       </c>
     </row>
@@ -3783,12 +3783,12 @@
           <t>DB-P2.2-02-4MF_1D.E</t>
         </is>
       </c>
-      <c r="L90" s="9" t="n">
+      <c r="L90" s="8" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="91" ht="18" customHeight="1">
-      <c r="B91" s="19" t="n">
+      <c r="B91" s="21" t="n">
         <v>10</v>
       </c>
       <c r="C91" s="25" t="inlineStr">
@@ -3822,7 +3822,7 @@
           <t>DB-P2.1-02-4MF_1D.MINUS.</t>
         </is>
       </c>
-      <c r="L91" s="9" t="n">
+      <c r="L91" s="8" t="n">
         <v>81</v>
       </c>
     </row>
@@ -3858,12 +3858,12 @@
           <t>DB-P2.2-02-4MF_1D.MINUS.</t>
         </is>
       </c>
-      <c r="L92" s="9" t="n">
+      <c r="L92" s="8" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="93" ht="18" customHeight="1">
-      <c r="B93" s="19" t="n">
+      <c r="B93" s="21" t="n">
         <v>14</v>
       </c>
       <c r="C93" s="25" t="inlineStr">
@@ -3897,7 +3897,7 @@
           <t>DB-P2.1-02-4MF_2D.A</t>
         </is>
       </c>
-      <c r="L93" s="9" t="n">
+      <c r="L93" s="8" t="n">
         <v>83</v>
       </c>
     </row>
@@ -3933,12 +3933,12 @@
           <t>DB-P2.2-02-4MF_2D.A</t>
         </is>
       </c>
-      <c r="L94" s="9" t="n">
+      <c r="L94" s="8" t="n">
         <v>84</v>
       </c>
     </row>
     <row r="95" ht="18" customHeight="1">
-      <c r="B95" s="19" t="n">
+      <c r="B95" s="21" t="n">
         <v>15</v>
       </c>
       <c r="C95" s="25" t="inlineStr">
@@ -3972,7 +3972,7 @@
           <t>DB-P2.1-02-4MF_2D.B</t>
         </is>
       </c>
-      <c r="L95" s="9" t="n">
+      <c r="L95" s="8" t="n">
         <v>85</v>
       </c>
     </row>
@@ -4008,12 +4008,12 @@
           <t>DB-P2.2-02-4MF_2D.B</t>
         </is>
       </c>
-      <c r="L96" s="9" t="n">
+      <c r="L96" s="8" t="n">
         <v>86</v>
       </c>
     </row>
     <row r="97" ht="18" customHeight="1">
-      <c r="B97" s="19" t="n">
+      <c r="B97" s="21" t="n">
         <v>16</v>
       </c>
       <c r="C97" s="25" t="inlineStr">
@@ -4047,7 +4047,7 @@
           <t>DB-P2.1-02-4MF_2D.C</t>
         </is>
       </c>
-      <c r="L97" s="9" t="n">
+      <c r="L97" s="8" t="n">
         <v>87</v>
       </c>
     </row>
@@ -4083,12 +4083,12 @@
           <t>DB-P2.2-02-4MF_2D.C</t>
         </is>
       </c>
-      <c r="L98" s="9" t="n">
+      <c r="L98" s="8" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="99" ht="18" customHeight="1">
-      <c r="B99" s="19" t="n">
+      <c r="B99" s="21" t="n">
         <v>17</v>
       </c>
       <c r="C99" s="25" t="inlineStr">
@@ -4122,7 +4122,7 @@
           <t>DB-P2.1-02-4MF_2D.D</t>
         </is>
       </c>
-      <c r="L99" s="9" t="n">
+      <c r="L99" s="8" t="n">
         <v>89</v>
       </c>
     </row>
@@ -4158,7 +4158,7 @@
           <t>DB-P2.2-02-4MF_2D.D</t>
         </is>
       </c>
-      <c r="L100" s="9" t="n">
+      <c r="L100" s="8" t="n">
         <v>90</v>
       </c>
     </row>
@@ -4197,7 +4197,7 @@
           <t>DB-P2-02-2MP_1D.A</t>
         </is>
       </c>
-      <c r="L101" s="9" t="n">
+      <c r="L101" s="8" t="n">
         <v>91</v>
       </c>
     </row>
@@ -4236,7 +4236,7 @@
           <t>DB-P2-02-2MP_2D.A</t>
         </is>
       </c>
-      <c r="L102" s="9" t="n">
+      <c r="L102" s="8" t="n">
         <v>92</v>
       </c>
     </row>
@@ -4275,7 +4275,7 @@
           <t>DB-P2-02-2MP_2D.B</t>
         </is>
       </c>
-      <c r="L103" s="9" t="n">
+      <c r="L103" s="8" t="n">
         <v>93</v>
       </c>
     </row>
@@ -4314,7 +4314,7 @@
           <t>DB-P2-02-2MP_2D.C</t>
         </is>
       </c>
-      <c r="L104" s="9" t="n">
+      <c r="L104" s="8" t="n">
         <v>94</v>
       </c>
     </row>
@@ -4353,7 +4353,7 @@
           <t>DB-P2-02-2MP_2D.D</t>
         </is>
       </c>
-      <c r="L105" s="9" t="n">
+      <c r="L105" s="8" t="n">
         <v>95</v>
       </c>
     </row>
@@ -4392,7 +4392,7 @@
           <t>DB-P2-02-2MP_2D.A_MIN</t>
         </is>
       </c>
-      <c r="L106" s="9" t="n">
+      <c r="L106" s="8" t="n">
         <v>96</v>
       </c>
     </row>
@@ -4431,12 +4431,12 @@
           <t>DB-P2-02-2MP_2D.B_MIN</t>
         </is>
       </c>
-      <c r="L107" s="9" t="n">
+      <c r="L107" s="8" t="n">
         <v>97</v>
       </c>
     </row>
     <row r="108" ht="18" customHeight="1">
-      <c r="B108" s="15" t="n">
+      <c r="B108" s="14" t="n">
         <v>12</v>
       </c>
       <c r="C108" s="25" t="inlineStr">
@@ -4470,12 +4470,12 @@
           <t>DB-P2-02-2ME_1D.A</t>
         </is>
       </c>
-      <c r="L108" s="9" t="n">
+      <c r="L108" s="8" t="n">
         <v>98</v>
       </c>
     </row>
     <row r="109" ht="18" customHeight="1">
-      <c r="B109" s="15" t="n">
+      <c r="B109" s="14" t="n">
         <v>13</v>
       </c>
       <c r="C109" s="25" t="inlineStr">
@@ -4509,12 +4509,12 @@
           <t>DB-P2-02-2ME_1D.B</t>
         </is>
       </c>
-      <c r="L109" s="9" t="n">
+      <c r="L109" s="8" t="n">
         <v>99</v>
       </c>
     </row>
     <row r="110" ht="18" customHeight="1">
-      <c r="B110" s="15" t="n">
+      <c r="B110" s="14" t="n">
         <v>29</v>
       </c>
       <c r="C110" s="25" t="inlineStr">
@@ -4548,12 +4548,12 @@
           <t>DB-P2-02-2ME_2D.A</t>
         </is>
       </c>
-      <c r="L110" s="9" t="n">
+      <c r="L110" s="8" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="111" ht="18" customHeight="1">
-      <c r="B111" s="15" t="n">
+      <c r="B111" s="14" t="n">
         <v>30</v>
       </c>
       <c r="C111" s="25" t="inlineStr">
@@ -4587,12 +4587,12 @@
           <t>DB-P2-02-2ME_2D.B</t>
         </is>
       </c>
-      <c r="L111" s="9" t="n">
+      <c r="L111" s="8" t="n">
         <v>101</v>
       </c>
     </row>
     <row r="112" ht="18" customHeight="1">
-      <c r="B112" s="15" t="n">
+      <c r="B112" s="14" t="n">
         <v>31</v>
       </c>
       <c r="C112" s="25" t="inlineStr">
@@ -4626,15 +4626,15 @@
           <t>DB-P2-02-2ME_2D.C</t>
         </is>
       </c>
-      <c r="L112" s="9" t="n">
+      <c r="L112" s="8" t="n">
         <v>102</v>
       </c>
     </row>
     <row r="113" ht="3" customHeight="1">
-      <c r="L113" s="9" t="n"/>
+      <c r="L113" s="8" t="n"/>
     </row>
     <row r="114" ht="18" customHeight="1">
-      <c r="B114" s="19" t="n">
+      <c r="B114" s="21" t="n">
         <v>43</v>
       </c>
       <c r="C114" s="25" t="inlineStr">
@@ -4668,12 +4668,12 @@
           <t>DB-P2-03-6MF_4D.A</t>
         </is>
       </c>
-      <c r="L114" s="9" t="n">
+      <c r="L114" s="8" t="n">
         <v>103</v>
       </c>
     </row>
     <row r="115" ht="18" customHeight="1">
-      <c r="B115" s="19" t="n">
+      <c r="B115" s="21" t="n">
         <v>44</v>
       </c>
       <c r="C115" s="25" t="inlineStr">
@@ -4707,12 +4707,12 @@
           <t>DB-P2-03-6MF_4D.B</t>
         </is>
       </c>
-      <c r="L115" s="9" t="n">
+      <c r="L115" s="8" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="116" ht="18" customHeight="1">
-      <c r="B116" s="21" t="n">
+      <c r="B116" s="22" t="n">
         <v>61</v>
       </c>
       <c r="C116" s="25" t="inlineStr">
@@ -4748,7 +4748,7 @@
           <t>DB-P2.1-03_Atico-3MF_0D.A_DA&amp;3MF_2D.A1_DA</t>
         </is>
       </c>
-      <c r="L116" s="9" t="n">
+      <c r="L116" s="8" t="n">
         <v>105</v>
       </c>
       <c r="M116" s="25" t="inlineStr">
@@ -4791,12 +4791,12 @@
           <t>DB-P2.2-03_Atico-3MF_0D.A_DA&amp;3MF_2D.A1_DA</t>
         </is>
       </c>
-      <c r="L117" s="9" t="n">
+      <c r="L117" s="8" t="n">
         <v>106</v>
       </c>
     </row>
     <row r="118" ht="18" customHeight="1">
-      <c r="B118" s="21" t="n">
+      <c r="B118" s="22" t="n">
         <v>63</v>
       </c>
       <c r="C118" s="25" t="inlineStr">
@@ -4832,7 +4832,7 @@
           <t>DB-P2.1-03_Atico-3MF_1D.A&amp;3MF_3D.A2</t>
         </is>
       </c>
-      <c r="L118" s="9" t="n">
+      <c r="L118" s="8" t="n">
         <v>107</v>
       </c>
     </row>
@@ -4870,12 +4870,12 @@
           <t>DB-P2.2-03_Atico-3MF_1D.A&amp;3MF_3D.A2</t>
         </is>
       </c>
-      <c r="L119" s="9" t="n">
+      <c r="L119" s="8" t="n">
         <v>108</v>
       </c>
     </row>
     <row r="120" ht="18" customHeight="1">
-      <c r="B120" s="21" t="n">
+      <c r="B120" s="22" t="n">
         <v>64</v>
       </c>
       <c r="C120" s="25" t="inlineStr">
@@ -4911,7 +4911,7 @@
           <t>DB-P2.1-03_Atico-3MF_0D.C&amp;3MF_3D.A1</t>
         </is>
       </c>
-      <c r="L120" s="9" t="n">
+      <c r="L120" s="8" t="n">
         <v>109</v>
       </c>
     </row>
@@ -4949,12 +4949,12 @@
           <t>DB-P2.2-03_Atico-3MF_0D.C&amp;3MF_3D.A1</t>
         </is>
       </c>
-      <c r="L121" s="9" t="n">
+      <c r="L121" s="8" t="n">
         <v>110</v>
       </c>
     </row>
     <row r="122" ht="18" customHeight="1">
-      <c r="B122" s="8" t="n">
+      <c r="B122" s="7" t="n">
         <v>67</v>
       </c>
       <c r="C122" s="25" t="inlineStr">
@@ -4990,7 +4990,7 @@
           <t>DB-P2-03_Atico-2ME_1D.A&amp;2ME_0D.1</t>
         </is>
       </c>
-      <c r="L122" s="9" t="n">
+      <c r="L122" s="8" t="n">
         <v>111</v>
       </c>
     </row>
@@ -5030,12 +5030,12 @@
           <t>DB-P3-00-LC3</t>
         </is>
       </c>
-      <c r="L124" s="9" t="n">
+      <c r="L124" s="8" t="n">
         <v>112</v>
       </c>
     </row>
     <row r="125" ht="18" customHeight="1">
-      <c r="B125" s="19" t="n">
+      <c r="B125" s="21" t="n">
         <v>18</v>
       </c>
       <c r="C125" s="25" t="inlineStr">
@@ -5069,12 +5069,12 @@
           <t>DB-P3-00-5MF_2D.A_E</t>
         </is>
       </c>
-      <c r="L125" s="9" t="n">
+      <c r="L125" s="8" t="n">
         <v>113</v>
       </c>
     </row>
     <row r="126" ht="18" customHeight="1">
-      <c r="B126" s="19" t="n">
+      <c r="B126" s="21" t="n">
         <v>19</v>
       </c>
       <c r="C126" s="25" t="inlineStr">
@@ -5108,12 +5108,12 @@
           <t>DB-P3-00-5MF_2D.B_E</t>
         </is>
       </c>
-      <c r="L126" s="9" t="n">
+      <c r="L126" s="8" t="n">
         <v>114</v>
       </c>
     </row>
     <row r="127" ht="18" customHeight="1">
-      <c r="B127" s="19" t="n">
+      <c r="B127" s="21" t="n">
         <v>20</v>
       </c>
       <c r="C127" s="25" t="inlineStr">
@@ -5147,13 +5147,13 @@
           <t>DB-P3-00-5MF_2D.C_E</t>
         </is>
       </c>
-      <c r="L127" s="9" t="n">
+      <c r="L127" s="8" t="n">
         <v>115</v>
       </c>
     </row>
     <row r="128" ht="3" customHeight="1"/>
     <row r="129" ht="18" customHeight="1">
-      <c r="B129" s="19" t="n">
+      <c r="B129" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C129" s="25" t="inlineStr">
@@ -5187,7 +5187,7 @@
           <t>DB-P3.1-01-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L129" s="9" t="n">
+      <c r="L129" s="8" t="n">
         <v>116</v>
       </c>
     </row>
@@ -5223,12 +5223,12 @@
           <t>DB-P3.2-01-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L130" s="9" t="n">
+      <c r="L130" s="8" t="n">
         <v>117</v>
       </c>
     </row>
     <row r="131" ht="18" customHeight="1">
-      <c r="B131" s="19" t="n">
+      <c r="B131" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C131" s="25" t="inlineStr">
@@ -5262,7 +5262,7 @@
           <t>DB-P3.1-01-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L131" s="9" t="n">
+      <c r="L131" s="8" t="n">
         <v>118</v>
       </c>
     </row>
@@ -5298,7 +5298,7 @@
           <t>DB-P3.2-01-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L132" s="9" t="n">
+      <c r="L132" s="8" t="n">
         <v>119</v>
       </c>
     </row>
@@ -5332,12 +5332,12 @@
       <c r="I133" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K133" s="26" t="inlineStr">
+      <c r="K133" s="15" t="inlineStr">
         <is>
           <t>DB-P3-01-2MP_1D.A</t>
         </is>
       </c>
-      <c r="L133" s="9" t="n">
+      <c r="L133" s="8" t="n">
         <v>120</v>
       </c>
     </row>
@@ -5376,7 +5376,7 @@
           <t>DB-P3-01-2MP_2D.A</t>
         </is>
       </c>
-      <c r="L134" s="9" t="n">
+      <c r="L134" s="8" t="n">
         <v>121</v>
       </c>
     </row>
@@ -5415,7 +5415,7 @@
           <t>DB-P3-01-2MP_2D.B</t>
         </is>
       </c>
-      <c r="L135" s="9" t="n">
+      <c r="L135" s="8" t="n">
         <v>122</v>
       </c>
     </row>
@@ -5454,7 +5454,7 @@
           <t>DB-P3-01-2MP_2D.C</t>
         </is>
       </c>
-      <c r="L136" s="9" t="n">
+      <c r="L136" s="8" t="n">
         <v>123</v>
       </c>
     </row>
@@ -5493,7 +5493,7 @@
           <t>DB-P3-01-2MP_2D.D</t>
         </is>
       </c>
-      <c r="L137" s="9" t="n">
+      <c r="L137" s="8" t="n">
         <v>124</v>
       </c>
     </row>
@@ -5532,7 +5532,7 @@
           <t>DB-P3-01-2MP_2D.A_MIN</t>
         </is>
       </c>
-      <c r="L138" s="9" t="n">
+      <c r="L138" s="8" t="n">
         <v>125</v>
       </c>
     </row>
@@ -5571,13 +5571,13 @@
           <t>DB-P3-01-2MP_2D.B_MIN</t>
         </is>
       </c>
-      <c r="L139" s="9" t="n">
+      <c r="L139" s="8" t="n">
         <v>126</v>
       </c>
     </row>
     <row r="140" ht="3" customHeight="1"/>
     <row r="141" ht="18" customHeight="1">
-      <c r="B141" s="19" t="n">
+      <c r="B141" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C141" s="25" t="inlineStr">
@@ -5611,7 +5611,7 @@
           <t>DB-P3.1-02-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L141" s="9" t="n">
+      <c r="L141" s="8" t="n">
         <v>127</v>
       </c>
     </row>
@@ -5647,12 +5647,12 @@
           <t>DB-P3.2-02-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L142" s="9" t="n">
+      <c r="L142" s="8" t="n">
         <v>128</v>
       </c>
     </row>
     <row r="143" ht="18" customHeight="1">
-      <c r="B143" s="19" t="n">
+      <c r="B143" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C143" s="25" t="inlineStr">
@@ -5686,7 +5686,7 @@
           <t>DB-P3.1-02-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L143" s="9" t="n">
+      <c r="L143" s="8" t="n">
         <v>129</v>
       </c>
     </row>
@@ -5722,7 +5722,7 @@
           <t>DB-P3.2-02-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L144" s="9" t="n">
+      <c r="L144" s="8" t="n">
         <v>130</v>
       </c>
     </row>
@@ -5761,7 +5761,7 @@
           <t>DB-P3-02-2MP_1D.A</t>
         </is>
       </c>
-      <c r="L145" s="9" t="n">
+      <c r="L145" s="8" t="n">
         <v>131</v>
       </c>
     </row>
@@ -5800,7 +5800,7 @@
           <t>DB-P3-02-2MP_2D.A</t>
         </is>
       </c>
-      <c r="L146" s="9" t="n">
+      <c r="L146" s="8" t="n">
         <v>132</v>
       </c>
     </row>
@@ -5839,7 +5839,7 @@
           <t>DB-P3-02-2MP_2D.B</t>
         </is>
       </c>
-      <c r="L147" s="9" t="n">
+      <c r="L147" s="8" t="n">
         <v>133</v>
       </c>
     </row>
@@ -5878,7 +5878,7 @@
           <t>DB-P3-02-2MP_2D.C</t>
         </is>
       </c>
-      <c r="L148" s="9" t="n">
+      <c r="L148" s="8" t="n">
         <v>134</v>
       </c>
     </row>
@@ -5917,7 +5917,7 @@
           <t>DB-P3-02-2MP_2D.D</t>
         </is>
       </c>
-      <c r="L149" s="9" t="n">
+      <c r="L149" s="8" t="n">
         <v>135</v>
       </c>
     </row>
@@ -5956,7 +5956,7 @@
           <t>DB-P3-02-2MP_2D.A_MIN</t>
         </is>
       </c>
-      <c r="L150" s="9" t="n">
+      <c r="L150" s="8" t="n">
         <v>136</v>
       </c>
     </row>
@@ -5995,13 +5995,13 @@
           <t>DB-P3-02-2MP_2D.B_MIN</t>
         </is>
       </c>
-      <c r="L151" s="9" t="n">
+      <c r="L151" s="8" t="n">
         <v>137</v>
       </c>
     </row>
     <row r="152" ht="3" customHeight="1"/>
     <row r="153" ht="18" customHeight="1">
-      <c r="B153" s="19" t="n">
+      <c r="B153" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C153" s="25" t="inlineStr">
@@ -6035,12 +6035,12 @@
           <t>DB-P3-03-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L153" s="9" t="n">
+      <c r="L153" s="8" t="n">
         <v>138</v>
       </c>
     </row>
     <row r="154" ht="18" customHeight="1">
-      <c r="B154" s="19" t="n">
+      <c r="B154" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C154" s="25" t="inlineStr">
@@ -6074,12 +6074,12 @@
           <t>DB-P3-03-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L154" s="9" t="n">
+      <c r="L154" s="8" t="n">
         <v>139</v>
       </c>
     </row>
     <row r="155" ht="18" customHeight="1">
-      <c r="B155" s="21" t="n">
+      <c r="B155" s="22" t="n">
         <v>61</v>
       </c>
       <c r="C155" s="25" t="inlineStr">
@@ -6110,17 +6110,17 @@
       <c r="I155" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="K155" s="18" t="inlineStr">
+      <c r="K155" s="15" t="inlineStr">
         <is>
           <t>DB-P3-03_Atico-3MF_0D.A_DA&amp;3MF_2D.A1_DA</t>
         </is>
       </c>
-      <c r="L155" s="9" t="n">
+      <c r="L155" s="8" t="n">
         <v>140</v>
       </c>
     </row>
     <row r="156" ht="18" customHeight="1">
-      <c r="B156" s="21" t="n">
+      <c r="B156" s="22" t="n">
         <v>62</v>
       </c>
       <c r="C156" s="25" t="inlineStr">
@@ -6156,12 +6156,12 @@
           <t>DB-P3-03_Atico-3MF_0D.B&amp;3MF_2D.2</t>
         </is>
       </c>
-      <c r="L156" s="9" t="n">
+      <c r="L156" s="8" t="n">
         <v>141</v>
       </c>
     </row>
     <row r="157" ht="18" customHeight="1">
-      <c r="B157" s="21" t="n">
+      <c r="B157" s="22" t="n">
         <v>63</v>
       </c>
       <c r="C157" s="25" t="inlineStr">
@@ -6197,12 +6197,12 @@
           <t>DB-P3-03_Atico-3MF_1D.A&amp;3MF_3D.A2</t>
         </is>
       </c>
-      <c r="L157" s="9" t="n">
+      <c r="L157" s="8" t="n">
         <v>142</v>
       </c>
     </row>
     <row r="158" ht="18" customHeight="1">
-      <c r="B158" s="21" t="n">
+      <c r="B158" s="22" t="n">
         <v>64</v>
       </c>
       <c r="C158" s="25" t="inlineStr">
@@ -6238,7 +6238,7 @@
           <t>DB-P3-03_Atico-3MF_0D.C&amp;3MF_3D.A1</t>
         </is>
       </c>
-      <c r="L158" s="9" t="n">
+      <c r="L158" s="8" t="n">
         <v>143</v>
       </c>
     </row>
@@ -6279,7 +6279,7 @@
           <t>DB-P3-03_Atico-2MP_1D.B&amp;2MP_1D.1</t>
         </is>
       </c>
-      <c r="L159" s="9" t="n">
+      <c r="L159" s="8" t="n">
         <v>144</v>
       </c>
     </row>
@@ -6316,17 +6316,11 @@
     <row r="190" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B141:B142"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="B120:B121"/>
     <mergeCell ref="B118:B119"/>
     <mergeCell ref="B85:B86"/>
     <mergeCell ref="B66:B67"/>
@@ -6339,11 +6333,17 @@
     <mergeCell ref="B97:B98"/>
     <mergeCell ref="B99:B100"/>
     <mergeCell ref="B116:B117"/>
-    <mergeCell ref="B141:B142"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>
@@ -6379,13 +6379,13 @@
     <col width="1.5703125" customWidth="1" style="25" min="10" max="10"/>
     <col width="51.28515625" customWidth="1" style="25" min="11" max="11"/>
     <col width="10.7109375" customWidth="1" style="25" min="12" max="12"/>
-    <col width="11.42578125" customWidth="1" style="25" min="13" max="13"/>
-    <col width="11.42578125" customWidth="1" style="25" min="14" max="16384"/>
+    <col width="11.42578125" customWidth="1" style="25" min="13" max="16"/>
+    <col width="11.42578125" customWidth="1" style="25" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="6" customHeight="1"/>
     <row r="2" ht="49.5" customHeight="1">
-      <c r="B2" s="22" t="inlineStr">
+      <c r="B2" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">V     E     R     S     I     Ó      N           1     </t>
         </is>
@@ -6393,48 +6393,48 @@
     </row>
     <row r="3" ht="4.5" customHeight="1"/>
     <row r="4" ht="50.1" customHeight="1">
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nº                                   Plano </t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="9" t="inlineStr">
         <is>
           <t>Estructura</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>Perfil</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="9" t="inlineStr">
         <is>
           <t>Planta</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>Tipología</t>
         </is>
       </c>
-      <c r="G4" s="11" t="n"/>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="G4" s="10" t="n"/>
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Situación </t>
         </is>
       </c>
-      <c r="I4" s="10" t="inlineStr">
+      <c r="I4" s="9" t="inlineStr">
         <is>
           <t>Nº         Dormit.</t>
         </is>
       </c>
-      <c r="K4" s="10" t="inlineStr">
+      <c r="K4" s="9" t="inlineStr">
         <is>
           <t>Nombre del Archivo (.jpg)</t>
         </is>
       </c>
-      <c r="L4" s="12" t="inlineStr">
+      <c r="L4" s="11" t="inlineStr">
         <is>
           <t>orden de Imágenes</t>
         </is>
@@ -6477,7 +6477,7 @@
           <t>V1-P1-00&amp;01A-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L5" s="9" t="n">
+      <c r="L5" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6518,7 +6518,7 @@
           <t>V1-P1-00&amp;01A-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -6559,7 +6559,7 @@
           <t>V1-P1-00&amp;01A-DUPLEX_3MF_1D.B&amp;3MF_3D.2</t>
         </is>
       </c>
-      <c r="L7" s="9" t="n">
+      <c r="L7" s="8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6600,7 +6600,7 @@
           <t>V1-P1-00&amp;01A-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L8" s="9" t="n">
+      <c r="L8" s="8" t="n">
         <v>4</v>
       </c>
     </row>
@@ -6642,7 +6642,7 @@
           <t>V1-P1-00&amp;01B-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L10" s="9" t="n">
+      <c r="L10" s="8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6683,7 +6683,7 @@
           <t>V1-P1-00&amp;01B-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L11" s="9" t="n">
+      <c r="L11" s="8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -6724,7 +6724,7 @@
           <t>V1-P1-00&amp;01B-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="8" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6766,7 +6766,7 @@
           <t>V1-P1-01&amp;02A-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L14" s="9" t="n">
+      <c r="L14" s="8" t="n">
         <v>8</v>
       </c>
     </row>
@@ -6807,7 +6807,7 @@
           <t>V1-P1-01&amp;02A-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L15" s="9" t="n">
+      <c r="L15" s="8" t="n">
         <v>9</v>
       </c>
     </row>
@@ -6848,7 +6848,7 @@
           <t>V1-P1-01&amp;02A-DUPLEX_3MF_1D.B&amp;3MF_3D.2</t>
         </is>
       </c>
-      <c r="L16" s="9" t="n">
+      <c r="L16" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -6889,12 +6889,12 @@
           <t>V1-P1-01&amp;02A-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L17" s="9" t="n">
+      <c r="L17" s="8" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="18" ht="4.5" customHeight="1">
-      <c r="K18" s="13" t="n"/>
+      <c r="K18" s="12" t="n"/>
     </row>
     <row r="19" ht="20.1" customHeight="1">
       <c r="B19" s="4" t="n">
@@ -6933,7 +6933,7 @@
           <t>V1-P1-01&amp;02B-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L19" s="9" t="n">
+      <c r="L19" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -6974,7 +6974,7 @@
           <t>V1-P1-01&amp;02B-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L20" s="9" t="n">
+      <c r="L20" s="8" t="n">
         <v>13</v>
       </c>
     </row>
@@ -7015,7 +7015,7 @@
           <t>V1-P1-01&amp;02B-DUPLEX_3MF_1D.B&amp;3MF_3D.2</t>
         </is>
       </c>
-      <c r="L21" s="9" t="n">
+      <c r="L21" s="8" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7056,7 +7056,7 @@
           <t>V1-P1-01&amp;02B-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L22" s="9" t="n">
+      <c r="L22" s="8" t="n">
         <v>15</v>
       </c>
     </row>
@@ -7098,7 +7098,7 @@
           <t>V1-P1-02&amp;03A-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L24" s="9" t="n">
+      <c r="L24" s="8" t="n">
         <v>16</v>
       </c>
     </row>
@@ -7139,7 +7139,7 @@
           <t>V1-P1-02&amp;03A-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L25" s="9" t="n">
+      <c r="L25" s="8" t="n">
         <v>17</v>
       </c>
     </row>
@@ -7180,7 +7180,7 @@
           <t>V1-P1-02&amp;03A-DUPLEX_3MF_1D.B&amp;3MF_3D.2</t>
         </is>
       </c>
-      <c r="L26" s="9" t="n">
+      <c r="L26" s="8" t="n">
         <v>18</v>
       </c>
     </row>
@@ -7221,12 +7221,12 @@
           <t>V1-P1-02&amp;03A-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L27" s="9" t="n">
+      <c r="L27" s="8" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="28" ht="4.5" customHeight="1">
-      <c r="K28" s="13" t="n"/>
+      <c r="K28" s="12" t="n"/>
     </row>
     <row r="29" ht="25.5" customHeight="1">
       <c r="B29" s="23" t="inlineStr">
@@ -7234,7 +7234,7 @@
           <t>LOS ÁTICOS SE DESCRIBEN EN EL DISEÑO BASE</t>
         </is>
       </c>
-      <c r="K29" s="13" t="n"/>
+      <c r="K29" s="12" t="n"/>
     </row>
     <row r="30" ht="50.1" customHeight="1"/>
     <row r="31" ht="18" customHeight="1">
@@ -7272,12 +7272,12 @@
           <t>V1-P2-00-LC2</t>
         </is>
       </c>
-      <c r="L31" s="9" t="n">
+      <c r="L31" s="8" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="1">
-      <c r="B32" s="19" t="n">
+      <c r="B32" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="25" t="inlineStr">
@@ -7311,12 +7311,12 @@
           <t>V1-P2-00-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L32" s="9" t="n">
+      <c r="L32" s="8" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="1">
-      <c r="B33" s="19" t="n">
+      <c r="B33" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C33" s="25" t="inlineStr">
@@ -7350,7 +7350,7 @@
           <t>V1-P2-00-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L33" s="9" t="n">
+      <c r="L33" s="8" t="n">
         <v>22</v>
       </c>
     </row>
@@ -7391,7 +7391,7 @@
           <t>V1-P2-00&amp;01AB-DUPLEX_2MP_1D.B&amp;2MP_3D.2</t>
         </is>
       </c>
-      <c r="L34" s="9" t="n">
+      <c r="L34" s="8" t="n">
         <v>23</v>
       </c>
     </row>
@@ -7432,7 +7432,7 @@
           <t>V1-P2-00&amp;01AB-DUPLEX_2MP_1D.C&amp;2MP_4D.1</t>
         </is>
       </c>
-      <c r="L35" s="9" t="n">
+      <c r="L35" s="8" t="n">
         <v>24</v>
       </c>
     </row>
@@ -7473,7 +7473,7 @@
           <t>V1-P2-00&amp;01AB-DUPLEX_2ME_1D.B&amp;2ME_3D.1</t>
         </is>
       </c>
-      <c r="L36" s="9" t="n">
+      <c r="L36" s="8" t="n">
         <v>25</v>
       </c>
     </row>
@@ -7514,13 +7514,13 @@
           <t>V1-P2-00&amp;01AB-DUPLEX_2ME_1D.C&amp;2ME_4D.1</t>
         </is>
       </c>
-      <c r="L37" s="9" t="n">
+      <c r="L37" s="8" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="38" ht="4.5" customHeight="1"/>
     <row r="39" ht="18" customHeight="1">
-      <c r="B39" s="19" t="n">
+      <c r="B39" s="21" t="n">
         <v>5</v>
       </c>
       <c r="C39" s="25" t="inlineStr">
@@ -7554,7 +7554,7 @@
           <t>V1-P2.1-01-4MF_1D.A</t>
         </is>
       </c>
-      <c r="L39" s="9" t="n">
+      <c r="L39" s="8" t="n">
         <v>27</v>
       </c>
     </row>
@@ -7590,12 +7590,12 @@
           <t>V1-P2.2-01-4MF_1D.A</t>
         </is>
       </c>
-      <c r="L40" s="9" t="n">
+      <c r="L40" s="8" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="B41" s="19" t="n">
+      <c r="B41" s="21" t="n">
         <v>6</v>
       </c>
       <c r="C41" s="25" t="inlineStr">
@@ -7629,7 +7629,7 @@
           <t>V1-P2.1-01-4MF_1D.B</t>
         </is>
       </c>
-      <c r="L41" s="9" t="n">
+      <c r="L41" s="8" t="n">
         <v>29</v>
       </c>
     </row>
@@ -7665,12 +7665,12 @@
           <t>V1-P2.2-01-4MF_1D.B</t>
         </is>
       </c>
-      <c r="L42" s="9" t="n">
+      <c r="L42" s="8" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="1">
-      <c r="B43" s="19" t="n">
+      <c r="B43" s="21" t="n">
         <v>7</v>
       </c>
       <c r="C43" s="25" t="inlineStr">
@@ -7704,7 +7704,7 @@
           <t>V1-P2.1-01-4MF_1D.C</t>
         </is>
       </c>
-      <c r="L43" s="9" t="n">
+      <c r="L43" s="8" t="n">
         <v>31</v>
       </c>
     </row>
@@ -7740,12 +7740,12 @@
           <t>V1-P2.2-01-4MF_1D.C</t>
         </is>
       </c>
-      <c r="L44" s="9" t="n">
+      <c r="L44" s="8" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="45" ht="18" customHeight="1">
-      <c r="B45" s="19" t="n">
+      <c r="B45" s="21" t="n">
         <v>8</v>
       </c>
       <c r="C45" s="25" t="inlineStr">
@@ -7779,7 +7779,7 @@
           <t>V1-P2.1-01-4MF_1D.D</t>
         </is>
       </c>
-      <c r="L45" s="9" t="n">
+      <c r="L45" s="8" t="n">
         <v>33</v>
       </c>
     </row>
@@ -7815,12 +7815,12 @@
           <t>V1-P2.2-01-4MF_1D.D</t>
         </is>
       </c>
-      <c r="L46" s="9" t="n">
+      <c r="L46" s="8" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="47" ht="18" customHeight="1">
-      <c r="B47" s="19" t="n">
+      <c r="B47" s="21" t="n">
         <v>9</v>
       </c>
       <c r="C47" s="25" t="inlineStr">
@@ -7854,7 +7854,7 @@
           <t>V1-P2.1-01-4MF_1D.E</t>
         </is>
       </c>
-      <c r="L47" s="9" t="n">
+      <c r="L47" s="8" t="n">
         <v>35</v>
       </c>
     </row>
@@ -7890,12 +7890,12 @@
           <t>V1-P2.2-01-4MF_1D.E</t>
         </is>
       </c>
-      <c r="L48" s="9" t="n">
+      <c r="L48" s="8" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="49" ht="18" customHeight="1">
-      <c r="B49" s="19" t="n">
+      <c r="B49" s="21" t="n">
         <v>10</v>
       </c>
       <c r="C49" s="25" t="inlineStr">
@@ -7929,7 +7929,7 @@
           <t>V1-P2.1-01-4MF_1D.MINUS.</t>
         </is>
       </c>
-      <c r="L49" s="9" t="n">
+      <c r="L49" s="8" t="n">
         <v>37</v>
       </c>
     </row>
@@ -7965,12 +7965,12 @@
           <t>V1-P2.2-01-4MF_1D.MINUS.</t>
         </is>
       </c>
-      <c r="L50" s="9" t="n">
+      <c r="L50" s="8" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="51" ht="18" customHeight="1">
-      <c r="B51" s="19" t="n">
+      <c r="B51" s="21" t="n">
         <v>14</v>
       </c>
       <c r="C51" s="25" t="inlineStr">
@@ -8004,7 +8004,7 @@
           <t>V1-P2.1-01-4MF_2D.A</t>
         </is>
       </c>
-      <c r="L51" s="9" t="n">
+      <c r="L51" s="8" t="n">
         <v>39</v>
       </c>
     </row>
@@ -8040,12 +8040,12 @@
           <t>V1-P2.2-01-4MF_2D.A</t>
         </is>
       </c>
-      <c r="L52" s="9" t="n">
+      <c r="L52" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="53" ht="18" customHeight="1">
-      <c r="B53" s="19" t="n">
+      <c r="B53" s="21" t="n">
         <v>15</v>
       </c>
       <c r="C53" s="25" t="inlineStr">
@@ -8079,7 +8079,7 @@
           <t>V1-P2.1-01-4MF_2D.B</t>
         </is>
       </c>
-      <c r="L53" s="9" t="n">
+      <c r="L53" s="8" t="n">
         <v>41</v>
       </c>
     </row>
@@ -8115,12 +8115,12 @@
           <t>V1-P2.2-01-4MF_2D.B</t>
         </is>
       </c>
-      <c r="L54" s="9" t="n">
+      <c r="L54" s="8" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="55" ht="18" customHeight="1">
-      <c r="B55" s="19" t="n">
+      <c r="B55" s="21" t="n">
         <v>16</v>
       </c>
       <c r="C55" s="25" t="inlineStr">
@@ -8154,7 +8154,7 @@
           <t>V1-P2.1-01-4MF_2D.C</t>
         </is>
       </c>
-      <c r="L55" s="9" t="n">
+      <c r="L55" s="8" t="n">
         <v>43</v>
       </c>
     </row>
@@ -8190,12 +8190,12 @@
           <t>V1-P2.2-01-4MF_2D.C</t>
         </is>
       </c>
-      <c r="L56" s="9" t="n">
+      <c r="L56" s="8" t="n">
         <v>44</v>
       </c>
     </row>
     <row r="57" ht="18" customHeight="1">
-      <c r="B57" s="19" t="n">
+      <c r="B57" s="21" t="n">
         <v>17</v>
       </c>
       <c r="C57" s="25" t="inlineStr">
@@ -8229,7 +8229,7 @@
           <t>V1-P2.1-01-4MF_2D.D</t>
         </is>
       </c>
-      <c r="L57" s="9" t="n">
+      <c r="L57" s="8" t="n">
         <v>45</v>
       </c>
     </row>
@@ -8265,7 +8265,7 @@
           <t>V1-P2.2-01-4MF_2D.D</t>
         </is>
       </c>
-      <c r="L58" s="9" t="n">
+      <c r="L58" s="8" t="n">
         <v>46</v>
       </c>
     </row>
@@ -8306,7 +8306,7 @@
           <t>V1-P2-01&amp;02AB-DUPLEX_2MP_1D.B&amp;2MP_3D.2</t>
         </is>
       </c>
-      <c r="L59" s="9" t="n">
+      <c r="L59" s="8" t="n">
         <v>47</v>
       </c>
     </row>
@@ -8347,7 +8347,7 @@
           <t>V1-P2-01&amp;02AB-DUPLEX_2MP_1D.C&amp;2MP_4D.1</t>
         </is>
       </c>
-      <c r="L60" s="9" t="n">
+      <c r="L60" s="8" t="n">
         <v>48</v>
       </c>
     </row>
@@ -8388,7 +8388,7 @@
           <t>V1-P2-01&amp;02AB-DUPLEX_2ME_1D.B&amp;2ME_3D.1</t>
         </is>
       </c>
-      <c r="L61" s="9" t="n">
+      <c r="L61" s="8" t="n">
         <v>49</v>
       </c>
     </row>
@@ -8429,7 +8429,7 @@
           <t>V1-P2-01&amp;02AB-DUPLEX_2ME_1D.C&amp;2ME_4D.1</t>
         </is>
       </c>
-      <c r="L62" s="9" t="n">
+      <c r="L62" s="8" t="n">
         <v>50</v>
       </c>
     </row>
@@ -8440,7 +8440,7 @@
           <t>LOS ÁTICOS  Y LAS VIVIENDAS EN LOS EJES 5-6-7-8-9-10 SE DESCRIBEN EN EL DISEÑO BASE</t>
         </is>
       </c>
-      <c r="K64" s="13" t="n"/>
+      <c r="K64" s="12" t="n"/>
     </row>
     <row r="65" ht="50.1" customHeight="1">
       <c r="L65" s="25" t="n">
@@ -8482,12 +8482,12 @@
           <t>V1-P3-00-LC1C</t>
         </is>
       </c>
-      <c r="L66" s="9" t="n">
+      <c r="L66" s="8" t="n">
         <v>51</v>
       </c>
     </row>
     <row r="67" ht="18" customHeight="1">
-      <c r="B67" s="19" t="n">
+      <c r="B67" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="25" t="inlineStr">
@@ -8521,12 +8521,12 @@
           <t>V1-P3-00-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L67" s="9" t="n">
+      <c r="L67" s="8" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="68" ht="18" customHeight="1">
-      <c r="B68" s="19" t="n">
+      <c r="B68" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C68" s="25" t="inlineStr">
@@ -8560,7 +8560,7 @@
           <t>V1-P3-00-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L68" s="9" t="n">
+      <c r="L68" s="8" t="n">
         <v>53</v>
       </c>
     </row>
@@ -8601,7 +8601,7 @@
           <t>V1-P3-00&amp;01AB-DUPLEX_2MP_1D.B&amp;2MP_3D.2</t>
         </is>
       </c>
-      <c r="L69" s="9" t="n">
+      <c r="L69" s="8" t="n">
         <v>54</v>
       </c>
     </row>
@@ -8642,12 +8642,12 @@
           <t>V1-P3-00&amp;01AB-DUPLEX_2MP_1D.C&amp;2MP_4D.1</t>
         </is>
       </c>
-      <c r="L70" s="9" t="n">
+      <c r="L70" s="8" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="71" ht="18" customHeight="1">
-      <c r="B71" s="19" t="n">
+      <c r="B71" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="25" t="inlineStr">
@@ -8681,7 +8681,7 @@
           <t>V1-P3.1-01-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L71" s="9" t="n">
+      <c r="L71" s="8" t="n">
         <v>56</v>
       </c>
     </row>
@@ -8717,12 +8717,12 @@
           <t>V1-P3.2-01-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L72" s="9" t="n">
+      <c r="L72" s="8" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="73" ht="18" customHeight="1">
-      <c r="B73" s="19" t="n">
+      <c r="B73" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C73" s="25" t="inlineStr">
@@ -8756,7 +8756,7 @@
           <t>V1-P3.1-01-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L73" s="9" t="n">
+      <c r="L73" s="8" t="n">
         <v>58</v>
       </c>
     </row>
@@ -8792,12 +8792,12 @@
           <t>V1-P3.2-01-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L74" s="9" t="n">
+      <c r="L74" s="8" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="75" ht="18" customHeight="1">
-      <c r="B75" s="19" t="n">
+      <c r="B75" s="21" t="n">
         <v>18</v>
       </c>
       <c r="C75" s="25" t="inlineStr">
@@ -8831,12 +8831,12 @@
           <t>V1-P3-02-5MF_2D.A_E</t>
         </is>
       </c>
-      <c r="L75" s="9" t="n">
+      <c r="L75" s="8" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="76" ht="18" customHeight="1">
-      <c r="B76" s="19" t="n">
+      <c r="B76" s="21" t="n">
         <v>19</v>
       </c>
       <c r="C76" s="25" t="inlineStr">
@@ -8870,12 +8870,12 @@
           <t>V1-P3-02-5MF_2D.B_E</t>
         </is>
       </c>
-      <c r="L76" s="9" t="n">
+      <c r="L76" s="8" t="n">
         <v>61</v>
       </c>
     </row>
     <row r="77" ht="18" customHeight="1">
-      <c r="B77" s="19" t="n">
+      <c r="B77" s="21" t="n">
         <v>20</v>
       </c>
       <c r="C77" s="25" t="inlineStr">
@@ -8909,12 +8909,12 @@
           <t>V1-P3-02-5MF_2D.C_E</t>
         </is>
       </c>
-      <c r="L77" s="9" t="n">
+      <c r="L77" s="8" t="n">
         <v>62</v>
       </c>
     </row>
     <row r="78" ht="4.5" customHeight="1">
-      <c r="K78" s="13" t="n"/>
+      <c r="K78" s="12" t="n"/>
     </row>
     <row r="79" ht="25.5" customHeight="1">
       <c r="B79" s="23" t="inlineStr">
@@ -8922,7 +8922,7 @@
           <t>LOS ÁTICOS SE DESCRIBEN EN EL DISEÑO BASE</t>
         </is>
       </c>
-      <c r="K79" s="13" t="n"/>
+      <c r="K79" s="12" t="n"/>
     </row>
     <row r="80" ht="18" customHeight="1"/>
     <row r="81" ht="18" customHeight="1"/>
@@ -8976,7 +8976,7 @@
   </sheetPr>
   <dimension ref="B2:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -8997,13 +8997,13 @@
     <col width="1.5703125" customWidth="1" style="25" min="10" max="10"/>
     <col width="51.7109375" customWidth="1" style="25" min="11" max="11"/>
     <col width="10.7109375" customWidth="1" style="25" min="12" max="12"/>
-    <col width="11.42578125" customWidth="1" style="25" min="13" max="13"/>
-    <col width="11.42578125" customWidth="1" style="25" min="14" max="16384"/>
+    <col width="11.42578125" customWidth="1" style="25" min="13" max="16"/>
+    <col width="11.42578125" customWidth="1" style="25" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="6" customHeight="1"/>
     <row r="2" ht="49.5" customHeight="1">
-      <c r="B2" s="22" t="inlineStr">
+      <c r="B2" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">V     E     R     S     I     Ó      N           2     </t>
         </is>
@@ -9011,48 +9011,48 @@
     </row>
     <row r="3" ht="4.5" customHeight="1"/>
     <row r="4" ht="50.1" customHeight="1">
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nº                                   Plano </t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="9" t="inlineStr">
         <is>
           <t>Estructura</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>Perfil</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="9" t="inlineStr">
         <is>
           <t>Planta</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>Tipología</t>
         </is>
       </c>
-      <c r="G4" s="11" t="n"/>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="G4" s="10" t="n"/>
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Situación </t>
         </is>
       </c>
-      <c r="I4" s="10" t="inlineStr">
+      <c r="I4" s="9" t="inlineStr">
         <is>
           <t>Nº         Dormit.</t>
         </is>
       </c>
-      <c r="K4" s="10" t="inlineStr">
+      <c r="K4" s="9" t="inlineStr">
         <is>
           <t>Nombre del Archivo (.jpg)</t>
         </is>
       </c>
-      <c r="L4" s="12" t="inlineStr">
+      <c r="L4" s="11" t="inlineStr">
         <is>
           <t>orden de Imágenes</t>
         </is>
@@ -9095,7 +9095,7 @@
           <t>V2-P1-00&amp;01A-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L5" s="9" t="n">
+      <c r="L5" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9136,7 +9136,7 @@
           <t>V2-P1-00&amp;01A-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -9177,7 +9177,7 @@
           <t>V2-P1-00&amp;01A-DUPLEX_3MF_1D.B&amp;3MF_3D.2</t>
         </is>
       </c>
-      <c r="L7" s="9" t="n">
+      <c r="L7" s="8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -9218,7 +9218,7 @@
           <t>V2-P1-00&amp;01A-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L8" s="9" t="n">
+      <c r="L8" s="8" t="n">
         <v>4</v>
       </c>
     </row>
@@ -9260,7 +9260,7 @@
           <t>V2-P1-00&amp;01B-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L10" s="9" t="n">
+      <c r="L10" s="8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9301,7 +9301,7 @@
           <t>V2-P1-00&amp;01B-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L11" s="9" t="n">
+      <c r="L11" s="8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -9342,7 +9342,7 @@
           <t>V2-P1-00&amp;01B-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="8" t="n">
         <v>7</v>
       </c>
     </row>
@@ -9384,7 +9384,7 @@
           <t>V2-P1-01&amp;02A-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L14" s="9" t="n">
+      <c r="L14" s="8" t="n">
         <v>8</v>
       </c>
     </row>
@@ -9425,7 +9425,7 @@
           <t>V2-P1-01&amp;02A-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L15" s="9" t="n">
+      <c r="L15" s="8" t="n">
         <v>9</v>
       </c>
     </row>
@@ -9466,7 +9466,7 @@
           <t>V2-P1-01&amp;02A-DUPLEX_3MF_1D.B&amp;3MF_3D.2</t>
         </is>
       </c>
-      <c r="L16" s="9" t="n">
+      <c r="L16" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -9507,12 +9507,12 @@
           <t>V2-P1-01&amp;02A-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L17" s="9" t="n">
+      <c r="L17" s="8" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="18" ht="4.5" customHeight="1">
-      <c r="K18" s="13" t="n"/>
+      <c r="K18" s="12" t="n"/>
     </row>
     <row r="19" ht="20.1" customHeight="1">
       <c r="B19" s="4" t="n">
@@ -9551,7 +9551,7 @@
           <t>V2-P1-01&amp;02B-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L19" s="9" t="n">
+      <c r="L19" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -9592,7 +9592,7 @@
           <t>V2-P1-01&amp;02B-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L20" s="9" t="n">
+      <c r="L20" s="8" t="n">
         <v>13</v>
       </c>
     </row>
@@ -9633,7 +9633,7 @@
           <t>V2-P1-01&amp;02B-DUPLEX_3MF_1D.B&amp;3MF_3D.2</t>
         </is>
       </c>
-      <c r="L21" s="9" t="n">
+      <c r="L21" s="8" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9674,7 +9674,7 @@
           <t>V2-P1-01&amp;02B-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L22" s="9" t="n">
+      <c r="L22" s="8" t="n">
         <v>15</v>
       </c>
     </row>
@@ -9716,7 +9716,7 @@
           <t>V2-P1-02&amp;03A-DUPLEX_3MF_0D.B&amp;3MF_1D.1</t>
         </is>
       </c>
-      <c r="L24" s="9" t="n">
+      <c r="L24" s="8" t="n">
         <v>16</v>
       </c>
     </row>
@@ -9757,7 +9757,7 @@
           <t>V2-P1-02&amp;03A-DUPLEX_3MF_0D.C&amp;3MF_2D.3</t>
         </is>
       </c>
-      <c r="L25" s="9" t="n">
+      <c r="L25" s="8" t="n">
         <v>17</v>
       </c>
     </row>
@@ -9798,7 +9798,7 @@
           <t>V2-P1-02&amp;03A-DUPLEX_3MF_1D.B&amp;3MF_3D.2</t>
         </is>
       </c>
-      <c r="L26" s="9" t="n">
+      <c r="L26" s="8" t="n">
         <v>18</v>
       </c>
     </row>
@@ -9839,12 +9839,12 @@
           <t>V2-P1-02&amp;03A-DUPLEX_3MF_0D.A_DA&amp;3MF_2D.1_DA</t>
         </is>
       </c>
-      <c r="L27" s="9" t="n">
+      <c r="L27" s="8" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="28" ht="4.5" customHeight="1">
-      <c r="K28" s="13" t="n"/>
+      <c r="K28" s="12" t="n"/>
     </row>
     <row r="29" ht="25.5" customHeight="1">
       <c r="B29" s="23" t="inlineStr">
@@ -9857,7 +9857,7 @@
           <t>P1 DE VERSIÓN 1 IGUAL P1 VERSIÓN 2</t>
         </is>
       </c>
-      <c r="K29" s="13" t="n"/>
+      <c r="K29" s="12" t="n"/>
     </row>
     <row r="30" ht="50.1" customHeight="1"/>
     <row r="31" ht="18" customHeight="1">
@@ -9895,12 +9895,12 @@
           <t>V2-P2-00-LC2</t>
         </is>
       </c>
-      <c r="L31" s="9" t="n">
+      <c r="L31" s="8" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="1">
-      <c r="B32" s="19" t="n">
+      <c r="B32" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="25" t="inlineStr">
@@ -9934,12 +9934,12 @@
           <t>V2-P2-00-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L32" s="9" t="n">
+      <c r="L32" s="8" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="1">
-      <c r="B33" s="19" t="n">
+      <c r="B33" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C33" s="25" t="inlineStr">
@@ -9973,7 +9973,7 @@
           <t>V2-P2-00-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L33" s="9" t="n">
+      <c r="L33" s="8" t="n">
         <v>22</v>
       </c>
     </row>
@@ -10014,7 +10014,7 @@
           <t>V2-P2-00&amp;01AB-DUPLEX_2MP_1D.B&amp;2MP_3D.2</t>
         </is>
       </c>
-      <c r="L34" s="9" t="n">
+      <c r="L34" s="8" t="n">
         <v>23</v>
       </c>
     </row>
@@ -10055,7 +10055,7 @@
           <t>V2-P2-00&amp;01AB-DUPLEX_2MP_1D.C&amp;2MP_4D.1</t>
         </is>
       </c>
-      <c r="L35" s="9" t="n">
+      <c r="L35" s="8" t="n">
         <v>24</v>
       </c>
     </row>
@@ -10096,7 +10096,7 @@
           <t>V2-P2-00&amp;01AB-DUPLEX_2ME_1D.B&amp;2ME_3D.1</t>
         </is>
       </c>
-      <c r="L36" s="9" t="n">
+      <c r="L36" s="8" t="n">
         <v>25</v>
       </c>
     </row>
@@ -10137,13 +10137,13 @@
           <t>V2-P2-00&amp;01AB-DUPLEX_2ME_1D.C&amp;2ME_4D.1</t>
         </is>
       </c>
-      <c r="L37" s="9" t="n">
+      <c r="L37" s="8" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="38" ht="4.5" customHeight="1"/>
     <row r="39" ht="18" customHeight="1">
-      <c r="B39" s="14" t="n">
+      <c r="B39" s="13" t="n">
         <v>53</v>
       </c>
       <c r="C39" s="25" t="inlineStr">
@@ -10179,12 +10179,12 @@
           <t>V2-P2.1-01&amp;02A-DUPLEX_4MF_1D.A&amp;3VERSIONES1D</t>
         </is>
       </c>
-      <c r="L39" s="9" t="n">
+      <c r="L39" s="8" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="40" ht="18" customHeight="1">
-      <c r="B40" s="14" t="n">
+      <c r="B40" s="13" t="n">
         <v>53</v>
       </c>
       <c r="C40" s="25" t="inlineStr">
@@ -10220,12 +10220,12 @@
           <t>V2-P2.2-01&amp;02B-DUPLEX_4MF_1D.A&amp;3VERSIONES1D</t>
         </is>
       </c>
-      <c r="L40" s="9" t="n">
+      <c r="L40" s="8" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="B41" s="14" t="n">
+      <c r="B41" s="13" t="n">
         <v>54</v>
       </c>
       <c r="C41" s="25" t="inlineStr">
@@ -10261,12 +10261,12 @@
           <t>V2-P2.1-01&amp;02A-DUPLEX_4MF_1D.B&amp;3VERSIONES1D</t>
         </is>
       </c>
-      <c r="L41" s="9" t="n">
+      <c r="L41" s="8" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="1">
-      <c r="B42" s="14" t="n">
+      <c r="B42" s="13" t="n">
         <v>54</v>
       </c>
       <c r="C42" s="25" t="inlineStr">
@@ -10302,13 +10302,13 @@
           <t>V2-P2.2-01&amp;02B-DUPLEX_4MF_1D.B&amp;3VERSIONES1D</t>
         </is>
       </c>
-      <c r="L42" s="9" t="n">
+      <c r="L42" s="8" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="1"/>
     <row r="44" ht="18" customHeight="1">
-      <c r="B44" s="19" t="n">
+      <c r="B44" s="21" t="n">
         <v>5</v>
       </c>
       <c r="C44" s="25" t="inlineStr">
@@ -10342,7 +10342,7 @@
           <t>V2-P2.1-01-4MF_1D.A</t>
         </is>
       </c>
-      <c r="L44" s="9" t="n">
+      <c r="L44" s="8" t="n">
         <v>31</v>
       </c>
     </row>
@@ -10378,12 +10378,12 @@
           <t>V2-P2.2-01-4MF_1D.A</t>
         </is>
       </c>
-      <c r="L45" s="9" t="n">
+      <c r="L45" s="8" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="46" ht="18" customHeight="1">
-      <c r="B46" s="19" t="n">
+      <c r="B46" s="21" t="n">
         <v>6</v>
       </c>
       <c r="C46" s="25" t="inlineStr">
@@ -10417,7 +10417,7 @@
           <t>V2-P2.1-01-4MF_1D.B</t>
         </is>
       </c>
-      <c r="L46" s="9" t="n">
+      <c r="L46" s="8" t="n">
         <v>33</v>
       </c>
     </row>
@@ -10453,12 +10453,12 @@
           <t>V2-P2.2-01-4MF_1D.B</t>
         </is>
       </c>
-      <c r="L47" s="9" t="n">
+      <c r="L47" s="8" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="48" ht="18" customHeight="1">
-      <c r="B48" s="19" t="n">
+      <c r="B48" s="21" t="n">
         <v>7</v>
       </c>
       <c r="C48" s="25" t="inlineStr">
@@ -10492,7 +10492,7 @@
           <t>V2-P2.1-01-4MF_1D.C</t>
         </is>
       </c>
-      <c r="L48" s="9" t="n">
+      <c r="L48" s="8" t="n">
         <v>35</v>
       </c>
     </row>
@@ -10528,12 +10528,12 @@
           <t>V2-P2.2-01-4MF_1D.C</t>
         </is>
       </c>
-      <c r="L49" s="9" t="n">
+      <c r="L49" s="8" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="50" ht="18" customHeight="1">
-      <c r="B50" s="19" t="n">
+      <c r="B50" s="21" t="n">
         <v>8</v>
       </c>
       <c r="C50" s="25" t="inlineStr">
@@ -10567,7 +10567,7 @@
           <t>V2-P2.1-01-4MF_1D.D</t>
         </is>
       </c>
-      <c r="L50" s="9" t="n">
+      <c r="L50" s="8" t="n">
         <v>37</v>
       </c>
     </row>
@@ -10603,12 +10603,12 @@
           <t>V2-P2.2-01-4MF_1D.D</t>
         </is>
       </c>
-      <c r="L51" s="9" t="n">
+      <c r="L51" s="8" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="52" ht="18" customHeight="1">
-      <c r="B52" s="19" t="n">
+      <c r="B52" s="21" t="n">
         <v>9</v>
       </c>
       <c r="C52" s="25" t="inlineStr">
@@ -10642,7 +10642,7 @@
           <t>V2-P2.1-01-4MF_1D.E</t>
         </is>
       </c>
-      <c r="L52" s="9" t="n">
+      <c r="L52" s="8" t="n">
         <v>39</v>
       </c>
     </row>
@@ -10678,12 +10678,12 @@
           <t>V2-P2.2-01-4MF_1D.E</t>
         </is>
       </c>
-      <c r="L53" s="9" t="n">
+      <c r="L53" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="54" ht="18" customHeight="1">
-      <c r="B54" s="19" t="n">
+      <c r="B54" s="21" t="n">
         <v>10</v>
       </c>
       <c r="C54" s="25" t="inlineStr">
@@ -10717,7 +10717,7 @@
           <t>V2-P2.1-01-4MF_1D.MINUS.</t>
         </is>
       </c>
-      <c r="L54" s="9" t="n">
+      <c r="L54" s="8" t="n">
         <v>41</v>
       </c>
     </row>
@@ -10753,12 +10753,12 @@
           <t>V2-P2.2-01-4MF_1D.MINUS.</t>
         </is>
       </c>
-      <c r="L55" s="9" t="n">
+      <c r="L55" s="8" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="56" ht="18" customHeight="1">
-      <c r="B56" s="19" t="n">
+      <c r="B56" s="21" t="n">
         <v>14</v>
       </c>
       <c r="C56" s="25" t="inlineStr">
@@ -10792,7 +10792,7 @@
           <t>V2-P2.1-01-4MF_2D.A</t>
         </is>
       </c>
-      <c r="L56" s="9" t="n">
+      <c r="L56" s="8" t="n">
         <v>43</v>
       </c>
     </row>
@@ -10828,12 +10828,12 @@
           <t>V2-P2.2-01-4MF_2D.A</t>
         </is>
       </c>
-      <c r="L57" s="9" t="n">
+      <c r="L57" s="8" t="n">
         <v>44</v>
       </c>
     </row>
     <row r="58" ht="18" customHeight="1">
-      <c r="B58" s="19" t="n">
+      <c r="B58" s="21" t="n">
         <v>15</v>
       </c>
       <c r="C58" s="25" t="inlineStr">
@@ -10867,7 +10867,7 @@
           <t>V2-P2.1-01-4MF_2D.B</t>
         </is>
       </c>
-      <c r="L58" s="9" t="n">
+      <c r="L58" s="8" t="n">
         <v>45</v>
       </c>
     </row>
@@ -10903,12 +10903,12 @@
           <t>V2-P2.2-01-4MF_2D.B</t>
         </is>
       </c>
-      <c r="L59" s="9" t="n">
+      <c r="L59" s="8" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="60" ht="18" customHeight="1">
-      <c r="B60" s="19" t="n">
+      <c r="B60" s="21" t="n">
         <v>16</v>
       </c>
       <c r="C60" s="25" t="inlineStr">
@@ -10942,7 +10942,7 @@
           <t>V2-P2.1-01-4MF_2D.C</t>
         </is>
       </c>
-      <c r="L60" s="9" t="n">
+      <c r="L60" s="8" t="n">
         <v>47</v>
       </c>
     </row>
@@ -10978,12 +10978,12 @@
           <t>V2-P2.2-01-4MF_2D.C</t>
         </is>
       </c>
-      <c r="L61" s="9" t="n">
+      <c r="L61" s="8" t="n">
         <v>48</v>
       </c>
     </row>
     <row r="62" ht="18" customHeight="1">
-      <c r="B62" s="19" t="n">
+      <c r="B62" s="21" t="n">
         <v>17</v>
       </c>
       <c r="C62" s="25" t="inlineStr">
@@ -11017,7 +11017,7 @@
           <t>V2-P2.1-01-4MF_2D.D</t>
         </is>
       </c>
-      <c r="L62" s="9" t="n">
+      <c r="L62" s="8" t="n">
         <v>49</v>
       </c>
     </row>
@@ -11053,7 +11053,7 @@
           <t>V2-P2.2-01-4MF_2D.D</t>
         </is>
       </c>
-      <c r="L63" s="9" t="n">
+      <c r="L63" s="8" t="n">
         <v>50</v>
       </c>
     </row>
@@ -11094,7 +11094,7 @@
           <t>V2-P2-01&amp;02AB-DUPLEX_2ME_1D.B&amp;2ME_3D.1</t>
         </is>
       </c>
-      <c r="L64" s="9" t="n">
+      <c r="L64" s="8" t="n">
         <v>51</v>
       </c>
     </row>
@@ -11135,7 +11135,7 @@
           <t>V2-P2-01&amp;02AB-DUPLEX_2ME_1D.C&amp;2ME_4D.1</t>
         </is>
       </c>
-      <c r="L65" s="9" t="n">
+      <c r="L65" s="8" t="n">
         <v>52</v>
       </c>
     </row>
@@ -11146,7 +11146,7 @@
           <t>LOS ÁTICOS  Y LAS VIVIENDAS EN LOS EJES 5-6-7-8-9-10 SE DESCRIBEN EN EL DISEÑO BASE</t>
         </is>
       </c>
-      <c r="K67" s="13" t="n"/>
+      <c r="K67" s="12" t="n"/>
     </row>
     <row r="68" ht="50.1" customHeight="1"/>
     <row r="69" ht="18" customHeight="1">
@@ -11184,12 +11184,12 @@
           <t>V2-P3-00-LC2</t>
         </is>
       </c>
-      <c r="L69" s="9" t="n">
+      <c r="L69" s="8" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="70" ht="18" customHeight="1">
-      <c r="B70" s="19" t="n">
+      <c r="B70" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C70" s="25" t="inlineStr">
@@ -11223,12 +11223,12 @@
           <t>V2-P3-00-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L70" s="9" t="n">
+      <c r="L70" s="8" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="71" ht="18" customHeight="1">
-      <c r="B71" s="19" t="n">
+      <c r="B71" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C71" s="25" t="inlineStr">
@@ -11262,7 +11262,7 @@
           <t>V2-P3-00-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L71" s="9" t="n">
+      <c r="L71" s="8" t="n">
         <v>55</v>
       </c>
     </row>
@@ -11303,7 +11303,7 @@
           <t>V2-P3-00&amp;01AB-DUPLEX_2MP_1D.B&amp;2MP_3D.2</t>
         </is>
       </c>
-      <c r="L72" s="9" t="n">
+      <c r="L72" s="8" t="n">
         <v>56</v>
       </c>
     </row>
@@ -11344,12 +11344,12 @@
           <t>V2-P3-00&amp;01AB-DUPLEX_2MP_1D.C&amp;2MP_4D.1</t>
         </is>
       </c>
-      <c r="L73" s="9" t="n">
+      <c r="L73" s="8" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="74" ht="18" customHeight="1">
-      <c r="B74" s="19" t="n">
+      <c r="B74" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C74" s="25" t="inlineStr">
@@ -11383,7 +11383,7 @@
           <t>V2-P3.1-01-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L74" s="9" t="n">
+      <c r="L74" s="8" t="n">
         <v>58</v>
       </c>
     </row>
@@ -11419,12 +11419,12 @@
           <t>V2-P3.2-01-3MF_1D.A</t>
         </is>
       </c>
-      <c r="L75" s="9" t="n">
+      <c r="L75" s="8" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="76" ht="18" customHeight="1">
-      <c r="B76" s="19" t="n">
+      <c r="B76" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C76" s="25" t="inlineStr">
@@ -11458,7 +11458,7 @@
           <t>V2-P3.1-01-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L76" s="9" t="n">
+      <c r="L76" s="8" t="n">
         <v>60</v>
       </c>
     </row>
@@ -11494,12 +11494,12 @@
           <t>V2-P3.2-01-3MF_1D.B</t>
         </is>
       </c>
-      <c r="L77" s="9" t="n">
+      <c r="L77" s="8" t="n">
         <v>61</v>
       </c>
     </row>
     <row r="78" ht="18" customHeight="1">
-      <c r="B78" s="19" t="n">
+      <c r="B78" s="21" t="n">
         <v>18</v>
       </c>
       <c r="C78" s="25" t="inlineStr">
@@ -11533,12 +11533,12 @@
           <t>V2-P3-02-5MF_2D.A_E</t>
         </is>
       </c>
-      <c r="L78" s="9" t="n">
+      <c r="L78" s="8" t="n">
         <v>62</v>
       </c>
     </row>
     <row r="79" ht="18" customHeight="1">
-      <c r="B79" s="19" t="n">
+      <c r="B79" s="21" t="n">
         <v>19</v>
       </c>
       <c r="C79" s="25" t="inlineStr">
@@ -11572,12 +11572,12 @@
           <t>V2-P3-02-5MF_2D.B_E</t>
         </is>
       </c>
-      <c r="L79" s="9" t="n">
+      <c r="L79" s="8" t="n">
         <v>63</v>
       </c>
     </row>
     <row r="80" ht="18" customHeight="1">
-      <c r="B80" s="19" t="n">
+      <c r="B80" s="21" t="n">
         <v>20</v>
       </c>
       <c r="C80" s="25" t="inlineStr">
@@ -11611,12 +11611,12 @@
           <t>V2-P3-02-5MF_2D.C_E</t>
         </is>
       </c>
-      <c r="L80" s="9" t="n">
+      <c r="L80" s="8" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="81" ht="4.5" customHeight="1">
-      <c r="K81" s="13" t="n"/>
+      <c r="K81" s="12" t="n"/>
     </row>
     <row r="82" ht="25.5" customHeight="1">
       <c r="B82" s="23" t="inlineStr">
@@ -11629,7 +11629,7 @@
           <t>P3 DE VERSIÓN 1 IGUAL P3 VERSIÓN 2</t>
         </is>
       </c>
-      <c r="K82" s="13" t="n"/>
+      <c r="K82" s="12" t="n"/>
     </row>
     <row r="83" ht="18" customHeight="1"/>
     <row r="84" ht="18" customHeight="1"/>
@@ -11653,17 +11653,6 @@
     <row r="102" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B67:H67"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B50:B51"/>
@@ -11671,6 +11660,17 @@
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B74:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
coord algorith implemented succesfully
</commit_message>
<xml_diff>
--- a/FreeWork/ADECUA/AppFinalQt/database.xlsx
+++ b/FreeWork/ADECUA/AppFinalQt/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="V1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="V2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DB" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="V1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="V2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -244,9 +244,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -256,16 +253,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -610,16 +610,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="FF92D050"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="B2:M159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="D143" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K152" sqref="K152"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -631,19 +632,19 @@
     <col width="11.7109375" customWidth="1" style="25" min="5" max="5"/>
     <col width="32.28515625" customWidth="1" style="25" min="6" max="6"/>
     <col width="1.85546875" customWidth="1" style="25" min="7" max="7"/>
-    <col width="30.85546875" customWidth="1" style="25" min="8" max="8"/>
+    <col width="53" customWidth="1" style="25" min="8" max="8"/>
     <col width="11.42578125" customWidth="1" style="25" min="9" max="9"/>
     <col width="4.42578125" customWidth="1" style="25" min="10" max="10"/>
     <col width="52" customWidth="1" style="25" min="11" max="11"/>
     <col width="22.5703125" customWidth="1" style="25" min="12" max="12"/>
     <col width="20.42578125" customWidth="1" style="25" min="13" max="13"/>
-    <col width="11.42578125" customWidth="1" style="25" min="14" max="17"/>
-    <col width="11.42578125" customWidth="1" style="25" min="18" max="16384"/>
+    <col width="11.42578125" customWidth="1" style="25" min="14" max="26"/>
+    <col width="11.42578125" customWidth="1" style="25" min="27" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="6" customHeight="1"/>
     <row r="2" ht="49.5" customHeight="1">
-      <c r="B2" s="19" t="inlineStr">
+      <c r="B2" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">D     I     S     E     Ñ     O           B     A     S     E </t>
         </is>
@@ -720,7 +721,7 @@
       </c>
       <c r="H5" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A</t>
+          <t>0001A0/0002A0/0003A0</t>
         </is>
       </c>
       <c r="I5" s="25" t="inlineStr">
@@ -728,7 +729,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K5" s="15" t="inlineStr">
+      <c r="K5" s="25" t="inlineStr">
         <is>
           <t>DB-P1-00-LC1A</t>
         </is>
@@ -738,7 +739,7 @@
       </c>
     </row>
     <row r="6" ht="18" customHeight="1">
-      <c r="B6" s="21" t="n">
+      <c r="B6" s="19" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="25" t="inlineStr">
@@ -761,13 +762,13 @@
       </c>
       <c r="H6" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-B</t>
+          <t>00010B/00020B/00030B</t>
         </is>
       </c>
       <c r="I6" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="26" t="inlineStr">
+      <c r="K6" s="25" t="inlineStr">
         <is>
           <t>DB-P1-00-3MF_1D.A_E</t>
         </is>
@@ -777,7 +778,7 @@
       </c>
     </row>
     <row r="7" ht="18" customHeight="1">
-      <c r="B7" s="21" t="n">
+      <c r="B7" s="19" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="25" t="inlineStr">
@@ -800,13 +801,13 @@
       </c>
       <c r="H7" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-B</t>
+          <t>00010B/00020B/00030B</t>
         </is>
       </c>
       <c r="I7" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="15" t="inlineStr">
+      <c r="K7" s="25" t="inlineStr">
         <is>
           <t>DB-P1-00-3MF_1D.B_E</t>
         </is>
@@ -840,13 +841,13 @@
       </c>
       <c r="H9" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-AB</t>
+          <t>0101AB/0102AB/0103AB</t>
         </is>
       </c>
       <c r="I9" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="K9" s="25" t="inlineStr">
+      <c r="K9" s="18" t="inlineStr">
         <is>
           <t>DB-P1-01-3MP_2D.A</t>
         </is>
@@ -879,13 +880,13 @@
       </c>
       <c r="H10" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-AB</t>
+          <t>0101AB/0102AB/0103AB</t>
         </is>
       </c>
       <c r="I10" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="K10" s="25" t="inlineStr">
+      <c r="K10" s="18" t="inlineStr">
         <is>
           <t>DB-P1-01-3MP_3D.A</t>
         </is>
@@ -918,13 +919,13 @@
       </c>
       <c r="H11" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-AB</t>
+          <t>0101AB/0102AB/0103AB</t>
         </is>
       </c>
       <c r="I11" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="K11" s="25" t="inlineStr">
+      <c r="K11" s="18" t="inlineStr">
         <is>
           <t>DB-P1-01-3MP_3D.B</t>
         </is>
@@ -957,13 +958,13 @@
       </c>
       <c r="H12" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-AB</t>
+          <t>0101AB/0102AB/0103AB</t>
         </is>
       </c>
       <c r="I12" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="K12" s="25" t="inlineStr">
+      <c r="K12" s="18" t="inlineStr">
         <is>
           <t>DB-P1-01-3MP_3D.C</t>
         </is>
@@ -996,13 +997,13 @@
       </c>
       <c r="H13" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-AB</t>
+          <t>0101AB/0102AB/0103AB</t>
         </is>
       </c>
       <c r="I13" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="K13" s="25" t="inlineStr">
+      <c r="K13" s="18" t="inlineStr">
         <is>
           <t>DB-P1-01-3MP_3D.D</t>
         </is>
@@ -1035,13 +1036,13 @@
       </c>
       <c r="H14" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-AB</t>
+          <t>0101AB/0102AB/0103AB</t>
         </is>
       </c>
       <c r="I14" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="K14" s="25" t="inlineStr">
+      <c r="K14" s="18" t="inlineStr">
         <is>
           <t>DB-P1-01-3MP_4D.A</t>
         </is>
@@ -1074,13 +1075,13 @@
       </c>
       <c r="H15" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-AB</t>
+          <t>0101AB/0102AB/0103AB</t>
         </is>
       </c>
       <c r="I15" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="K15" s="25" t="inlineStr">
+      <c r="K15" s="18" t="inlineStr">
         <is>
           <t>DB-P1-01-3MP_4D.B</t>
         </is>
@@ -1114,13 +1115,13 @@
       </c>
       <c r="H17" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-AB</t>
+          <t>0201AB/0202AB/0203AB</t>
         </is>
       </c>
       <c r="I17" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="K17" s="15" t="inlineStr">
+      <c r="K17" s="25" t="inlineStr">
         <is>
           <t>DB-P1-02-3MP_2D.A</t>
         </is>
@@ -1153,7 +1154,7 @@
       </c>
       <c r="H18" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-AB</t>
+          <t>0201AB/0202AB/0203AB</t>
         </is>
       </c>
       <c r="I18" s="25" t="n">
@@ -1192,7 +1193,7 @@
       </c>
       <c r="H19" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-AB</t>
+          <t>0201AB/0202AB/0203AB</t>
         </is>
       </c>
       <c r="I19" s="25" t="n">
@@ -1231,7 +1232,7 @@
       </c>
       <c r="H20" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-AB</t>
+          <t>0201AB/0202AB/0203AB</t>
         </is>
       </c>
       <c r="I20" s="25" t="n">
@@ -1270,7 +1271,7 @@
       </c>
       <c r="H21" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-AB</t>
+          <t>0201AB/0202AB/0203AB</t>
         </is>
       </c>
       <c r="I21" s="25" t="n">
@@ -1309,7 +1310,7 @@
       </c>
       <c r="H22" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-AB</t>
+          <t>0201AB/0202AB/0203AB</t>
         </is>
       </c>
       <c r="I22" s="25" t="n">
@@ -1348,7 +1349,7 @@
       </c>
       <c r="H23" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-AB</t>
+          <t>0201AB/0202AB/0203AB</t>
         </is>
       </c>
       <c r="I23" s="25" t="n">
@@ -1365,7 +1366,7 @@
     </row>
     <row r="24" ht="3" customHeight="1"/>
     <row r="25" ht="18" customHeight="1">
-      <c r="B25" s="21" t="n">
+      <c r="B25" s="19" t="n">
         <v>3</v>
       </c>
       <c r="C25" s="25" t="inlineStr">
@@ -1388,7 +1389,7 @@
       </c>
       <c r="H25" s="25" t="inlineStr">
         <is>
-          <t>03-1-2-3-A</t>
+          <t>0301A0/0302A0/0303A0</t>
         </is>
       </c>
       <c r="I25" s="25" t="n">
@@ -1404,7 +1405,7 @@
       </c>
     </row>
     <row r="26" ht="18" customHeight="1">
-      <c r="B26" s="21" t="n">
+      <c r="B26" s="19" t="n">
         <v>4</v>
       </c>
       <c r="C26" s="25" t="inlineStr">
@@ -1427,7 +1428,7 @@
       </c>
       <c r="H26" s="25" t="inlineStr">
         <is>
-          <t>03-1-2-3-A</t>
+          <t>0301A0/0302A0/0303A0</t>
         </is>
       </c>
       <c r="I26" s="25" t="n">
@@ -1443,7 +1444,7 @@
       </c>
     </row>
     <row r="27" ht="18" customHeight="1">
-      <c r="B27" s="22" t="n">
+      <c r="B27" s="21" t="n">
         <v>61</v>
       </c>
       <c r="C27" s="25" t="inlineStr">
@@ -1468,7 +1469,7 @@
       </c>
       <c r="H27" s="25" t="inlineStr">
         <is>
-          <t>03-1-2-3-B&amp;04-1-2-3 AB</t>
+          <t>03010B/03020B/03030B_0401AB/0402AB/0403AB</t>
         </is>
       </c>
       <c r="I27" s="25" t="n">
@@ -1484,7 +1485,7 @@
       </c>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="B28" s="22" t="n">
+      <c r="B28" s="21" t="n">
         <v>62</v>
       </c>
       <c r="C28" s="25" t="inlineStr">
@@ -1509,7 +1510,7 @@
       </c>
       <c r="H28" s="25" t="inlineStr">
         <is>
-          <t>03-1-2-3-B&amp;04-1-2-3 AB</t>
+          <t>03010B/03020B/03030B_0401AB/0402AB/0403AB</t>
         </is>
       </c>
       <c r="I28" s="25" t="n">
@@ -1525,7 +1526,7 @@
       </c>
     </row>
     <row r="29" ht="18" customHeight="1">
-      <c r="B29" s="22" t="n">
+      <c r="B29" s="21" t="n">
         <v>63</v>
       </c>
       <c r="C29" s="25" t="inlineStr">
@@ -1550,7 +1551,7 @@
       </c>
       <c r="H29" s="25" t="inlineStr">
         <is>
-          <t>03-1-2-3-B&amp;04-1-2-3 AB</t>
+          <t>03010B/03020B/03030B_0401AB/0402AB/0403AB</t>
         </is>
       </c>
       <c r="I29" s="25" t="n">
@@ -1566,7 +1567,7 @@
       </c>
     </row>
     <row r="30" ht="18" customHeight="1">
-      <c r="B30" s="22" t="n">
+      <c r="B30" s="21" t="n">
         <v>64</v>
       </c>
       <c r="C30" s="25" t="inlineStr">
@@ -1591,7 +1592,7 @@
       </c>
       <c r="H30" s="25" t="inlineStr">
         <is>
-          <t>03-1-2-3-B&amp;04-1-2-3 AB</t>
+          <t>03010B/03020B/03030B_0401AB/0402AB/0403AB</t>
         </is>
       </c>
       <c r="I30" s="25" t="n">
@@ -1629,7 +1630,7 @@
       </c>
       <c r="H32" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-A</t>
+          <t>0006A0/0007A0/0008A0</t>
         </is>
       </c>
       <c r="I32" s="25" t="inlineStr">
@@ -1647,7 +1648,7 @@
       </c>
     </row>
     <row r="33" ht="18" customHeight="1">
-      <c r="B33" s="21" t="n">
+      <c r="B33" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="25" t="inlineStr">
@@ -1670,13 +1671,13 @@
       </c>
       <c r="H33" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-B</t>
+          <t>00060B/00070B/00080B</t>
         </is>
       </c>
       <c r="I33" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K33" s="15" t="inlineStr">
+      <c r="K33" s="25" t="inlineStr">
         <is>
           <t>DB-P2-00-3MF_1D.A</t>
         </is>
@@ -1686,7 +1687,7 @@
       </c>
     </row>
     <row r="34" ht="18" customHeight="1">
-      <c r="B34" s="21" t="n">
+      <c r="B34" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C34" s="25" t="inlineStr">
@@ -1709,7 +1710,7 @@
       </c>
       <c r="H34" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-B</t>
+          <t>00060B/00070B/00080B</t>
         </is>
       </c>
       <c r="I34" s="25" t="n">
@@ -1748,7 +1749,7 @@
       </c>
       <c r="H35" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB</t>
+          <t>0009AB/0010AB</t>
         </is>
       </c>
       <c r="I35" s="25" t="n">
@@ -1787,7 +1788,7 @@
       </c>
       <c r="H36" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB</t>
+          <t>0009AB/0010AB</t>
         </is>
       </c>
       <c r="I36" s="25" t="n">
@@ -1826,7 +1827,7 @@
       </c>
       <c r="H37" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB</t>
+          <t>0009AB/0010AB</t>
         </is>
       </c>
       <c r="I37" s="25" t="n">
@@ -1865,7 +1866,7 @@
       </c>
       <c r="H38" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB</t>
+          <t>0009AB/0010AB</t>
         </is>
       </c>
       <c r="I38" s="25" t="n">
@@ -1904,7 +1905,7 @@
       </c>
       <c r="H39" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB</t>
+          <t>0009AB/0010AB</t>
         </is>
       </c>
       <c r="I39" s="25" t="n">
@@ -1943,7 +1944,7 @@
       </c>
       <c r="H40" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB</t>
+          <t>0009AB/0010AB</t>
         </is>
       </c>
       <c r="I40" s="25" t="n">
@@ -1982,7 +1983,7 @@
       </c>
       <c r="H41" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB</t>
+          <t>0009AB/0010AB</t>
         </is>
       </c>
       <c r="I41" s="25" t="n">
@@ -2021,7 +2022,7 @@
       </c>
       <c r="H42" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB</t>
+          <t>0011AB/0012AB</t>
         </is>
       </c>
       <c r="I42" s="25" t="n">
@@ -2060,7 +2061,7 @@
       </c>
       <c r="H43" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB</t>
+          <t>0011AB/0012AB</t>
         </is>
       </c>
       <c r="I43" s="25" t="n">
@@ -2099,7 +2100,7 @@
       </c>
       <c r="H44" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB</t>
+          <t>0011AB/0012AB</t>
         </is>
       </c>
       <c r="I44" s="25" t="n">
@@ -2138,7 +2139,7 @@
       </c>
       <c r="H45" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB</t>
+          <t>0011AB/0012AB</t>
         </is>
       </c>
       <c r="I45" s="25" t="n">
@@ -2177,7 +2178,7 @@
       </c>
       <c r="H46" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB</t>
+          <t>0011AB/0012AB</t>
         </is>
       </c>
       <c r="I46" s="25" t="n">
@@ -2194,7 +2195,7 @@
     </row>
     <row r="47" ht="11.25" customHeight="1"/>
     <row r="48" ht="18" customHeight="1">
-      <c r="B48" s="21" t="n">
+      <c r="B48" s="19" t="n">
         <v>5</v>
       </c>
       <c r="C48" s="25" t="inlineStr">
@@ -2217,7 +2218,7 @@
       </c>
       <c r="H48" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I48" s="25" t="n">
@@ -2253,7 +2254,7 @@
       </c>
       <c r="H49" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I49" s="25" t="n">
@@ -2269,7 +2270,7 @@
       </c>
     </row>
     <row r="50" ht="18" customHeight="1">
-      <c r="B50" s="21" t="n">
+      <c r="B50" s="19" t="n">
         <v>6</v>
       </c>
       <c r="C50" s="25" t="inlineStr">
@@ -2292,7 +2293,7 @@
       </c>
       <c r="H50" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I50" s="25" t="n">
@@ -2328,7 +2329,7 @@
       </c>
       <c r="H51" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I51" s="25" t="n">
@@ -2344,7 +2345,7 @@
       </c>
     </row>
     <row r="52" ht="18" customHeight="1">
-      <c r="B52" s="21" t="n">
+      <c r="B52" s="19" t="n">
         <v>7</v>
       </c>
       <c r="C52" s="25" t="inlineStr">
@@ -2367,7 +2368,7 @@
       </c>
       <c r="H52" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I52" s="25" t="n">
@@ -2403,7 +2404,7 @@
       </c>
       <c r="H53" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I53" s="25" t="n">
@@ -2419,7 +2420,7 @@
       </c>
     </row>
     <row r="54" ht="18" customHeight="1">
-      <c r="B54" s="21" t="n">
+      <c r="B54" s="19" t="n">
         <v>8</v>
       </c>
       <c r="C54" s="25" t="inlineStr">
@@ -2442,7 +2443,7 @@
       </c>
       <c r="H54" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I54" s="25" t="n">
@@ -2478,7 +2479,7 @@
       </c>
       <c r="H55" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I55" s="25" t="n">
@@ -2494,7 +2495,7 @@
       </c>
     </row>
     <row r="56" ht="18" customHeight="1">
-      <c r="B56" s="21" t="n">
+      <c r="B56" s="19" t="n">
         <v>9</v>
       </c>
       <c r="C56" s="25" t="inlineStr">
@@ -2517,7 +2518,7 @@
       </c>
       <c r="H56" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I56" s="25" t="n">
@@ -2553,7 +2554,7 @@
       </c>
       <c r="H57" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I57" s="25" t="n">
@@ -2569,7 +2570,7 @@
       </c>
     </row>
     <row r="58" ht="18" customHeight="1">
-      <c r="B58" s="21" t="n">
+      <c r="B58" s="19" t="n">
         <v>10</v>
       </c>
       <c r="C58" s="25" t="inlineStr">
@@ -2592,7 +2593,7 @@
       </c>
       <c r="H58" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I58" s="25" t="n">
@@ -2628,7 +2629,7 @@
       </c>
       <c r="H59" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I59" s="25" t="n">
@@ -2644,7 +2645,7 @@
       </c>
     </row>
     <row r="60" ht="18" customHeight="1">
-      <c r="B60" s="21" t="n">
+      <c r="B60" s="19" t="n">
         <v>14</v>
       </c>
       <c r="C60" s="25" t="inlineStr">
@@ -2667,7 +2668,7 @@
       </c>
       <c r="H60" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I60" s="25" t="n">
@@ -2703,7 +2704,7 @@
       </c>
       <c r="H61" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I61" s="25" t="n">
@@ -2719,7 +2720,7 @@
       </c>
     </row>
     <row r="62" ht="18" customHeight="1">
-      <c r="B62" s="21" t="n">
+      <c r="B62" s="19" t="n">
         <v>15</v>
       </c>
       <c r="C62" s="25" t="inlineStr">
@@ -2742,7 +2743,7 @@
       </c>
       <c r="H62" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I62" s="25" t="n">
@@ -2778,7 +2779,7 @@
       </c>
       <c r="H63" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I63" s="25" t="n">
@@ -2794,7 +2795,7 @@
       </c>
     </row>
     <row r="64" ht="18" customHeight="1">
-      <c r="B64" s="21" t="n">
+      <c r="B64" s="19" t="n">
         <v>16</v>
       </c>
       <c r="C64" s="25" t="inlineStr">
@@ -2817,7 +2818,7 @@
       </c>
       <c r="H64" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I64" s="25" t="n">
@@ -2853,7 +2854,7 @@
       </c>
       <c r="H65" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I65" s="25" t="n">
@@ -2869,7 +2870,7 @@
       </c>
     </row>
     <row r="66" ht="18" customHeight="1">
-      <c r="B66" s="21" t="n">
+      <c r="B66" s="19" t="n">
         <v>17</v>
       </c>
       <c r="C66" s="25" t="inlineStr">
@@ -2892,7 +2893,7 @@
       </c>
       <c r="H66" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I66" s="25" t="n">
@@ -2928,7 +2929,7 @@
       </c>
       <c r="H67" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I67" s="25" t="n">
@@ -2967,7 +2968,7 @@
       </c>
       <c r="H68" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB</t>
+          <t>0109AB/0110AB</t>
         </is>
       </c>
       <c r="I68" s="25" t="n">
@@ -3006,7 +3007,7 @@
       </c>
       <c r="H69" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB</t>
+          <t>0109AB/0110AB</t>
         </is>
       </c>
       <c r="I69" s="25" t="n">
@@ -3045,7 +3046,7 @@
       </c>
       <c r="H70" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB</t>
+          <t>0109AB/0110AB</t>
         </is>
       </c>
       <c r="I70" s="25" t="n">
@@ -3084,7 +3085,7 @@
       </c>
       <c r="H71" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB</t>
+          <t>0109AB/0110AB</t>
         </is>
       </c>
       <c r="I71" s="25" t="n">
@@ -3123,7 +3124,7 @@
       </c>
       <c r="H72" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB</t>
+          <t>0109AB/0110AB</t>
         </is>
       </c>
       <c r="I72" s="25" t="n">
@@ -3162,7 +3163,7 @@
       </c>
       <c r="H73" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB</t>
+          <t>0109AB/0110AB</t>
         </is>
       </c>
       <c r="I73" s="25" t="n">
@@ -3201,7 +3202,7 @@
       </c>
       <c r="H74" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB</t>
+          <t>0109AB/0110AB</t>
         </is>
       </c>
       <c r="I74" s="25" t="n">
@@ -3240,7 +3241,7 @@
       </c>
       <c r="H75" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB</t>
+          <t>0111AB/0112AB</t>
         </is>
       </c>
       <c r="I75" s="25" t="n">
@@ -3279,7 +3280,7 @@
       </c>
       <c r="H76" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB</t>
+          <t>0111AB/0112AB</t>
         </is>
       </c>
       <c r="I76" s="25" t="n">
@@ -3318,7 +3319,7 @@
       </c>
       <c r="H77" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB</t>
+          <t>0111AB/0112AB</t>
         </is>
       </c>
       <c r="I77" s="25" t="n">
@@ -3357,7 +3358,7 @@
       </c>
       <c r="H78" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB</t>
+          <t>0111AB/0112AB</t>
         </is>
       </c>
       <c r="I78" s="25" t="n">
@@ -3396,7 +3397,7 @@
       </c>
       <c r="H79" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB</t>
+          <t>0111AB/0112AB</t>
         </is>
       </c>
       <c r="I79" s="25" t="n">
@@ -3413,7 +3414,7 @@
     </row>
     <row r="80" ht="3" customHeight="1"/>
     <row r="81" ht="18" customHeight="1">
-      <c r="B81" s="21" t="n">
+      <c r="B81" s="19" t="n">
         <v>5</v>
       </c>
       <c r="C81" s="25" t="inlineStr">
@@ -3436,7 +3437,7 @@
       </c>
       <c r="H81" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I81" s="25" t="n">
@@ -3472,7 +3473,7 @@
       </c>
       <c r="H82" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I82" s="25" t="n">
@@ -3488,7 +3489,7 @@
       </c>
     </row>
     <row r="83" ht="18" customHeight="1">
-      <c r="B83" s="21" t="n">
+      <c r="B83" s="19" t="n">
         <v>6</v>
       </c>
       <c r="C83" s="25" t="inlineStr">
@@ -3511,7 +3512,7 @@
       </c>
       <c r="H83" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I83" s="25" t="n">
@@ -3547,7 +3548,7 @@
       </c>
       <c r="H84" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I84" s="25" t="n">
@@ -3563,7 +3564,7 @@
       </c>
     </row>
     <row r="85" ht="18" customHeight="1">
-      <c r="B85" s="21" t="n">
+      <c r="B85" s="19" t="n">
         <v>7</v>
       </c>
       <c r="C85" s="25" t="inlineStr">
@@ -3586,7 +3587,7 @@
       </c>
       <c r="H85" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I85" s="25" t="n">
@@ -3622,7 +3623,7 @@
       </c>
       <c r="H86" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I86" s="25" t="n">
@@ -3638,7 +3639,7 @@
       </c>
     </row>
     <row r="87" ht="18" customHeight="1">
-      <c r="B87" s="21" t="n">
+      <c r="B87" s="19" t="n">
         <v>8</v>
       </c>
       <c r="C87" s="25" t="inlineStr">
@@ -3661,7 +3662,7 @@
       </c>
       <c r="H87" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I87" s="25" t="n">
@@ -3697,7 +3698,7 @@
       </c>
       <c r="H88" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I88" s="25" t="n">
@@ -3713,7 +3714,7 @@
       </c>
     </row>
     <row r="89" ht="18" customHeight="1">
-      <c r="B89" s="21" t="n">
+      <c r="B89" s="19" t="n">
         <v>9</v>
       </c>
       <c r="C89" s="25" t="inlineStr">
@@ -3736,7 +3737,7 @@
       </c>
       <c r="H89" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I89" s="25" t="n">
@@ -3772,7 +3773,7 @@
       </c>
       <c r="H90" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I90" s="25" t="n">
@@ -3788,7 +3789,7 @@
       </c>
     </row>
     <row r="91" ht="18" customHeight="1">
-      <c r="B91" s="21" t="n">
+      <c r="B91" s="19" t="n">
         <v>10</v>
       </c>
       <c r="C91" s="25" t="inlineStr">
@@ -3811,7 +3812,7 @@
       </c>
       <c r="H91" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I91" s="25" t="n">
@@ -3847,7 +3848,7 @@
       </c>
       <c r="H92" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I92" s="25" t="n">
@@ -3863,7 +3864,7 @@
       </c>
     </row>
     <row r="93" ht="18" customHeight="1">
-      <c r="B93" s="21" t="n">
+      <c r="B93" s="19" t="n">
         <v>14</v>
       </c>
       <c r="C93" s="25" t="inlineStr">
@@ -3886,7 +3887,7 @@
       </c>
       <c r="H93" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I93" s="25" t="n">
@@ -3922,7 +3923,7 @@
       </c>
       <c r="H94" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I94" s="25" t="n">
@@ -3938,7 +3939,7 @@
       </c>
     </row>
     <row r="95" ht="18" customHeight="1">
-      <c r="B95" s="21" t="n">
+      <c r="B95" s="19" t="n">
         <v>15</v>
       </c>
       <c r="C95" s="25" t="inlineStr">
@@ -3961,7 +3962,7 @@
       </c>
       <c r="H95" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I95" s="25" t="n">
@@ -3997,7 +3998,7 @@
       </c>
       <c r="H96" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I96" s="25" t="n">
@@ -4013,7 +4014,7 @@
       </c>
     </row>
     <row r="97" ht="18" customHeight="1">
-      <c r="B97" s="21" t="n">
+      <c r="B97" s="19" t="n">
         <v>16</v>
       </c>
       <c r="C97" s="25" t="inlineStr">
@@ -4036,7 +4037,7 @@
       </c>
       <c r="H97" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I97" s="25" t="n">
@@ -4072,7 +4073,7 @@
       </c>
       <c r="H98" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I98" s="25" t="n">
@@ -4088,7 +4089,7 @@
       </c>
     </row>
     <row r="99" ht="18" customHeight="1">
-      <c r="B99" s="21" t="n">
+      <c r="B99" s="19" t="n">
         <v>17</v>
       </c>
       <c r="C99" s="25" t="inlineStr">
@@ -4111,7 +4112,7 @@
       </c>
       <c r="H99" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-A</t>
+          <t>0205A0/0206A0/0207A0/0208A0</t>
         </is>
       </c>
       <c r="I99" s="25" t="n">
@@ -4147,7 +4148,7 @@
       </c>
       <c r="H100" s="25" t="inlineStr">
         <is>
-          <t>02-5-6-7-8-B</t>
+          <t>02050B/02060B/02070B/02080B</t>
         </is>
       </c>
       <c r="I100" s="25" t="n">
@@ -4186,7 +4187,7 @@
       </c>
       <c r="H101" s="25" t="inlineStr">
         <is>
-          <t>02-9-10-AB</t>
+          <t>0209AB/0210AB</t>
         </is>
       </c>
       <c r="I101" s="25" t="n">
@@ -4225,7 +4226,7 @@
       </c>
       <c r="H102" s="25" t="inlineStr">
         <is>
-          <t>02-9-10-AB</t>
+          <t>0209AB/0210AB</t>
         </is>
       </c>
       <c r="I102" s="25" t="n">
@@ -4264,7 +4265,7 @@
       </c>
       <c r="H103" s="25" t="inlineStr">
         <is>
-          <t>02-9-10-AB</t>
+          <t>0209AB/0210AB</t>
         </is>
       </c>
       <c r="I103" s="25" t="n">
@@ -4303,7 +4304,7 @@
       </c>
       <c r="H104" s="25" t="inlineStr">
         <is>
-          <t>02-9-10-AB</t>
+          <t>0209AB/0210AB</t>
         </is>
       </c>
       <c r="I104" s="25" t="n">
@@ -4342,7 +4343,7 @@
       </c>
       <c r="H105" s="25" t="inlineStr">
         <is>
-          <t>02-9-10-AB</t>
+          <t>0209AB/0210AB</t>
         </is>
       </c>
       <c r="I105" s="25" t="n">
@@ -4381,7 +4382,7 @@
       </c>
       <c r="H106" s="25" t="inlineStr">
         <is>
-          <t>02-9-10-AB</t>
+          <t>0209AB/0210AB</t>
         </is>
       </c>
       <c r="I106" s="25" t="n">
@@ -4420,7 +4421,7 @@
       </c>
       <c r="H107" s="25" t="inlineStr">
         <is>
-          <t>02-9-10-AB</t>
+          <t>0209AB/0210AB</t>
         </is>
       </c>
       <c r="I107" s="25" t="n">
@@ -4459,7 +4460,7 @@
       </c>
       <c r="H108" s="25" t="inlineStr">
         <is>
-          <t>02-11-12-AB</t>
+          <t xml:space="preserve">0211AB/0212AB  </t>
         </is>
       </c>
       <c r="I108" s="25" t="n">
@@ -4498,7 +4499,7 @@
       </c>
       <c r="H109" s="25" t="inlineStr">
         <is>
-          <t>02-11-12-AB</t>
+          <t xml:space="preserve">0211AB/0212AB  </t>
         </is>
       </c>
       <c r="I109" s="25" t="n">
@@ -4537,7 +4538,7 @@
       </c>
       <c r="H110" s="25" t="inlineStr">
         <is>
-          <t>02-11-12-AB</t>
+          <t xml:space="preserve">0211AB/0212AB  </t>
         </is>
       </c>
       <c r="I110" s="25" t="n">
@@ -4576,7 +4577,7 @@
       </c>
       <c r="H111" s="25" t="inlineStr">
         <is>
-          <t>02-11-12-AB</t>
+          <t xml:space="preserve">0211AB/0212AB  </t>
         </is>
       </c>
       <c r="I111" s="25" t="n">
@@ -4615,7 +4616,7 @@
       </c>
       <c r="H112" s="25" t="inlineStr">
         <is>
-          <t>02-11-12-AB</t>
+          <t xml:space="preserve">0211AB/0212AB  </t>
         </is>
       </c>
       <c r="I112" s="25" t="n">
@@ -4634,7 +4635,7 @@
       <c r="L113" s="8" t="n"/>
     </row>
     <row r="114" ht="18" customHeight="1">
-      <c r="B114" s="21" t="n">
+      <c r="B114" s="19" t="n">
         <v>43</v>
       </c>
       <c r="C114" s="25" t="inlineStr">
@@ -4657,7 +4658,7 @@
       </c>
       <c r="H114" s="25" t="inlineStr">
         <is>
-          <t>03-5-6-7-8-9-10-A</t>
+          <t xml:space="preserve">0305A0/0306A0/0307A0/0308A0/0309A0/0310A0     </t>
         </is>
       </c>
       <c r="I114" s="25" t="n">
@@ -4673,7 +4674,7 @@
       </c>
     </row>
     <row r="115" ht="18" customHeight="1">
-      <c r="B115" s="21" t="n">
+      <c r="B115" s="19" t="n">
         <v>44</v>
       </c>
       <c r="C115" s="25" t="inlineStr">
@@ -4696,7 +4697,7 @@
       </c>
       <c r="H115" s="25" t="inlineStr">
         <is>
-          <t>03-5-6-7-8-9-10-A</t>
+          <t xml:space="preserve">0305A0/0306A0/0307A0/0308A0/0309A0/0310A0    </t>
         </is>
       </c>
       <c r="I115" s="25" t="n">
@@ -4712,7 +4713,7 @@
       </c>
     </row>
     <row r="116" ht="18" customHeight="1">
-      <c r="B116" s="22" t="n">
+      <c r="B116" s="21" t="n">
         <v>61</v>
       </c>
       <c r="C116" s="25" t="inlineStr">
@@ -4737,7 +4738,7 @@
       </c>
       <c r="H116" s="25" t="inlineStr">
         <is>
-          <t>03-5-6-7-B&amp;04-5-6-7 AB</t>
+          <t xml:space="preserve">03050B/03060B/03070B_0305AB/0306AB/0307AB  </t>
         </is>
       </c>
       <c r="I116" s="25" t="n">
@@ -4780,7 +4781,7 @@
       </c>
       <c r="H117" s="25" t="inlineStr">
         <is>
-          <t>03-8-9-10-B&amp;04-8-9-10 AB</t>
+          <t xml:space="preserve">03080B/03090B/03100B_0308AB/0309AB/0310AB  </t>
         </is>
       </c>
       <c r="I117" s="25" t="n">
@@ -4796,7 +4797,7 @@
       </c>
     </row>
     <row r="118" ht="18" customHeight="1">
-      <c r="B118" s="22" t="n">
+      <c r="B118" s="21" t="n">
         <v>63</v>
       </c>
       <c r="C118" s="25" t="inlineStr">
@@ -4821,7 +4822,7 @@
       </c>
       <c r="H118" s="25" t="inlineStr">
         <is>
-          <t>03-5-6-7-B&amp;04-5-6-7 AB</t>
+          <t xml:space="preserve">03050B/03060B/03070B_0305AB/0306AB/0307AB  </t>
         </is>
       </c>
       <c r="I118" s="25" t="n">
@@ -4859,7 +4860,7 @@
       </c>
       <c r="H119" s="25" t="inlineStr">
         <is>
-          <t>03-8-9-10-B&amp;04-8-9-10 AB</t>
+          <t xml:space="preserve">03080B/03090B/03100B_0308AB/0309AB/0310AB  </t>
         </is>
       </c>
       <c r="I119" s="25" t="n">
@@ -4875,7 +4876,7 @@
       </c>
     </row>
     <row r="120" ht="18" customHeight="1">
-      <c r="B120" s="22" t="n">
+      <c r="B120" s="21" t="n">
         <v>64</v>
       </c>
       <c r="C120" s="25" t="inlineStr">
@@ -4900,7 +4901,7 @@
       </c>
       <c r="H120" s="25" t="inlineStr">
         <is>
-          <t>03-5-6-7-B&amp;04-5-6-7 AB</t>
+          <t xml:space="preserve">03050B/03060B/03070B_0305AB/0306AB/0307AB  </t>
         </is>
       </c>
       <c r="I120" s="25" t="n">
@@ -4938,7 +4939,7 @@
       </c>
       <c r="H121" s="25" t="inlineStr">
         <is>
-          <t>03-8-9-10-B&amp;04-8-9-10 AB</t>
+          <t xml:space="preserve">03080B/03090B/03100B_0308AB/0309AB/0310AB  </t>
         </is>
       </c>
       <c r="I121" s="25" t="n">
@@ -4979,7 +4980,7 @@
       </c>
       <c r="H122" s="25" t="inlineStr">
         <is>
-          <t>03-11-12-AB&amp;04-11-12-AB</t>
+          <t>0311AB/0312AB_ 0411AB/0412AB</t>
         </is>
       </c>
       <c r="I122" s="25" t="n">
@@ -5017,7 +5018,7 @@
       </c>
       <c r="H124" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-17-18-A</t>
+          <t>0014A0/0015A0/0016A0/ 0017A0/0018A0</t>
         </is>
       </c>
       <c r="I124" s="25" t="inlineStr">
@@ -5035,7 +5036,7 @@
       </c>
     </row>
     <row r="125" ht="18" customHeight="1">
-      <c r="B125" s="21" t="n">
+      <c r="B125" s="19" t="n">
         <v>18</v>
       </c>
       <c r="C125" s="25" t="inlineStr">
@@ -5058,7 +5059,7 @@
       </c>
       <c r="H125" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-17-18-B</t>
+          <t>0014A0/0015A0/0016A0/ 0017A0/0018A0</t>
         </is>
       </c>
       <c r="I125" s="25" t="n">
@@ -5074,7 +5075,7 @@
       </c>
     </row>
     <row r="126" ht="18" customHeight="1">
-      <c r="B126" s="21" t="n">
+      <c r="B126" s="19" t="n">
         <v>19</v>
       </c>
       <c r="C126" s="25" t="inlineStr">
@@ -5097,7 +5098,7 @@
       </c>
       <c r="H126" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-17-18-B</t>
+          <t>0014A0/0015A0/0016A0/ 0017A0/0018A0</t>
         </is>
       </c>
       <c r="I126" s="25" t="n">
@@ -5113,7 +5114,7 @@
       </c>
     </row>
     <row r="127" ht="18" customHeight="1">
-      <c r="B127" s="21" t="n">
+      <c r="B127" s="19" t="n">
         <v>20</v>
       </c>
       <c r="C127" s="25" t="inlineStr">
@@ -5136,7 +5137,7 @@
       </c>
       <c r="H127" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-17-18-B</t>
+          <t>0014A0/0015A0/0016A0/ 0017A0/0018A0</t>
         </is>
       </c>
       <c r="I127" s="25" t="n">
@@ -5153,7 +5154,7 @@
     </row>
     <row r="128" ht="3" customHeight="1"/>
     <row r="129" ht="18" customHeight="1">
-      <c r="B129" s="21" t="n">
+      <c r="B129" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C129" s="25" t="inlineStr">
@@ -5176,7 +5177,7 @@
       </c>
       <c r="H129" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t>0114A0/0115A0/0116A0</t>
         </is>
       </c>
       <c r="I129" s="25" t="n">
@@ -5212,7 +5213,7 @@
       </c>
       <c r="H130" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t>01140B/01150B/01160B</t>
         </is>
       </c>
       <c r="I130" s="25" t="n">
@@ -5228,7 +5229,7 @@
       </c>
     </row>
     <row r="131" ht="18" customHeight="1">
-      <c r="B131" s="21" t="n">
+      <c r="B131" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C131" s="25" t="inlineStr">
@@ -5251,7 +5252,7 @@
       </c>
       <c r="H131" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t>0114A0/0115A0/0116A0</t>
         </is>
       </c>
       <c r="I131" s="25" t="n">
@@ -5287,7 +5288,7 @@
       </c>
       <c r="H132" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t>01140B/01150B/01160B</t>
         </is>
       </c>
       <c r="I132" s="25" t="n">
@@ -5326,13 +5327,13 @@
       </c>
       <c r="H133" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0117AB/0118AB</t>
         </is>
       </c>
       <c r="I133" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K133" s="15" t="inlineStr">
+      <c r="K133" s="25" t="inlineStr">
         <is>
           <t>DB-P3-01-2MP_1D.A</t>
         </is>
@@ -5365,7 +5366,7 @@
       </c>
       <c r="H134" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0117AB/0118AB</t>
         </is>
       </c>
       <c r="I134" s="25" t="n">
@@ -5404,7 +5405,7 @@
       </c>
       <c r="H135" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0117AB/0118AB</t>
         </is>
       </c>
       <c r="I135" s="25" t="n">
@@ -5443,7 +5444,7 @@
       </c>
       <c r="H136" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0117AB/0118AB</t>
         </is>
       </c>
       <c r="I136" s="25" t="n">
@@ -5482,7 +5483,7 @@
       </c>
       <c r="H137" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0117AB/0118AB</t>
         </is>
       </c>
       <c r="I137" s="25" t="n">
@@ -5521,7 +5522,7 @@
       </c>
       <c r="H138" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0117AB/0118AB</t>
         </is>
       </c>
       <c r="I138" s="25" t="n">
@@ -5560,7 +5561,7 @@
       </c>
       <c r="H139" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0117AB/0118AB</t>
         </is>
       </c>
       <c r="I139" s="25" t="n">
@@ -5577,7 +5578,7 @@
     </row>
     <row r="140" ht="3" customHeight="1"/>
     <row r="141" ht="18" customHeight="1">
-      <c r="B141" s="21" t="n">
+      <c r="B141" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C141" s="25" t="inlineStr">
@@ -5600,7 +5601,7 @@
       </c>
       <c r="H141" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t xml:space="preserve">0214A0/0215A0/0216A0  </t>
         </is>
       </c>
       <c r="I141" s="25" t="n">
@@ -5636,7 +5637,7 @@
       </c>
       <c r="H142" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">02140B/02150B/02160B  </t>
         </is>
       </c>
       <c r="I142" s="25" t="n">
@@ -5652,7 +5653,7 @@
       </c>
     </row>
     <row r="143" ht="18" customHeight="1">
-      <c r="B143" s="21" t="n">
+      <c r="B143" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C143" s="25" t="inlineStr">
@@ -5675,7 +5676,7 @@
       </c>
       <c r="H143" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t xml:space="preserve">0214A0/0215A0/0216A0  </t>
         </is>
       </c>
       <c r="I143" s="25" t="n">
@@ -5711,7 +5712,7 @@
       </c>
       <c r="H144" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">02140B/02150B/02160B  </t>
         </is>
       </c>
       <c r="I144" s="25" t="n">
@@ -5750,7 +5751,7 @@
       </c>
       <c r="H145" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0217AB/0218AB</t>
         </is>
       </c>
       <c r="I145" s="25" t="n">
@@ -5789,7 +5790,7 @@
       </c>
       <c r="H146" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0217AB/0218AB</t>
         </is>
       </c>
       <c r="I146" s="25" t="n">
@@ -5828,7 +5829,7 @@
       </c>
       <c r="H147" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0217AB/0218AB</t>
         </is>
       </c>
       <c r="I147" s="25" t="n">
@@ -5867,7 +5868,7 @@
       </c>
       <c r="H148" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0217AB/0218AB</t>
         </is>
       </c>
       <c r="I148" s="25" t="n">
@@ -5906,7 +5907,7 @@
       </c>
       <c r="H149" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0217AB/0218AB</t>
         </is>
       </c>
       <c r="I149" s="25" t="n">
@@ -5945,7 +5946,7 @@
       </c>
       <c r="H150" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0217AB/0218AB</t>
         </is>
       </c>
       <c r="I150" s="25" t="n">
@@ -5984,7 +5985,7 @@
       </c>
       <c r="H151" s="25" t="inlineStr">
         <is>
-          <t>02-17-18-AB</t>
+          <t>0217AB/0218AB</t>
         </is>
       </c>
       <c r="I151" s="25" t="n">
@@ -6001,7 +6002,7 @@
     </row>
     <row r="152" ht="3" customHeight="1"/>
     <row r="153" ht="18" customHeight="1">
-      <c r="B153" s="21" t="n">
+      <c r="B153" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C153" s="25" t="inlineStr">
@@ -6024,7 +6025,7 @@
       </c>
       <c r="H153" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-B</t>
+          <t>00060B/00070B/00080B</t>
         </is>
       </c>
       <c r="I153" s="25" t="n">
@@ -6040,7 +6041,7 @@
       </c>
     </row>
     <row r="154" ht="18" customHeight="1">
-      <c r="B154" s="21" t="n">
+      <c r="B154" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C154" s="25" t="inlineStr">
@@ -6063,7 +6064,7 @@
       </c>
       <c r="H154" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-B</t>
+          <t>00060B/00070B/00080B</t>
         </is>
       </c>
       <c r="I154" s="25" t="n">
@@ -6079,7 +6080,7 @@
       </c>
     </row>
     <row r="155" ht="18" customHeight="1">
-      <c r="B155" s="22" t="n">
+      <c r="B155" s="21" t="n">
         <v>61</v>
       </c>
       <c r="C155" s="25" t="inlineStr">
@@ -6104,13 +6105,13 @@
       </c>
       <c r="H155" s="25" t="inlineStr">
         <is>
-          <t>03-14-15-16-B&amp;04-14-15-16 AB</t>
+          <t>03140B/03150B/03160B_0414AB/0415AB/0416AB</t>
         </is>
       </c>
       <c r="I155" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="K155" s="15" t="inlineStr">
+      <c r="K155" s="25" t="inlineStr">
         <is>
           <t>DB-P3-03_Atico-3MF_0D.A_DA&amp;3MF_2D.A1_DA</t>
         </is>
@@ -6120,7 +6121,7 @@
       </c>
     </row>
     <row r="156" ht="18" customHeight="1">
-      <c r="B156" s="22" t="n">
+      <c r="B156" s="21" t="n">
         <v>62</v>
       </c>
       <c r="C156" s="25" t="inlineStr">
@@ -6145,7 +6146,7 @@
       </c>
       <c r="H156" s="25" t="inlineStr">
         <is>
-          <t>03-14-15-16-B&amp;04-14-15-16 AB</t>
+          <t>03140B/03150B/03160B_0414AB/0415AB/0416AB</t>
         </is>
       </c>
       <c r="I156" s="25" t="n">
@@ -6161,7 +6162,7 @@
       </c>
     </row>
     <row r="157" ht="18" customHeight="1">
-      <c r="B157" s="22" t="n">
+      <c r="B157" s="21" t="n">
         <v>63</v>
       </c>
       <c r="C157" s="25" t="inlineStr">
@@ -6186,7 +6187,7 @@
       </c>
       <c r="H157" s="25" t="inlineStr">
         <is>
-          <t>03-14-15-16-B&amp;04-14-15-16 AB</t>
+          <t>03140B/03150B/03160B_0414AB/0415AB/0416AB</t>
         </is>
       </c>
       <c r="I157" s="25" t="n">
@@ -6202,7 +6203,7 @@
       </c>
     </row>
     <row r="158" ht="18" customHeight="1">
-      <c r="B158" s="22" t="n">
+      <c r="B158" s="21" t="n">
         <v>64</v>
       </c>
       <c r="C158" s="25" t="inlineStr">
@@ -6227,7 +6228,7 @@
       </c>
       <c r="H158" s="25" t="inlineStr">
         <is>
-          <t>03-14-15-16-B&amp;04-14-15-16 AB</t>
+          <t>03140B/03150B/03160B_0414AB/0415AB/0416AB</t>
         </is>
       </c>
       <c r="I158" s="25" t="n">
@@ -6268,7 +6269,7 @@
       </c>
       <c r="H159" s="25" t="inlineStr">
         <is>
-          <t>03-17-18-AB&amp;04-17-18-AB</t>
+          <t>0317AB/0318AB_0417AB/0418AB</t>
         </is>
       </c>
       <c r="I159" s="25" t="n">
@@ -6316,34 +6317,34 @@
     <row r="190" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="B131:B132"/>
     <mergeCell ref="B141:B142"/>
     <mergeCell ref="B143:B144"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B89:B90"/>
     <mergeCell ref="B95:B96"/>
     <mergeCell ref="B97:B98"/>
     <mergeCell ref="B99:B100"/>
     <mergeCell ref="B116:B117"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="B120:B121"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>
@@ -6353,39 +6354,40 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="FF92D050"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="B2:L79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11:L12"/>
+      <selection pane="bottomRight" activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col width="2.140625" customWidth="1" style="25" min="1" max="1"/>
     <col width="8.85546875" customWidth="1" style="25" min="2" max="2"/>
-    <col width="12.42578125" customWidth="1" style="25" min="3" max="3"/>
-    <col width="9.7109375" customWidth="1" style="25" min="4" max="4"/>
-    <col width="10.42578125" customWidth="1" style="25" min="5" max="5"/>
+    <col width="10.42578125" customWidth="1" style="25" min="3" max="3"/>
+    <col width="8.28515625" customWidth="1" style="25" min="4" max="4"/>
+    <col width="9.42578125" customWidth="1" style="25" min="5" max="5"/>
     <col width="39.7109375" customWidth="1" style="25" min="6" max="6"/>
     <col width="1.140625" customWidth="1" style="25" min="7" max="7"/>
-    <col width="29.28515625" customWidth="1" style="25" min="8" max="8"/>
+    <col width="52.5703125" customWidth="1" style="25" min="8" max="8"/>
     <col width="10.42578125" customWidth="1" style="25" min="9" max="9"/>
     <col width="1.5703125" customWidth="1" style="25" min="10" max="10"/>
     <col width="51.28515625" customWidth="1" style="25" min="11" max="11"/>
     <col width="10.7109375" customWidth="1" style="25" min="12" max="12"/>
-    <col width="11.42578125" customWidth="1" style="25" min="13" max="16"/>
-    <col width="11.42578125" customWidth="1" style="25" min="17" max="16384"/>
+    <col width="11.42578125" customWidth="1" style="25" min="13" max="25"/>
+    <col width="11.42578125" customWidth="1" style="25" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="6" customHeight="1"/>
     <row r="2" ht="49.5" customHeight="1">
-      <c r="B2" s="19" t="inlineStr">
+      <c r="B2" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">V     E     R     S     I     Ó      N           1     </t>
         </is>
@@ -6466,7 +6468,7 @@
       </c>
       <c r="H5" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A&amp;01-1-2-3-A</t>
+          <t xml:space="preserve">0001A0/0002A0/0003A0_0101A0/0102A0/0103A0 </t>
         </is>
       </c>
       <c r="I5" s="25" t="n">
@@ -6507,7 +6509,7 @@
       </c>
       <c r="H6" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A&amp;01-1-2-3-A</t>
+          <t xml:space="preserve">0001A0/0002A0/0003A0_0101A0/0102A0/0103A0 </t>
         </is>
       </c>
       <c r="I6" s="25" t="n">
@@ -6548,7 +6550,7 @@
       </c>
       <c r="H7" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A&amp;01-1-2-3-A</t>
+          <t xml:space="preserve">0001A0/0002A0/0003A0_0101A0/0102A0/0103A0 </t>
         </is>
       </c>
       <c r="I7" s="25" t="n">
@@ -6589,7 +6591,7 @@
       </c>
       <c r="H8" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A&amp;01-1-2-3-A</t>
+          <t xml:space="preserve">0001A0/0002A0/0003A0_0101A0/0102A0/0103A0 </t>
         </is>
       </c>
       <c r="I8" s="25" t="n">
@@ -6631,7 +6633,7 @@
       </c>
       <c r="H10" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-B&amp;01-1-2-3-B</t>
+          <t>00010B/00020B/00030B_01010B/01020B/01030B</t>
         </is>
       </c>
       <c r="I10" s="25" t="n">
@@ -6672,7 +6674,7 @@
       </c>
       <c r="H11" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-B&amp;01-1-2-3-B</t>
+          <t>00010B/00020B/00030B_01010B/01020B/01030B</t>
         </is>
       </c>
       <c r="I11" s="25" t="n">
@@ -6713,7 +6715,7 @@
       </c>
       <c r="H12" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-B&amp;01-1-2-3-B</t>
+          <t>00010B/00020B/00030B_01010B/01020B/01030B</t>
         </is>
       </c>
       <c r="I12" s="25" t="n">
@@ -6755,7 +6757,7 @@
       </c>
       <c r="H14" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-A&amp;02-1-2-3-A</t>
+          <t xml:space="preserve">0101A0/0102A0/0103A0_0201A0/0202A0/0203A0 </t>
         </is>
       </c>
       <c r="I14" s="25" t="n">
@@ -6796,7 +6798,7 @@
       </c>
       <c r="H15" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-A&amp;02-1-2-3-A</t>
+          <t xml:space="preserve">0101A0/0102A0/0103A0_0201A0/0202A0/0203A0 </t>
         </is>
       </c>
       <c r="I15" s="25" t="n">
@@ -6837,7 +6839,7 @@
       </c>
       <c r="H16" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-A&amp;02-1-2-3-A</t>
+          <t xml:space="preserve">0101A0/0102A0/0103A0_0201A0/0202A0/0203A0 </t>
         </is>
       </c>
       <c r="I16" s="25" t="n">
@@ -6878,7 +6880,7 @@
       </c>
       <c r="H17" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-A&amp;02-1-2-3-A</t>
+          <t xml:space="preserve">0101A0/0102A0/0103A0_0201A0/0202A0/0203A0 </t>
         </is>
       </c>
       <c r="I17" s="25" t="n">
@@ -6922,7 +6924,7 @@
       </c>
       <c r="H19" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-B&amp;02-1-2-3-B</t>
+          <t xml:space="preserve">01010B/01020B/01030B_02010B/02020B/02030B </t>
         </is>
       </c>
       <c r="I19" s="25" t="n">
@@ -6963,7 +6965,7 @@
       </c>
       <c r="H20" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-B&amp;02-1-2-3-B</t>
+          <t xml:space="preserve">01010B/01020B/01030B_02010B/02020B/02030B </t>
         </is>
       </c>
       <c r="I20" s="25" t="n">
@@ -7004,7 +7006,7 @@
       </c>
       <c r="H21" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-B&amp;02-1-2-3-B</t>
+          <t xml:space="preserve">01010B/01020B/01030B_02010B/02020B/02030B </t>
         </is>
       </c>
       <c r="I21" s="25" t="n">
@@ -7045,7 +7047,7 @@
       </c>
       <c r="H22" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-B&amp;02-1-2-3-B</t>
+          <t xml:space="preserve">01010B/01020B/01030B_02010B/02020B/02030B </t>
         </is>
       </c>
       <c r="I22" s="25" t="n">
@@ -7087,7 +7089,7 @@
       </c>
       <c r="H24" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-A&amp;03-1-2-3-A</t>
+          <t xml:space="preserve">0201A0/0202A0/0203A0_0301A0/0302A0/0303A0 </t>
         </is>
       </c>
       <c r="I24" s="25" t="n">
@@ -7128,7 +7130,7 @@
       </c>
       <c r="H25" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-A&amp;03-1-2-3-A</t>
+          <t xml:space="preserve">0201A0/0202A0/0203A0_0301A0/0302A0/0303A0 </t>
         </is>
       </c>
       <c r="I25" s="25" t="n">
@@ -7169,7 +7171,7 @@
       </c>
       <c r="H26" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-A&amp;03-1-2-3-A</t>
+          <t xml:space="preserve">0201A0/0202A0/0203A0_0301A0/0302A0/0303A0 </t>
         </is>
       </c>
       <c r="I26" s="25" t="n">
@@ -7210,7 +7212,7 @@
       </c>
       <c r="H27" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-A&amp;03-1-2-3-A</t>
+          <t xml:space="preserve">0201A0/0202A0/0203A0_0301A0/0302A0/0303A0 </t>
         </is>
       </c>
       <c r="I27" s="25" t="n">
@@ -7259,7 +7261,7 @@
       </c>
       <c r="H31" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-A</t>
+          <t xml:space="preserve">0006A0/0007A0/0008A0 </t>
         </is>
       </c>
       <c r="I31" s="25" t="inlineStr">
@@ -7277,7 +7279,7 @@
       </c>
     </row>
     <row r="32" ht="18" customHeight="1">
-      <c r="B32" s="21" t="n">
+      <c r="B32" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="25" t="inlineStr">
@@ -7300,7 +7302,7 @@
       </c>
       <c r="H32" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-B</t>
+          <t xml:space="preserve">00060B/00070B/00080B </t>
         </is>
       </c>
       <c r="I32" s="25" t="n">
@@ -7316,7 +7318,7 @@
       </c>
     </row>
     <row r="33" ht="18" customHeight="1">
-      <c r="B33" s="21" t="n">
+      <c r="B33" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C33" s="25" t="inlineStr">
@@ -7339,7 +7341,7 @@
       </c>
       <c r="H33" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-B</t>
+          <t xml:space="preserve">00060B/00070B/00080B </t>
         </is>
       </c>
       <c r="I33" s="25" t="n">
@@ -7380,7 +7382,7 @@
       </c>
       <c r="H34" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB&amp;01-9-10-AB</t>
+          <t>0009AB/0010AB_0109AB/0110AB</t>
         </is>
       </c>
       <c r="I34" s="25" t="n">
@@ -7421,7 +7423,7 @@
       </c>
       <c r="H35" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB&amp;01-9-10-AB</t>
+          <t>0009AB/0010AB_0109AB/0110AB</t>
         </is>
       </c>
       <c r="I35" s="25" t="n">
@@ -7462,7 +7464,7 @@
       </c>
       <c r="H36" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB&amp;01-11-12-AB</t>
+          <t>0011AB/0120AB_0111AB/0112AB</t>
         </is>
       </c>
       <c r="I36" s="25" t="n">
@@ -7503,7 +7505,7 @@
       </c>
       <c r="H37" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB&amp;01-11-12-AB</t>
+          <t>0011AB/0120AB_0111AB/0112AB</t>
         </is>
       </c>
       <c r="I37" s="25" t="n">
@@ -7520,7 +7522,7 @@
     </row>
     <row r="38" ht="4.5" customHeight="1"/>
     <row r="39" ht="18" customHeight="1">
-      <c r="B39" s="21" t="n">
+      <c r="B39" s="19" t="n">
         <v>5</v>
       </c>
       <c r="C39" s="25" t="inlineStr">
@@ -7543,7 +7545,7 @@
       </c>
       <c r="H39" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I39" s="25" t="n">
@@ -7579,7 +7581,7 @@
       </c>
       <c r="H40" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I40" s="25" t="n">
@@ -7595,7 +7597,7 @@
       </c>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="B41" s="21" t="n">
+      <c r="B41" s="19" t="n">
         <v>6</v>
       </c>
       <c r="C41" s="25" t="inlineStr">
@@ -7618,7 +7620,7 @@
       </c>
       <c r="H41" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I41" s="25" t="n">
@@ -7654,7 +7656,7 @@
       </c>
       <c r="H42" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I42" s="25" t="n">
@@ -7670,7 +7672,7 @@
       </c>
     </row>
     <row r="43" ht="18" customHeight="1">
-      <c r="B43" s="21" t="n">
+      <c r="B43" s="19" t="n">
         <v>7</v>
       </c>
       <c r="C43" s="25" t="inlineStr">
@@ -7693,7 +7695,7 @@
       </c>
       <c r="H43" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I43" s="25" t="n">
@@ -7729,7 +7731,7 @@
       </c>
       <c r="H44" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I44" s="25" t="n">
@@ -7745,7 +7747,7 @@
       </c>
     </row>
     <row r="45" ht="18" customHeight="1">
-      <c r="B45" s="21" t="n">
+      <c r="B45" s="19" t="n">
         <v>8</v>
       </c>
       <c r="C45" s="25" t="inlineStr">
@@ -7768,7 +7770,7 @@
       </c>
       <c r="H45" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I45" s="25" t="n">
@@ -7804,7 +7806,7 @@
       </c>
       <c r="H46" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I46" s="25" t="n">
@@ -7820,7 +7822,7 @@
       </c>
     </row>
     <row r="47" ht="18" customHeight="1">
-      <c r="B47" s="21" t="n">
+      <c r="B47" s="19" t="n">
         <v>9</v>
       </c>
       <c r="C47" s="25" t="inlineStr">
@@ -7843,7 +7845,7 @@
       </c>
       <c r="H47" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I47" s="25" t="n">
@@ -7879,7 +7881,7 @@
       </c>
       <c r="H48" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I48" s="25" t="n">
@@ -7895,7 +7897,7 @@
       </c>
     </row>
     <row r="49" ht="18" customHeight="1">
-      <c r="B49" s="21" t="n">
+      <c r="B49" s="19" t="n">
         <v>10</v>
       </c>
       <c r="C49" s="25" t="inlineStr">
@@ -7918,7 +7920,7 @@
       </c>
       <c r="H49" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I49" s="25" t="n">
@@ -7954,7 +7956,7 @@
       </c>
       <c r="H50" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I50" s="25" t="n">
@@ -7970,7 +7972,7 @@
       </c>
     </row>
     <row r="51" ht="18" customHeight="1">
-      <c r="B51" s="21" t="n">
+      <c r="B51" s="19" t="n">
         <v>14</v>
       </c>
       <c r="C51" s="25" t="inlineStr">
@@ -7993,7 +7995,7 @@
       </c>
       <c r="H51" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I51" s="25" t="n">
@@ -8029,7 +8031,7 @@
       </c>
       <c r="H52" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I52" s="25" t="n">
@@ -8045,7 +8047,7 @@
       </c>
     </row>
     <row r="53" ht="18" customHeight="1">
-      <c r="B53" s="21" t="n">
+      <c r="B53" s="19" t="n">
         <v>15</v>
       </c>
       <c r="C53" s="25" t="inlineStr">
@@ -8068,7 +8070,7 @@
       </c>
       <c r="H53" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I53" s="25" t="n">
@@ -8104,7 +8106,7 @@
       </c>
       <c r="H54" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I54" s="25" t="n">
@@ -8120,7 +8122,7 @@
       </c>
     </row>
     <row r="55" ht="18" customHeight="1">
-      <c r="B55" s="21" t="n">
+      <c r="B55" s="19" t="n">
         <v>16</v>
       </c>
       <c r="C55" s="25" t="inlineStr">
@@ -8143,7 +8145,7 @@
       </c>
       <c r="H55" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I55" s="25" t="n">
@@ -8179,7 +8181,7 @@
       </c>
       <c r="H56" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I56" s="25" t="n">
@@ -8195,7 +8197,7 @@
       </c>
     </row>
     <row r="57" ht="18" customHeight="1">
-      <c r="B57" s="21" t="n">
+      <c r="B57" s="19" t="n">
         <v>17</v>
       </c>
       <c r="C57" s="25" t="inlineStr">
@@ -8218,7 +8220,7 @@
       </c>
       <c r="H57" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0</t>
         </is>
       </c>
       <c r="I57" s="25" t="n">
@@ -8254,7 +8256,7 @@
       </c>
       <c r="H58" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t>01050B/01060B/01070B/01080B</t>
         </is>
       </c>
       <c r="I58" s="25" t="n">
@@ -8295,7 +8297,7 @@
       </c>
       <c r="H59" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB&amp;02-9-10-AB</t>
+          <t xml:space="preserve">0109AB/0110AB_0209AB/0210AB  </t>
         </is>
       </c>
       <c r="I59" s="25" t="n">
@@ -8336,7 +8338,7 @@
       </c>
       <c r="H60" s="25" t="inlineStr">
         <is>
-          <t>01-9-10-AB&amp;02-9-10-AB</t>
+          <t xml:space="preserve">0109AB/0110AB_0209AB/0210AB  </t>
         </is>
       </c>
       <c r="I60" s="25" t="n">
@@ -8377,7 +8379,7 @@
       </c>
       <c r="H61" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB&amp;02-11-12-AB</t>
+          <t xml:space="preserve">0111AB/0112AB_0211AB/0212AB   </t>
         </is>
       </c>
       <c r="I61" s="25" t="n">
@@ -8418,7 +8420,7 @@
       </c>
       <c r="H62" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB&amp;02-11-12-AB</t>
+          <t xml:space="preserve">0111AB/0112AB_0211AB/0212AB   </t>
         </is>
       </c>
       <c r="I62" s="25" t="n">
@@ -8469,7 +8471,7 @@
       </c>
       <c r="H66" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t xml:space="preserve">0014A0/0015A0/0016A0  </t>
         </is>
       </c>
       <c r="I66" s="25" t="inlineStr">
@@ -8487,7 +8489,7 @@
       </c>
     </row>
     <row r="67" ht="18" customHeight="1">
-      <c r="B67" s="21" t="n">
+      <c r="B67" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="25" t="inlineStr">
@@ -8510,7 +8512,7 @@
       </c>
       <c r="H67" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">00140B/00150B/00160B </t>
         </is>
       </c>
       <c r="I67" s="25" t="n">
@@ -8526,7 +8528,7 @@
       </c>
     </row>
     <row r="68" ht="18" customHeight="1">
-      <c r="B68" s="21" t="n">
+      <c r="B68" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C68" s="25" t="inlineStr">
@@ -8549,7 +8551,7 @@
       </c>
       <c r="H68" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">00140B/00150B/00160B </t>
         </is>
       </c>
       <c r="I68" s="25" t="n">
@@ -8590,7 +8592,7 @@
       </c>
       <c r="H69" s="25" t="inlineStr">
         <is>
-          <t>00-17-18-AB&amp;01-17-18-AB</t>
+          <t xml:space="preserve">0017AB/0018AB_0117AB/0118AB   </t>
         </is>
       </c>
       <c r="I69" s="25" t="n">
@@ -8631,7 +8633,7 @@
       </c>
       <c r="H70" s="25" t="inlineStr">
         <is>
-          <t>00-17-18-AB&amp;01-17-18-AB</t>
+          <t xml:space="preserve">0017AB/0018AB_0117AB/0118AB   </t>
         </is>
       </c>
       <c r="I70" s="25" t="n">
@@ -8647,7 +8649,7 @@
       </c>
     </row>
     <row r="71" ht="18" customHeight="1">
-      <c r="B71" s="21" t="n">
+      <c r="B71" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="25" t="inlineStr">
@@ -8670,7 +8672,7 @@
       </c>
       <c r="H71" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t xml:space="preserve">0114A0/0115A0/0116A0  </t>
         </is>
       </c>
       <c r="I71" s="25" t="n">
@@ -8706,7 +8708,7 @@
       </c>
       <c r="H72" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">01140B/01150B/01160B  </t>
         </is>
       </c>
       <c r="I72" s="25" t="n">
@@ -8722,7 +8724,7 @@
       </c>
     </row>
     <row r="73" ht="18" customHeight="1">
-      <c r="B73" s="21" t="n">
+      <c r="B73" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C73" s="25" t="inlineStr">
@@ -8745,7 +8747,7 @@
       </c>
       <c r="H73" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t xml:space="preserve">0114A0/0115A0/0116A0  </t>
         </is>
       </c>
       <c r="I73" s="25" t="n">
@@ -8781,7 +8783,7 @@
       </c>
       <c r="H74" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">01140B/01150B/01160B  </t>
         </is>
       </c>
       <c r="I74" s="25" t="n">
@@ -8797,7 +8799,7 @@
       </c>
     </row>
     <row r="75" ht="18" customHeight="1">
-      <c r="B75" s="21" t="n">
+      <c r="B75" s="19" t="n">
         <v>18</v>
       </c>
       <c r="C75" s="25" t="inlineStr">
@@ -8820,7 +8822,7 @@
       </c>
       <c r="H75" s="25" t="inlineStr">
         <is>
-          <t>02-14-15-16-17-18-B</t>
+          <t>02140B/02150B/02160B/02170B/02180B</t>
         </is>
       </c>
       <c r="I75" s="25" t="n">
@@ -8836,7 +8838,7 @@
       </c>
     </row>
     <row r="76" ht="18" customHeight="1">
-      <c r="B76" s="21" t="n">
+      <c r="B76" s="19" t="n">
         <v>19</v>
       </c>
       <c r="C76" s="25" t="inlineStr">
@@ -8859,7 +8861,7 @@
       </c>
       <c r="H76" s="25" t="inlineStr">
         <is>
-          <t>02-14-15-16-17-18-B</t>
+          <t>02140B/02150B/02160B/02170B/02180B</t>
         </is>
       </c>
       <c r="I76" s="25" t="n">
@@ -8875,7 +8877,7 @@
       </c>
     </row>
     <row r="77" ht="18" customHeight="1">
-      <c r="B77" s="21" t="n">
+      <c r="B77" s="19" t="n">
         <v>20</v>
       </c>
       <c r="C77" s="25" t="inlineStr">
@@ -8898,7 +8900,7 @@
       </c>
       <c r="H77" s="25" t="inlineStr">
         <is>
-          <t>02-14-15-16-17-18-B</t>
+          <t>02140B/02150B/02160B/02170B/02180B</t>
         </is>
       </c>
       <c r="I77" s="25" t="n">
@@ -8946,21 +8948,21 @@
     <row r="99" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B64:H64"/>
     <mergeCell ref="B71:B72"/>
     <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B55:B56"/>
     <mergeCell ref="B43:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8977,10 +8979,10 @@
   <dimension ref="B2:L82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11:L12"/>
+      <selection pane="bottomRight" activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8992,18 +8994,18 @@
     <col width="10.42578125" customWidth="1" style="25" min="5" max="5"/>
     <col width="39.7109375" customWidth="1" style="25" min="6" max="6"/>
     <col width="1.140625" customWidth="1" style="25" min="7" max="7"/>
-    <col width="29.28515625" customWidth="1" style="25" min="8" max="8"/>
+    <col width="51.5703125" customWidth="1" style="25" min="8" max="8"/>
     <col width="11.42578125" customWidth="1" style="25" min="9" max="9"/>
     <col width="1.5703125" customWidth="1" style="25" min="10" max="10"/>
     <col width="51.7109375" customWidth="1" style="25" min="11" max="11"/>
     <col width="10.7109375" customWidth="1" style="25" min="12" max="12"/>
-    <col width="11.42578125" customWidth="1" style="25" min="13" max="16"/>
-    <col width="11.42578125" customWidth="1" style="25" min="17" max="16384"/>
+    <col width="11.42578125" customWidth="1" style="25" min="13" max="25"/>
+    <col width="11.42578125" customWidth="1" style="25" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="6" customHeight="1"/>
     <row r="2" ht="49.5" customHeight="1">
-      <c r="B2" s="19" t="inlineStr">
+      <c r="B2" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">V     E     R     S     I     Ó      N           2     </t>
         </is>
@@ -9084,7 +9086,7 @@
       </c>
       <c r="H5" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A&amp;01-1-2-3-A</t>
+          <t>0001A0/0002A0/0003A0_ 0101A0/0102A0/0103A0</t>
         </is>
       </c>
       <c r="I5" s="25" t="n">
@@ -9125,7 +9127,7 @@
       </c>
       <c r="H6" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A&amp;01-1-2-3-A</t>
+          <t>0001A0/0002A0/0003A0_ 0101A0/0102A0/0103A0</t>
         </is>
       </c>
       <c r="I6" s="25" t="n">
@@ -9166,7 +9168,7 @@
       </c>
       <c r="H7" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A&amp;01-1-2-3-A</t>
+          <t>0001A0/0002A0/0003A0_ 0101A0/0102A0/0103A0</t>
         </is>
       </c>
       <c r="I7" s="25" t="n">
@@ -9207,7 +9209,7 @@
       </c>
       <c r="H8" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-A&amp;01-1-2-3-A</t>
+          <t>0001A0/0002A0/0003A0_ 0101A0/0102A0/0103A0</t>
         </is>
       </c>
       <c r="I8" s="25" t="n">
@@ -9249,7 +9251,7 @@
       </c>
       <c r="H10" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-B&amp;01-1-2-3-B</t>
+          <t>00010B/00020B/00030B_ 01010B/01020B/01030B</t>
         </is>
       </c>
       <c r="I10" s="25" t="n">
@@ -9290,7 +9292,7 @@
       </c>
       <c r="H11" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-B&amp;01-1-2-3-B</t>
+          <t>00010B/00020B/00030B_ 01010B/01020B/01030B</t>
         </is>
       </c>
       <c r="I11" s="25" t="n">
@@ -9331,7 +9333,7 @@
       </c>
       <c r="H12" s="25" t="inlineStr">
         <is>
-          <t>00-1-2-3-B&amp;01-1-2-3-B</t>
+          <t>00010B/00020B/00030B_ 01010B/01020B/01030B</t>
         </is>
       </c>
       <c r="I12" s="25" t="n">
@@ -9373,7 +9375,7 @@
       </c>
       <c r="H14" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-A&amp;02-1-2-3-A</t>
+          <t>0101A0/0102A0/0103A0_ 0201A0/0202A0/0203A0</t>
         </is>
       </c>
       <c r="I14" s="25" t="n">
@@ -9414,7 +9416,7 @@
       </c>
       <c r="H15" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-A&amp;02-1-2-3-A</t>
+          <t>0101A0/0102A0/0103A0_ 0201A0/0202A0/0203A0</t>
         </is>
       </c>
       <c r="I15" s="25" t="n">
@@ -9455,7 +9457,7 @@
       </c>
       <c r="H16" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-A&amp;02-1-2-3-A</t>
+          <t>0101A0/0102A0/0103A0_ 0201A0/0202A0/0203A0</t>
         </is>
       </c>
       <c r="I16" s="25" t="n">
@@ -9496,7 +9498,7 @@
       </c>
       <c r="H17" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-A&amp;02-1-2-3-A</t>
+          <t>0101A0/0102A0/0103A0_ 0201A0/0202A0/0203A0</t>
         </is>
       </c>
       <c r="I17" s="25" t="n">
@@ -9540,7 +9542,7 @@
       </c>
       <c r="H19" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-B&amp;02-1-2-3-B</t>
+          <t>01010B/01020B/01030B_ 02010B/02020B/02030B</t>
         </is>
       </c>
       <c r="I19" s="25" t="n">
@@ -9581,7 +9583,7 @@
       </c>
       <c r="H20" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-B&amp;02-1-2-3-B</t>
+          <t>01010B/01020B/01030B_ 02010B/02020B/02030B</t>
         </is>
       </c>
       <c r="I20" s="25" t="n">
@@ -9622,7 +9624,7 @@
       </c>
       <c r="H21" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-B&amp;02-1-2-3-B</t>
+          <t>01010B/01020B/01030B_ 02010B/02020B/02030B</t>
         </is>
       </c>
       <c r="I21" s="25" t="n">
@@ -9663,7 +9665,7 @@
       </c>
       <c r="H22" s="25" t="inlineStr">
         <is>
-          <t>01-1-2-3-B&amp;02-1-2-3-B</t>
+          <t>01010B/01020B/01030B_ 02010B/02020B/02030B</t>
         </is>
       </c>
       <c r="I22" s="25" t="n">
@@ -9705,7 +9707,7 @@
       </c>
       <c r="H24" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-A&amp;03-1-2-3-A</t>
+          <t>0201A0/0202A0/0203A0_ 0301A0/0302A0/0303A0</t>
         </is>
       </c>
       <c r="I24" s="25" t="n">
@@ -9746,7 +9748,7 @@
       </c>
       <c r="H25" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-A&amp;03-1-2-3-A</t>
+          <t>0201A0/0202A0/0203A0_ 0301A0/0302A0/0303A0</t>
         </is>
       </c>
       <c r="I25" s="25" t="n">
@@ -9787,7 +9789,7 @@
       </c>
       <c r="H26" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-A&amp;03-1-2-3-A</t>
+          <t>0201A0/0202A0/0203A0_ 0301A0/0302A0/0303A0</t>
         </is>
       </c>
       <c r="I26" s="25" t="n">
@@ -9828,7 +9830,7 @@
       </c>
       <c r="H27" s="25" t="inlineStr">
         <is>
-          <t>02-1-2-3-A&amp;03-1-2-3-A</t>
+          <t>0201A0/0202A0/0203A0_ 0301A0/0302A0/0303A0</t>
         </is>
       </c>
       <c r="I27" s="25" t="n">
@@ -9882,7 +9884,7 @@
       </c>
       <c r="H31" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-A</t>
+          <t xml:space="preserve">0006A0/0007A0/0008A0 </t>
         </is>
       </c>
       <c r="I31" s="25" t="inlineStr">
@@ -9900,7 +9902,7 @@
       </c>
     </row>
     <row r="32" ht="18" customHeight="1">
-      <c r="B32" s="21" t="n">
+      <c r="B32" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="25" t="inlineStr">
@@ -9923,7 +9925,7 @@
       </c>
       <c r="H32" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-B</t>
+          <t xml:space="preserve">00060B/00070B/00080B </t>
         </is>
       </c>
       <c r="I32" s="25" t="n">
@@ -9939,7 +9941,7 @@
       </c>
     </row>
     <row r="33" ht="18" customHeight="1">
-      <c r="B33" s="21" t="n">
+      <c r="B33" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C33" s="25" t="inlineStr">
@@ -9962,7 +9964,7 @@
       </c>
       <c r="H33" s="25" t="inlineStr">
         <is>
-          <t>00-6-7-8-B</t>
+          <t xml:space="preserve">00060B/00070B/00080B </t>
         </is>
       </c>
       <c r="I33" s="25" t="n">
@@ -10003,7 +10005,7 @@
       </c>
       <c r="H34" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB&amp;01-9-10-AB</t>
+          <t xml:space="preserve">0009AB/0010AB_0109AB/0110AB  </t>
         </is>
       </c>
       <c r="I34" s="25" t="n">
@@ -10044,7 +10046,7 @@
       </c>
       <c r="H35" s="25" t="inlineStr">
         <is>
-          <t>00-9-10-AB&amp;01-9-10-AB</t>
+          <t xml:space="preserve">0009AB/0010AB_0109AB/0110AB  </t>
         </is>
       </c>
       <c r="I35" s="25" t="n">
@@ -10085,7 +10087,7 @@
       </c>
       <c r="H36" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB&amp;01-11-12-AB</t>
+          <t xml:space="preserve">0009AB/0010AB_0109AB/0110AB  </t>
         </is>
       </c>
       <c r="I36" s="25" t="n">
@@ -10126,7 +10128,7 @@
       </c>
       <c r="H37" s="25" t="inlineStr">
         <is>
-          <t>00-11-12-AB&amp;01-11-12-AB</t>
+          <t xml:space="preserve">0009AB/0010AB_0109AB/0110AB  </t>
         </is>
       </c>
       <c r="I37" s="25" t="n">
@@ -10168,7 +10170,7 @@
       </c>
       <c r="H39" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A&amp;02-5-6-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0_0205A0/0206A0</t>
         </is>
       </c>
       <c r="I39" s="25" t="n">
@@ -10209,7 +10211,7 @@
       </c>
       <c r="H40" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B&amp;02-5-6-B</t>
+          <t>01050B/01060B/01070B/01080B_02050B/02060B</t>
         </is>
       </c>
       <c r="I40" s="25" t="n">
@@ -10250,7 +10252,7 @@
       </c>
       <c r="H41" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A&amp;02-5-6-A</t>
+          <t>0105A0/0106A0/0107A0/0108A0_0205A0/0206A0</t>
         </is>
       </c>
       <c r="I41" s="25" t="n">
@@ -10291,7 +10293,7 @@
       </c>
       <c r="H42" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B&amp;02-5-6-B</t>
+          <t>01050B/01060B/01070B/01080B_02050B/02060B</t>
         </is>
       </c>
       <c r="I42" s="25" t="n">
@@ -10308,7 +10310,7 @@
     </row>
     <row r="43" ht="18" customHeight="1"/>
     <row r="44" ht="18" customHeight="1">
-      <c r="B44" s="21" t="n">
+      <c r="B44" s="19" t="n">
         <v>5</v>
       </c>
       <c r="C44" s="25" t="inlineStr">
@@ -10331,7 +10333,7 @@
       </c>
       <c r="H44" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I44" s="25" t="n">
@@ -10367,7 +10369,7 @@
       </c>
       <c r="H45" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I45" s="25" t="n">
@@ -10383,7 +10385,7 @@
       </c>
     </row>
     <row r="46" ht="18" customHeight="1">
-      <c r="B46" s="21" t="n">
+      <c r="B46" s="19" t="n">
         <v>6</v>
       </c>
       <c r="C46" s="25" t="inlineStr">
@@ -10406,7 +10408,7 @@
       </c>
       <c r="H46" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I46" s="25" t="n">
@@ -10442,7 +10444,7 @@
       </c>
       <c r="H47" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I47" s="25" t="n">
@@ -10458,7 +10460,7 @@
       </c>
     </row>
     <row r="48" ht="18" customHeight="1">
-      <c r="B48" s="21" t="n">
+      <c r="B48" s="19" t="n">
         <v>7</v>
       </c>
       <c r="C48" s="25" t="inlineStr">
@@ -10481,7 +10483,7 @@
       </c>
       <c r="H48" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I48" s="25" t="n">
@@ -10517,7 +10519,7 @@
       </c>
       <c r="H49" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I49" s="25" t="n">
@@ -10533,7 +10535,7 @@
       </c>
     </row>
     <row r="50" ht="18" customHeight="1">
-      <c r="B50" s="21" t="n">
+      <c r="B50" s="19" t="n">
         <v>8</v>
       </c>
       <c r="C50" s="25" t="inlineStr">
@@ -10556,7 +10558,7 @@
       </c>
       <c r="H50" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I50" s="25" t="n">
@@ -10592,7 +10594,7 @@
       </c>
       <c r="H51" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I51" s="25" t="n">
@@ -10608,7 +10610,7 @@
       </c>
     </row>
     <row r="52" ht="18" customHeight="1">
-      <c r="B52" s="21" t="n">
+      <c r="B52" s="19" t="n">
         <v>9</v>
       </c>
       <c r="C52" s="25" t="inlineStr">
@@ -10631,7 +10633,7 @@
       </c>
       <c r="H52" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I52" s="25" t="n">
@@ -10667,7 +10669,7 @@
       </c>
       <c r="H53" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I53" s="25" t="n">
@@ -10683,7 +10685,7 @@
       </c>
     </row>
     <row r="54" ht="18" customHeight="1">
-      <c r="B54" s="21" t="n">
+      <c r="B54" s="19" t="n">
         <v>10</v>
       </c>
       <c r="C54" s="25" t="inlineStr">
@@ -10706,7 +10708,7 @@
       </c>
       <c r="H54" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I54" s="25" t="n">
@@ -10742,7 +10744,7 @@
       </c>
       <c r="H55" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I55" s="25" t="n">
@@ -10758,7 +10760,7 @@
       </c>
     </row>
     <row r="56" ht="18" customHeight="1">
-      <c r="B56" s="21" t="n">
+      <c r="B56" s="19" t="n">
         <v>14</v>
       </c>
       <c r="C56" s="25" t="inlineStr">
@@ -10781,7 +10783,7 @@
       </c>
       <c r="H56" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I56" s="25" t="n">
@@ -10817,7 +10819,7 @@
       </c>
       <c r="H57" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I57" s="25" t="n">
@@ -10833,7 +10835,7 @@
       </c>
     </row>
     <row r="58" ht="18" customHeight="1">
-      <c r="B58" s="21" t="n">
+      <c r="B58" s="19" t="n">
         <v>15</v>
       </c>
       <c r="C58" s="25" t="inlineStr">
@@ -10856,7 +10858,7 @@
       </c>
       <c r="H58" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I58" s="25" t="n">
@@ -10892,7 +10894,7 @@
       </c>
       <c r="H59" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I59" s="25" t="n">
@@ -10908,7 +10910,7 @@
       </c>
     </row>
     <row r="60" ht="18" customHeight="1">
-      <c r="B60" s="21" t="n">
+      <c r="B60" s="19" t="n">
         <v>16</v>
       </c>
       <c r="C60" s="25" t="inlineStr">
@@ -10931,7 +10933,7 @@
       </c>
       <c r="H60" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I60" s="25" t="n">
@@ -10967,7 +10969,7 @@
       </c>
       <c r="H61" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I61" s="25" t="n">
@@ -10983,7 +10985,7 @@
       </c>
     </row>
     <row r="62" ht="18" customHeight="1">
-      <c r="B62" s="21" t="n">
+      <c r="B62" s="19" t="n">
         <v>17</v>
       </c>
       <c r="C62" s="25" t="inlineStr">
@@ -11006,7 +11008,7 @@
       </c>
       <c r="H62" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-A</t>
+          <t xml:space="preserve">0205A0/0206A0/0207A0/0208A0  </t>
         </is>
       </c>
       <c r="I62" s="25" t="n">
@@ -11042,7 +11044,7 @@
       </c>
       <c r="H63" s="25" t="inlineStr">
         <is>
-          <t>01-5-6-7-8-B</t>
+          <t xml:space="preserve">02050B/02060B/02070B/02080B  </t>
         </is>
       </c>
       <c r="I63" s="25" t="n">
@@ -11083,7 +11085,7 @@
       </c>
       <c r="H64" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB&amp;02-11-12-AB</t>
+          <t xml:space="preserve">0111AB/0112AB_0211AB/0212AB  </t>
         </is>
       </c>
       <c r="I64" s="25" t="n">
@@ -11124,7 +11126,7 @@
       </c>
       <c r="H65" s="25" t="inlineStr">
         <is>
-          <t>01-11-12-AB&amp;02-11-12-AB</t>
+          <t xml:space="preserve">0111AB/0112AB_0211AB/0212AB  </t>
         </is>
       </c>
       <c r="I65" s="25" t="n">
@@ -11171,7 +11173,7 @@
       </c>
       <c r="H69" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t xml:space="preserve">0014A0/0015A0/0016A0   </t>
         </is>
       </c>
       <c r="I69" s="25" t="inlineStr">
@@ -11189,7 +11191,7 @@
       </c>
     </row>
     <row r="70" ht="18" customHeight="1">
-      <c r="B70" s="21" t="n">
+      <c r="B70" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C70" s="25" t="inlineStr">
@@ -11212,7 +11214,7 @@
       </c>
       <c r="H70" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">00140B/00150B/00160B  </t>
         </is>
       </c>
       <c r="I70" s="25" t="n">
@@ -11228,7 +11230,7 @@
       </c>
     </row>
     <row r="71" ht="18" customHeight="1">
-      <c r="B71" s="21" t="n">
+      <c r="B71" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C71" s="25" t="inlineStr">
@@ -11251,7 +11253,7 @@
       </c>
       <c r="H71" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">00140B/00150B/00160B  </t>
         </is>
       </c>
       <c r="I71" s="25" t="n">
@@ -11292,7 +11294,7 @@
       </c>
       <c r="H72" s="25" t="inlineStr">
         <is>
-          <t>00-17-18-AB&amp;01-17-18-AB</t>
+          <t xml:space="preserve">0017AB/0018AB_0117AB/0118AB   </t>
         </is>
       </c>
       <c r="I72" s="25" t="n">
@@ -11333,7 +11335,7 @@
       </c>
       <c r="H73" s="25" t="inlineStr">
         <is>
-          <t>00-17-18-AB&amp;01-17-18-AB</t>
+          <t xml:space="preserve">0017AB/0018AB_0117AB/0118AB   </t>
         </is>
       </c>
       <c r="I73" s="25" t="n">
@@ -11349,7 +11351,7 @@
       </c>
     </row>
     <row r="74" ht="18" customHeight="1">
-      <c r="B74" s="21" t="n">
+      <c r="B74" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C74" s="25" t="inlineStr">
@@ -11372,7 +11374,7 @@
       </c>
       <c r="H74" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t xml:space="preserve">0014A0/0015A0/0016A0   </t>
         </is>
       </c>
       <c r="I74" s="25" t="n">
@@ -11408,7 +11410,7 @@
       </c>
       <c r="H75" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">00140B/00150B/00160B   </t>
         </is>
       </c>
       <c r="I75" s="25" t="n">
@@ -11424,7 +11426,7 @@
       </c>
     </row>
     <row r="76" ht="18" customHeight="1">
-      <c r="B76" s="21" t="n">
+      <c r="B76" s="19" t="n">
         <v>2</v>
       </c>
       <c r="C76" s="25" t="inlineStr">
@@ -11447,7 +11449,7 @@
       </c>
       <c r="H76" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-A</t>
+          <t xml:space="preserve">0014A0/0015A0/0016A0   </t>
         </is>
       </c>
       <c r="I76" s="25" t="n">
@@ -11483,7 +11485,7 @@
       </c>
       <c r="H77" s="25" t="inlineStr">
         <is>
-          <t>00-14-15-16-B</t>
+          <t xml:space="preserve">00140B/00150B/00160B   </t>
         </is>
       </c>
       <c r="I77" s="25" t="n">
@@ -11499,7 +11501,7 @@
       </c>
     </row>
     <row r="78" ht="18" customHeight="1">
-      <c r="B78" s="21" t="n">
+      <c r="B78" s="19" t="n">
         <v>18</v>
       </c>
       <c r="C78" s="25" t="inlineStr">
@@ -11522,7 +11524,7 @@
       </c>
       <c r="H78" s="25" t="inlineStr">
         <is>
-          <t>02-14-15-16-17-18-B</t>
+          <t xml:space="preserve">02140B/02150B/02160B/02170B/02180B </t>
         </is>
       </c>
       <c r="I78" s="25" t="n">
@@ -11538,7 +11540,7 @@
       </c>
     </row>
     <row r="79" ht="18" customHeight="1">
-      <c r="B79" s="21" t="n">
+      <c r="B79" s="19" t="n">
         <v>19</v>
       </c>
       <c r="C79" s="25" t="inlineStr">
@@ -11561,7 +11563,7 @@
       </c>
       <c r="H79" s="25" t="inlineStr">
         <is>
-          <t>02-14-15-16-17-18-B</t>
+          <t xml:space="preserve">02140B/02150B/02160B/02170B/02180B </t>
         </is>
       </c>
       <c r="I79" s="25" t="n">
@@ -11577,7 +11579,7 @@
       </c>
     </row>
     <row r="80" ht="18" customHeight="1">
-      <c r="B80" s="21" t="n">
+      <c r="B80" s="19" t="n">
         <v>20</v>
       </c>
       <c r="C80" s="25" t="inlineStr">
@@ -11600,7 +11602,7 @@
       </c>
       <c r="H80" s="25" t="inlineStr">
         <is>
-          <t>02-14-15-16-17-18-B</t>
+          <t xml:space="preserve">02140B/02150B/02160B/02170B/02180B </t>
         </is>
       </c>
       <c r="I80" s="25" t="n">
@@ -11653,24 +11655,24 @@
     <row r="102" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="B60:B61"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B48:B49"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B52:B53"/>
     <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B67:H67"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B74:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>